<commit_message>
fin grupo B 2
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D486DA-2DF9-4244-AC38-EC9780E83EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1D53B9-8669-46B1-9708-03F02F52D80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,8 +9778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9905,7 +9905,7 @@
       </c>
       <c r="E5" s="197">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:E4),0))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:F4),0))</f>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>55.011000000000003</v>
+        <v>60.011000000000003</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="S5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="T5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>35.005000000000003</v>
+        <v>40.005000000000003</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10007,7 +10007,7 @@
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>50.012</v>
+        <v>55.012</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10059,7 +10059,7 @@
       </c>
       <c r="S6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="T6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>35.006</v>
+        <v>40.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10109,7 +10109,7 @@
       </c>
       <c r="E7" s="197">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:E6),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
@@ -10125,7 +10125,7 @@
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>40.012999999999998</v>
+        <v>45.012999999999998</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="S7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>40.006999999999998</v>
+        <v>45.006999999999998</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10211,7 +10211,7 @@
       </c>
       <c r="E8" s="201">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:E7),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>40.009</v>
+        <v>45.009</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10263,7 +10263,7 @@
       </c>
       <c r="S8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="T8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>30.007999999999999</v>
+        <v>35.008000000000003</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10313,7 +10313,7 @@
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>40.006999999999998</v>
+        <v>45.006999999999998</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="S9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10381,7 +10381,7 @@
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>40.009</v>
+        <v>45.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10415,7 +10415,7 @@
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>35.006</v>
+        <v>40.006</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="S10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>30.01</v>
+        <v>35.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10517,7 +10517,7 @@
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>35.005000000000003</v>
+        <v>40.005000000000003</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10569,7 +10569,7 @@
       </c>
       <c r="S11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>55.011000000000003</v>
+        <v>60.011000000000003</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10619,7 +10619,7 @@
       </c>
       <c r="E12" s="197">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:E11),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
@@ -10635,7 +10635,7 @@
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>30.01</v>
+        <v>35.01</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10671,7 +10671,7 @@
       </c>
       <c r="S12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="T12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>50.012</v>
+        <v>55.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10721,7 +10721,7 @@
       </c>
       <c r="E13" s="201">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:E12),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:F12),0))</f>
@@ -10737,7 +10737,7 @@
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>30.007999999999999</v>
+        <v>35.008000000000003</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10773,7 +10773,7 @@
       </c>
       <c r="S13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>40.012999999999998</v>
+        <v>45.012999999999998</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12637,17 +12637,17 @@
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="221" t="str">
+      <c r="G8" s="221">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="H8" s="222" t="str">
+        <v>0</v>
+      </c>
+      <c r="H8" s="222">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="I8" s="223" t="str">
+        <v>2</v>
+      </c>
+      <c r="I8" s="223">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
@@ -19060,17 +19060,17 @@
         <f t="shared" ref="AE3" ca="1" si="7">IF(OR(AC3="",AD3=""),"",IF(AC3&gt;AD3,1,IF(AC3=AD3,"x",2)))</f>
         <v>2</v>
       </c>
-      <c r="AF3" s="191" t="str">
+      <c r="AF3" s="191">
         <f ca="1">VLOOKUP(AF2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AG3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="191">
         <f ca="1">VLOOKUP(AF2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AH3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="191">
         <f t="shared" ref="AH3" ca="1" si="8">IF(OR(AF3="",AG3=""),"",IF(AF3&gt;AG3,1,IF(AF3=AG3,"x",2)))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AI3" s="191" t="str">
         <f ca="1">VLOOKUP(AI2,Aux!$F:$O,9,0)</f>
@@ -20362,7 +20362,7 @@
       </c>
       <c r="AH7">
         <f ca="1">IF($B7=0,0,IF(AND(AF$3=TotalApuestas!AF2,Resultado!AG$3=TotalApuestas!AG2),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH2,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI7">
         <f ca="1">IF($B7=0,0,IF(AI$3=TotalApuestas!AI2,AI$5,0))</f>
@@ -20828,7 +20828,7 @@
       </c>
       <c r="AH8">
         <f ca="1">IF($B8=0,0,IF(AND(AF$3=TotalApuestas!AF3,Resultado!AG$3=TotalApuestas!AG3),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH3,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI8">
         <f ca="1">IF($B8=0,0,IF(AI$3=TotalApuestas!AI3,AI$5,0))</f>
@@ -21294,7 +21294,7 @@
       </c>
       <c r="AH9">
         <f ca="1">IF($B9=0,0,IF(AND(AF$3=TotalApuestas!AF4,Resultado!AG$3=TotalApuestas!AG4),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH4,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI9">
         <f ca="1">IF($B9=0,0,IF(AI$3=TotalApuestas!AI4,AI$5,0))</f>
@@ -21760,7 +21760,7 @@
       </c>
       <c r="AH10">
         <f ca="1">IF($B10=0,0,IF(AND(AF$3=TotalApuestas!AF5,Resultado!AG$3=TotalApuestas!AG5),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH5,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI10">
         <f ca="1">IF($B10=0,0,IF(AI$3=TotalApuestas!AI5,AI$5,0))</f>
@@ -22226,7 +22226,7 @@
       </c>
       <c r="AH11">
         <f ca="1">IF($B11=0,0,IF(AND(AF$3=TotalApuestas!AF6,Resultado!AG$3=TotalApuestas!AG6),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH6,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI11">
         <f ca="1">IF($B11=0,0,IF(AI$3=TotalApuestas!AI6,AI$5,0))</f>
@@ -22692,7 +22692,7 @@
       </c>
       <c r="AH12">
         <f ca="1">IF($B12=0,0,IF(AND(AF$3=TotalApuestas!AF7,Resultado!AG$3=TotalApuestas!AG7),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH7,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI12">
         <f ca="1">IF($B12=0,0,IF(AI$3=TotalApuestas!AI7,AI$5,0))</f>
@@ -23158,7 +23158,7 @@
       </c>
       <c r="AH13">
         <f ca="1">IF($B13=0,0,IF(AND(AF$3=TotalApuestas!AF8,Resultado!AG$3=TotalApuestas!AG8),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH8,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI13">
         <f ca="1">IF($B13=0,0,IF(AI$3=TotalApuestas!AI8,AI$5,0))</f>
@@ -23624,7 +23624,7 @@
       </c>
       <c r="AH14">
         <f ca="1">IF($B14=0,0,IF(AND(AF$3=TotalApuestas!AF9,Resultado!AG$3=TotalApuestas!AG9),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH9,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI14">
         <f ca="1">IF($B14=0,0,IF(AI$3=TotalApuestas!AI9,AI$5,0))</f>
@@ -24090,7 +24090,7 @@
       </c>
       <c r="AH15">
         <f ca="1">IF($B15=0,0,IF(AND(AF$3=TotalApuestas!AF10,Resultado!AG$3=TotalApuestas!AG10),Resultado!AH$5+VLOOKUP(AH$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AH$3=TotalApuestas!AH10,AH$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI15">
         <f ca="1">IF($B15=0,0,IF(AI$3=TotalApuestas!AI10,AI$5,0))</f>
@@ -41349,17 +41349,17 @@
         <f ca="1">+Resultado!AE3</f>
         <v>2</v>
       </c>
-      <c r="AF1" s="84" t="str">
+      <c r="AF1" s="84">
         <f ca="1">+Resultado!AF3</f>
-        <v/>
-      </c>
-      <c r="AG1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="AG1" s="84">
         <f ca="1">+Resultado!AG3</f>
-        <v/>
-      </c>
-      <c r="AH1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="84">
         <f ca="1">+Resultado!AH3</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AI1" s="84" t="str">
         <f ca="1">+Resultado!AI3</f>
@@ -41713,7 +41713,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -41984,7 +41984,7 @@
       <c r="AQ5" s="53"/>
       <c r="AR5" s="245">
         <f>+VLOOKUP(AR7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
@@ -42255,11 +42255,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -42271,7 +42271,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -42279,7 +42279,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -42293,15 +42293,15 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AG9" s="53" cm="1">
         <f t="array" ref="AG9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH9" s="53" cm="1">
         <f t="array" ref="AH9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -42313,7 +42313,7 @@
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
@@ -42321,15 +42321,15 @@
       </c>
       <c r="AL9" s="252">
         <f>+SUMIFS($AR9:$AU9,$AR$5:$AU$5,AF9)</f>
-        <v>302</v>
+        <v>0</v>
       </c>
       <c r="AM9" s="252">
         <f>+AJ9-AK9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN9" s="53">
         <f>+_xlfn.RANK.EQ(AF9,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM9,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ9,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL9,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.1110089999999999</v>
+        <v>1.1130089999999999</v>
       </c>
       <c r="AO9" s="53">
         <f>+_xlfn.RANK.EQ(AN9,$AN$9:$AN$15,1)</f>
@@ -42356,7 +42356,7 @@
 (SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="AU9" s="53" cm="1">
         <f t="array" ref="AU9">(SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -42545,11 +42545,11 @@
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.3320109999999996</v>
+        <v>3.2310110000000001</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11:AO15" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AP11" s="53"/>
       <c r="AQ11" s="53"/>
@@ -42678,9 +42678,9 @@
       <c r="O13"/>
       <c r="P13" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(3,$AO$9:$AO$15,0))</f>
-        <v>Chile</v>
-      </c>
-      <c r="Q13" s="157" t="e" vm="4">
+        <v>Perú</v>
+      </c>
+      <c r="Q13" s="157" t="e" vm="3">
         <f>IFERROR(VLOOKUP(P13,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
@@ -42699,7 +42699,7 @@
       </c>
       <c r="V13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,6,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,7,0)</f>
@@ -42707,11 +42707,11 @@
       </c>
       <c r="X13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,8,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="161">
         <f>+W13-X13</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z13" s="60"/>
       <c r="AA13" s="57"/>
@@ -42725,7 +42725,7 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" si="1"/>
@@ -42741,7 +42741,7 @@
       </c>
       <c r="AI13" s="53" cm="1">
         <f t="array" ref="AI13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
@@ -42749,7 +42749,7 @@
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
@@ -42757,15 +42757,15 @@
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.2320129999999998</v>
+        <v>3.2310129999999999</v>
       </c>
       <c r="AO13" s="53">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AP13" s="53"/>
       <c r="AQ13" s="53"/>
@@ -42774,7 +42774,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AR$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AR$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AR$7))</f>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="AS13" s="53" cm="1">
         <f t="array" ref="AS13">(SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AS$7)))*300+
@@ -42869,11 +42869,15 @@
         <f>+VLOOKUP(B15,Aux!F:S,5,0)</f>
         <v>Chile</v>
       </c>
-      <c r="H15" s="258"/>
+      <c r="H15" s="258">
+        <v>0</v>
+      </c>
       <c r="I15" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="258"/>
+      <c r="J15" s="258">
+        <v>1</v>
+      </c>
       <c r="K15" s="38" t="str">
         <f>+VLOOKUP(B15,Aux!F:S,6,0)</f>
         <v>Argentina</v>
@@ -42890,9 +42894,9 @@
       <c r="O15"/>
       <c r="P15" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(4,$AO$9:$AO$15,0))</f>
-        <v>Perú</v>
-      </c>
-      <c r="Q15" s="157" t="e" vm="3">
+        <v>Chile</v>
+      </c>
+      <c r="Q15" s="157" t="e" vm="4">
         <f>IFERROR(VLOOKUP(P15,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
@@ -42965,7 +42969,7 @@
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
@@ -42973,7 +42977,7 @@
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.3240150000000002</v>
+        <v>2.2230150000000002</v>
       </c>
       <c r="AO15" s="53">
         <f t="shared" si="2"/>
@@ -50279,13 +50283,13 @@
       <c r="M11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="68" t="str">
+      <c r="N11" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O11" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O11" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
termino jornada 2 B
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1D53B9-8669-46B1-9708-03F02F52D80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A6CA7-DF0C-469E-AE1E-CAF0CC9C5482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,8 +9778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9901,19 +9901,19 @@
       </c>
       <c r="D5" s="151" t="str">
         <f ca="1">+VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:D4),0)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="E5" s="197">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:E4),0))</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:F4),0))</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:G4),0))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:H4),0))</f>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>60.011000000000003</v>
+        <v>70.012</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="T5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>40.005000000000003</v>
+        <v>50.005000000000003</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10003,19 +10003,19 @@
       </c>
       <c r="D6" s="151" t="str">
         <f ca="1">+VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:D5),0)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>55.012</v>
+        <v>70.010999999999996</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="Q6" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R6" s="126" t="str">
         <f>Resultado!B8</f>
@@ -10063,7 +10063,7 @@
       </c>
       <c r="T6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>40.006</v>
+        <v>45.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10113,7 +10113,7 @@
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
@@ -10125,7 +10125,7 @@
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>45.012999999999998</v>
+        <v>60.012999999999998</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="T7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>45.006999999999998</v>
+        <v>55.006999999999998</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>45.009</v>
+        <v>60.009</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="T8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>35.008000000000003</v>
+        <v>50.008000000000003</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10317,7 +10317,7 @@
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>45.006999999999998</v>
+        <v>55.006999999999998</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10369,7 +10369,7 @@
       </c>
       <c r="T9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="U9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10381,7 +10381,7 @@
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>45.009</v>
+        <v>60.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10411,7 +10411,7 @@
       </c>
       <c r="D10" s="151" t="str">
         <f ca="1">+VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:D9),0)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
@@ -10419,11 +10419,11 @@
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>40.006</v>
+        <v>50.008000000000003</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10471,7 +10471,7 @@
       </c>
       <c r="T10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>35.01</v>
+        <v>40.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10521,7 +10521,7 @@
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>40.005000000000003</v>
+        <v>50.005000000000003</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10561,7 +10561,7 @@
       </c>
       <c r="Q11" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="126" t="str">
         <f>Resultado!B13</f>
@@ -10573,7 +10573,7 @@
       </c>
       <c r="T11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>60.011000000000003</v>
+        <v>70.010999999999996</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10615,15 +10615,15 @@
       </c>
       <c r="D12" s="151" t="str">
         <f ca="1">+VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:D11),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="E12" s="197">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:E11),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
@@ -10631,11 +10631,11 @@
       </c>
       <c r="H12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:H11),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>35.01</v>
+        <v>45.006</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10663,7 +10663,7 @@
       </c>
       <c r="Q12" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R12" s="126" t="str">
         <f>Resultado!B14</f>
@@ -10675,7 +10675,7 @@
       </c>
       <c r="T12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="U12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>55.012</v>
+        <v>70.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10717,11 +10717,11 @@
       </c>
       <c r="D13" s="152" t="str">
         <f ca="1">+VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:D12),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E13" s="201">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:E12),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:F12),0))</f>
@@ -10729,15 +10729,15 @@
       </c>
       <c r="G13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:G12),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:H12),0))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>35.008000000000003</v>
+        <v>40.01</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10777,7 +10777,7 @@
       </c>
       <c r="T13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>45.012999999999998</v>
+        <v>60.012999999999998</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,7 +12232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -12513,7 +12513,7 @@
       <c r="R6" s="214"/>
       <c r="S6" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D5=0,"",ClasificaciónPorra!D5)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="T6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">IF(OR(T$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12529,11 +12529,11 @@
       </c>
       <c r="W6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">IF(OR(W$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Canadá</v>
       </c>
       <c r="X6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">IF(OR(X$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="Y6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y6" ca="1">IF(OR(Y$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
@@ -12545,7 +12545,7 @@
       </c>
       <c r="AA6" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA6" ca="1">IF(OR(AA$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Colombia</v>
       </c>
       <c r="AB6" s="123"/>
       <c r="AD6"/>
@@ -12582,7 +12582,7 @@
       <c r="R7" s="214"/>
       <c r="S7" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="T7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">IF(OR(T$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12598,11 +12598,11 @@
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Chile</v>
       </c>
       <c r="X7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">IF(OR(X$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Colombia</v>
       </c>
       <c r="Y7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y7" ca="1">IF(OR(Y$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
@@ -12614,7 +12614,7 @@
       </c>
       <c r="AA7" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA7" ca="1">IF(OR(AA$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="AB7" s="123"/>
       <c r="AD7"/>
@@ -12649,29 +12649,29 @@
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
         <v>1</v>
       </c>
-      <c r="J8" s="221" t="str">
+      <c r="J8" s="221">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="K8" s="222" t="str">
+        <v>3</v>
+      </c>
+      <c r="K8" s="222">
         <f ca="1">+IF(J8="","",IF(J8&gt;L8,1,IF(J8=L8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="L8" s="223" t="str">
+        <v>1</v>
+      </c>
+      <c r="L8" s="223">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="M8" s="221" t="str">
+        <v>1</v>
+      </c>
+      <c r="M8" s="221">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="N8" s="222" t="str">
+        <v>1</v>
+      </c>
+      <c r="N8" s="222">
         <f ca="1">+IF(M8="","",IF(M8&gt;O8,1,IF(M8=O8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="O8" s="223" t="str">
+        <v>1</v>
+      </c>
+      <c r="O8" s="223">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P8" s="123"/>
       <c r="R8" s="214"/>
@@ -12763,11 +12763,11 @@
       <c r="B10" s="214"/>
       <c r="C10" s="224" t="str">
         <f ca="1">IF(ClasificaciónPorra!D5=0,"",ClasificaciónPorra!D5)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="D10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="226">
         <f t="shared" ref="E10" ca="1" si="2">+IF(D10="","",IF(D10&gt;F10,1,IF(D10=F10,"X",2)))</f>
@@ -12775,11 +12775,11 @@
       </c>
       <c r="F10" s="225" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="226">
         <f t="shared" ref="H10" ca="1" si="3">+IF(G10="","",IF(G10&gt;I10,1,IF(G10=I10,"X",2)))</f>
@@ -12787,11 +12787,11 @@
       </c>
       <c r="I10" s="228" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" s="226">
         <f t="shared" ref="K10" ca="1" si="4">+IF(J10="","",IF(J10&gt;L10,1,IF(J10=L10,"X",2)))</f>
@@ -12799,15 +12799,15 @@
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="226" t="str">
+        <v>1</v>
+      </c>
+      <c r="N10" s="226">
         <f t="shared" ref="N10" ca="1" si="5">+IF(M10="","",IF(M10&gt;O10,1,IF(M10=O10,"X",2)))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -12859,11 +12859,11 @@
       <c r="B11" s="214"/>
       <c r="C11" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="231">
         <f t="shared" ref="E11:E29" ca="1" si="6">+IF(D11="","",IF(D11&gt;F11,1,IF(D11=F11,"X",2)))</f>
@@ -12871,11 +12871,11 @@
       </c>
       <c r="F11" s="230" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="231">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
@@ -12883,11 +12883,11 @@
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
@@ -12895,15 +12895,15 @@
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="N11" s="231">
+        <v>0</v>
+      </c>
+      <c r="N11" s="231" t="str">
         <f t="shared" ref="N11:N29" ca="1" si="9">+IF(M11="","",IF(M11&gt;O11,1,IF(M11=O11,"X",2)))</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="O11" s="233" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -12913,7 +12913,7 @@
       <c r="R11" s="214"/>
       <c r="S11" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">IF(OR(T$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12921,15 +12921,15 @@
       </c>
       <c r="U11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(OR(U$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(OR(V$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="W11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">IF(OR(W$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Canadá</v>
       </c>
       <c r="X11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">IF(OR(X$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -13105,7 +13105,7 @@
       <c r="R13" s="214"/>
       <c r="S13" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="T13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">IF(OR(T$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13121,7 +13121,7 @@
       </c>
       <c r="W13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">IF(OR(W$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Chile</v>
       </c>
       <c r="X13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">IF(OR(X$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -13201,7 +13201,7 @@
       <c r="R14" s="214"/>
       <c r="S14" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D13=0,"",ClasificaciónPorra!D13)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">IF(OR(T$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13209,11 +13209,11 @@
       </c>
       <c r="U14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">IF(OR(U$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">IF(OR(V$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="W14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">IF(OR(W$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
@@ -13243,15 +13243,15 @@
       <c r="B15" s="214"/>
       <c r="C15" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="231">
+        <v>0</v>
+      </c>
+      <c r="E15" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
@@ -13267,7 +13267,7 @@
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13285,13 +13285,13 @@
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="N15" s="231" t="str">
+      <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="123"/>
       <c r="R15" s="214"/>
@@ -13435,7 +13435,7 @@
       <c r="B17" s="214"/>
       <c r="C17" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
@@ -13443,11 +13443,11 @@
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13531,19 +13531,19 @@
       <c r="B18" s="214"/>
       <c r="C18" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D13=0,"",ClasificaciónPorra!D13)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="231" t="str">
+        <v>1</v>
+      </c>
+      <c r="E18" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="F18" s="230" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13555,7 +13555,7 @@
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13573,13 +13573,13 @@
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="N18" s="231">
+      <c r="N18" s="231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="O18" s="233" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="123"/>
       <c r="R18" s="214"/>
@@ -19072,29 +19072,29 @@
         <f t="shared" ref="AH3" ca="1" si="8">IF(OR(AF3="",AG3=""),"",IF(AF3&gt;AG3,1,IF(AF3=AG3,"x",2)))</f>
         <v>2</v>
       </c>
-      <c r="AI3" s="191" t="str">
+      <c r="AI3" s="191">
         <f ca="1">VLOOKUP(AI2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AJ3" s="191" t="str">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="191">
         <f ca="1">VLOOKUP(AI2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AK3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="191">
         <f t="shared" ref="AK3" ca="1" si="9">IF(OR(AI3="",AJ3=""),"",IF(AI3&gt;AJ3,1,IF(AI3=AJ3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="AL3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="191">
         <f ca="1">VLOOKUP(AL2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AM3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="191">
         <f ca="1">VLOOKUP(AL2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AN3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="191">
         <f t="shared" ref="AN3" ca="1" si="10">IF(OR(AL3="",AM3=""),"",IF(AL3&gt;AM3,1,IF(AL3=AM3,"x",2)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AO3" s="191" t="str">
         <f ca="1">VLOOKUP(AO2,Aux!$F:$O,9,0)</f>
@@ -20374,7 +20374,7 @@
       </c>
       <c r="AK7">
         <f ca="1">IF($B7=0,0,IF(AND(AI$3=TotalApuestas!AI2,Resultado!AJ$3=TotalApuestas!AJ2),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK2,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL7">
         <f ca="1">IF($B7=0,0,IF(AL$3=TotalApuestas!AL2,AL$5,0))</f>
@@ -20386,7 +20386,7 @@
       </c>
       <c r="AN7">
         <f ca="1">IF($B7=0,0,IF(AND(AL$3=TotalApuestas!AL2,Resultado!AM$3=TotalApuestas!AM2),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN2,AN$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO7">
         <f ca="1">IF($B7=0,0,IF(AO$3=TotalApuestas!AO2,AO$5,0))</f>
@@ -20840,7 +20840,7 @@
       </c>
       <c r="AK8">
         <f ca="1">IF($B8=0,0,IF(AND(AI$3=TotalApuestas!AI3,Resultado!AJ$3=TotalApuestas!AJ3),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK3,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL8">
         <f ca="1">IF($B8=0,0,IF(AL$3=TotalApuestas!AL3,AL$5,0))</f>
@@ -21306,7 +21306,7 @@
       </c>
       <c r="AK9">
         <f ca="1">IF($B9=0,0,IF(AND(AI$3=TotalApuestas!AI4,Resultado!AJ$3=TotalApuestas!AJ4),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK4,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL9">
         <f ca="1">IF($B9=0,0,IF(AL$3=TotalApuestas!AL4,AL$5,0))</f>
@@ -21318,7 +21318,7 @@
       </c>
       <c r="AN9">
         <f ca="1">IF($B9=0,0,IF(AND(AL$3=TotalApuestas!AL4,Resultado!AM$3=TotalApuestas!AM4),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN4,AN$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO9">
         <f ca="1">IF($B9=0,0,IF(AO$3=TotalApuestas!AO4,AO$5,0))</f>
@@ -21772,7 +21772,7 @@
       </c>
       <c r="AK10">
         <f ca="1">IF($B10=0,0,IF(AND(AI$3=TotalApuestas!AI5,Resultado!AJ$3=TotalApuestas!AJ5),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK5,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL10">
         <f ca="1">IF($B10=0,0,IF(AL$3=TotalApuestas!AL5,AL$5,0))</f>
@@ -21784,7 +21784,7 @@
       </c>
       <c r="AN10">
         <f ca="1">IF($B10=0,0,IF(AND(AL$3=TotalApuestas!AL5,Resultado!AM$3=TotalApuestas!AM5),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN5,AN$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO10">
         <f ca="1">IF($B10=0,0,IF(AO$3=TotalApuestas!AO5,AO$5,0))</f>
@@ -22238,7 +22238,7 @@
       </c>
       <c r="AK11">
         <f ca="1">IF($B11=0,0,IF(AND(AI$3=TotalApuestas!AI6,Resultado!AJ$3=TotalApuestas!AJ6),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK6,AK$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL11">
         <f ca="1">IF($B11=0,0,IF(AL$3=TotalApuestas!AL6,AL$5,0))</f>
@@ -22250,7 +22250,7 @@
       </c>
       <c r="AN11">
         <f ca="1">IF($B11=0,0,IF(AND(AL$3=TotalApuestas!AL6,Resultado!AM$3=TotalApuestas!AM6),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN6,AN$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO11">
         <f ca="1">IF($B11=0,0,IF(AO$3=TotalApuestas!AO6,AO$5,0))</f>
@@ -22704,7 +22704,7 @@
       </c>
       <c r="AK12">
         <f ca="1">IF($B12=0,0,IF(AND(AI$3=TotalApuestas!AI7,Resultado!AJ$3=TotalApuestas!AJ7),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK7,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL12">
         <f ca="1">IF($B12=0,0,IF(AL$3=TotalApuestas!AL7,AL$5,0))</f>
@@ -23170,7 +23170,7 @@
       </c>
       <c r="AK13">
         <f ca="1">IF($B13=0,0,IF(AND(AI$3=TotalApuestas!AI8,Resultado!AJ$3=TotalApuestas!AJ8),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK8,AK$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL13">
         <f ca="1">IF($B13=0,0,IF(AL$3=TotalApuestas!AL8,AL$5,0))</f>
@@ -23636,7 +23636,7 @@
       </c>
       <c r="AK14">
         <f ca="1">IF($B14=0,0,IF(AND(AI$3=TotalApuestas!AI9,Resultado!AJ$3=TotalApuestas!AJ9),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK9,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL14">
         <f ca="1">IF($B14=0,0,IF(AL$3=TotalApuestas!AL9,AL$5,0))</f>
@@ -23648,7 +23648,7 @@
       </c>
       <c r="AN14">
         <f ca="1">IF($B14=0,0,IF(AND(AL$3=TotalApuestas!AL9,Resultado!AM$3=TotalApuestas!AM9),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN9,AN$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO14">
         <f ca="1">IF($B14=0,0,IF(AO$3=TotalApuestas!AO9,AO$5,0))</f>
@@ -24102,7 +24102,7 @@
       </c>
       <c r="AK15">
         <f ca="1">IF($B15=0,0,IF(AND(AI$3=TotalApuestas!AI10,Resultado!AJ$3=TotalApuestas!AJ10),Resultado!AK$5+VLOOKUP(AK$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AK$3=TotalApuestas!AK10,AK$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL15">
         <f ca="1">IF($B15=0,0,IF(AL$3=TotalApuestas!AL10,AL$5,0))</f>
@@ -24114,7 +24114,7 @@
       </c>
       <c r="AN15">
         <f ca="1">IF($B15=0,0,IF(AND(AL$3=TotalApuestas!AL10,Resultado!AM$3=TotalApuestas!AM10),Resultado!AN$5+VLOOKUP(AN$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AN$3=TotalApuestas!AN10,AN$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO15">
         <f ca="1">IF($B15=0,0,IF(AO$3=TotalApuestas!AO10,AO$5,0))</f>
@@ -41361,29 +41361,29 @@
         <f ca="1">+Resultado!AH3</f>
         <v>2</v>
       </c>
-      <c r="AI1" s="84" t="str">
+      <c r="AI1" s="84">
         <f ca="1">+Resultado!AI3</f>
-        <v/>
-      </c>
-      <c r="AJ1" s="84" t="str">
+        <v>3</v>
+      </c>
+      <c r="AJ1" s="84">
         <f ca="1">+Resultado!AJ3</f>
-        <v/>
-      </c>
-      <c r="AK1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="84">
         <f ca="1">+Resultado!AK3</f>
-        <v/>
-      </c>
-      <c r="AL1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AL1" s="84">
         <f ca="1">+Resultado!AL3</f>
-        <v/>
-      </c>
-      <c r="AM1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="84">
         <f ca="1">+Resultado!AM3</f>
-        <v/>
-      </c>
-      <c r="AN1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN1" s="84">
         <f ca="1">+Resultado!AN3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AO1" s="84" t="str">
         <f ca="1">+Resultado!AO3</f>
@@ -43321,7 +43321,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43596,11 +43596,11 @@
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AU5" s="245">
         <f>+VLOOKUP(AU7,$AD$9:$AF$15,3,0)</f>
@@ -43863,11 +43863,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -43879,7 +43879,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -43887,7 +43887,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -43901,7 +43901,7 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
@@ -43917,7 +43917,7 @@
       </c>
       <c r="AI9" s="53" cm="1">
         <f t="array" ref="AI9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
@@ -43925,7 +43925,7 @@
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL9" s="252">
         <f>+SUMIFS($AR9:$AU9,$AR$5:$AU$5,AF9)</f>
@@ -43933,15 +43933,15 @@
       </c>
       <c r="AM9" s="252">
         <f>+AJ9-AK9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="53">
         <f>+_xlfn.RANK.EQ(AF9,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM9,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ9,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL9,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.1210089999999999</v>
+        <v>2.3310089999999994</v>
       </c>
       <c r="AO9" s="53">
         <f>+_xlfn.RANK.EQ(AN9,$AN$9:$AN$15,1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP9" s="53"/>
       <c r="AQ9" s="53"/>
@@ -43964,7 +43964,7 @@
 (SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="AU9" s="53" cm="1">
         <f t="array" ref="AU9">(SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -44070,9 +44070,9 @@
       <c r="O11"/>
       <c r="P11" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(2,$AO$9:$AO$15,0))</f>
-        <v>México</v>
-      </c>
-      <c r="Q11" s="157" t="e" vm="7">
+        <v>Ecuador</v>
+      </c>
+      <c r="Q11" s="157" t="e" vm="5">
         <f>IFERROR(VLOOKUP(P11,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
@@ -44091,15 +44091,15 @@
       </c>
       <c r="V11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,6,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,7,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,8,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="161">
         <f>+W11-X11</f>
@@ -44117,15 +44117,15 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11" si="0">+AG11+AH11+AI11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11" si="1">+AG11*3+AH11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG11" s="53" cm="1">
         <f t="array" ref="AG11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11" s="53" cm="1">
         <f t="array" ref="AH11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -44137,11 +44137,11 @@
       </c>
       <c r="AJ11" s="53" cm="1">
         <f t="array" ref="AJ11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)+($K$9:$K$22=$AD11)*($J$9:$J$22))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AK11" s="53" cm="1">
         <f t="array" ref="AK11">SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL11" s="252">
         <f>+SUMIFS($AR11:$AU11,$AR$5:$AU$5,AF11)</f>
@@ -44149,15 +44149,15 @@
       </c>
       <c r="AM11" s="252">
         <f>+AJ11-AK11</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.3210109999999999</v>
+        <v>2.2110110000000001</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AP11" s="53"/>
       <c r="AQ11" s="53"/>
@@ -44187,7 +44187,7 @@
 (SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AU$7)))*100
 +SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($J$9:$J$22)*($G$9:$G$22=AU$7))
 -SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22)*($G$9:$G$22=AU$7))</f>
-        <v>100</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="2:47" s="54" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -44261,11 +44261,15 @@
         <f>+VLOOKUP(B13,Aux!F:S,5,0)</f>
         <v>Ecuador</v>
       </c>
-      <c r="H13" s="258"/>
+      <c r="H13" s="258">
+        <v>3</v>
+      </c>
       <c r="I13" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="258"/>
+      <c r="J13" s="258">
+        <v>1</v>
+      </c>
       <c r="K13" s="38" t="str">
         <f>+VLOOKUP(B13,Aux!F:S,6,0)</f>
         <v>Jamaica</v>
@@ -44282,20 +44286,20 @@
       <c r="O13"/>
       <c r="P13" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(3,$AO$9:$AO$15,0))</f>
-        <v>Ecuador</v>
-      </c>
-      <c r="Q13" s="157" t="e" vm="5">
+        <v>México</v>
+      </c>
+      <c r="Q13" s="157" t="e" vm="7">
         <f>IFERROR(VLOOKUP(P13,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
       <c r="R13" s="158"/>
       <c r="S13" s="159">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,5,0)</f>
@@ -44311,11 +44315,11 @@
       </c>
       <c r="X13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,8,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="161">
         <f>+W13-X13</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="60"/>
       <c r="AA13" s="57"/>
@@ -44329,15 +44333,15 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" ref="AE13" si="3">+AG13+AH13+AI13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" ref="AF13" si="4">+AG13*3+AH13</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AG13" s="53" cm="1">
         <f t="array" ref="AG13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH13" s="53" cm="1">
         <f t="array" ref="AH13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -44349,7 +44353,7 @@
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
@@ -44357,15 +44361,15 @@
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.111013</v>
+        <v>1.123013</v>
       </c>
       <c r="AO13" s="53">
         <f t="shared" ref="AO13" si="5">+_xlfn.RANK.EQ(AN13,$AN$9:$AN$15,1)</f>
@@ -44378,7 +44382,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AR$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AR$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AR$7))</f>
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="AS13" s="53" cm="1">
         <f t="array" ref="AS13">(SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AS$7)))*300+
@@ -44473,11 +44477,15 @@
         <f>+VLOOKUP(B15,Aux!F:S,5,0)</f>
         <v>Venezuela</v>
       </c>
-      <c r="H15" s="258"/>
+      <c r="H15" s="258">
+        <v>1</v>
+      </c>
       <c r="I15" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="258"/>
+      <c r="J15" s="258">
+        <v>0</v>
+      </c>
       <c r="K15" s="38" t="str">
         <f>+VLOOKUP(B15,Aux!F:S,6,0)</f>
         <v>México</v>
@@ -44515,19 +44523,19 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -44541,7 +44549,7 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" ref="AE15" si="6">+AG15+AH15+AI15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" ref="AF15" si="7">+AG15*3+AH15</f>
@@ -44557,27 +44565,27 @@
       </c>
       <c r="AI15" s="53" cm="1">
         <f t="array" ref="AI15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ15" s="53" cm="1">
         <f t="array" ref="AJ15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)+($K$9:$K$22=$AD15)*($J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="53" cm="1">
         <f t="array" ref="AK15">SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.3410149999999996</v>
+        <v>4.433015000000001</v>
       </c>
       <c r="AO15" s="53">
         <f t="shared" ref="AO15" si="8">+_xlfn.RANK.EQ(AN15,$AN$9:$AN$15,1)</f>
@@ -44597,7 +44605,7 @@
 (SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AS$7)))*100
 +SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($J$9:$J$22)*($G$9:$G$22=AS$7))
 -SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22)*($G$9:$G$22=AS$7))</f>
-        <v>100</v>
+        <v>-2</v>
       </c>
       <c r="AT15" s="53" cm="1">
         <f t="array" ref="AT15">(SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AT$7)))*300+
@@ -48230,9 +48238,9 @@
       <c r="M9" s="6"/>
       <c r="N9" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="N9" ca="1">INDIRECT(RIGHT(B9,1)&amp;"!P"&amp;7+LEFT(B9,1)*2)</f>
-        <v>México</v>
-      </c>
-      <c r="O9" s="180" t="e" vm="7">
+        <v>Ecuador</v>
+      </c>
+      <c r="O9" s="180" t="e" vm="5">
         <f ca="1">IFERROR(VLOOKUP(N9,Aux!$A:$C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
@@ -50344,13 +50352,13 @@
       <c r="M12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="68" t="str">
+      <c r="N12" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O12" s="68" t="str">
+        <v>3</v>
+      </c>
+      <c r="O12" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>15</v>
@@ -50405,13 +50413,13 @@
       <c r="M13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="68" t="str">
+      <c r="N13" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O13" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="O13" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
final 2 ronda grupo c
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A6CA7-DF0C-469E-AE1E-CAF0CC9C5482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43629719-881A-4DA4-B9DE-906FB5CBF499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="G5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:G4),0))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:H4),0))</f>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>70.012</v>
+        <v>75.012</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="U5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="V5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>50.005000000000003</v>
+        <v>55.005000000000003</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10015,7 +10015,7 @@
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>70.010999999999996</v>
+        <v>75.010999999999996</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10067,7 +10067,7 @@
       </c>
       <c r="U6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="V6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>45.006</v>
+        <v>50.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10117,7 +10117,7 @@
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
@@ -10125,7 +10125,7 @@
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>60.012999999999998</v>
+        <v>65.013000000000005</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10169,7 +10169,7 @@
       </c>
       <c r="U7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>55.006999999999998</v>
+        <v>60.006999999999998</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10219,7 +10219,7 @@
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>60.009</v>
+        <v>65.009</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10271,7 +10271,7 @@
       </c>
       <c r="U8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>50.008000000000003</v>
+        <v>55.008000000000003</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10321,7 +10321,7 @@
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>55.006999999999998</v>
+        <v>60.006999999999998</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="U9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10381,7 +10381,7 @@
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>60.009</v>
+        <v>65.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10423,7 +10423,7 @@
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>50.008000000000003</v>
+        <v>55.008000000000003</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10475,7 +10475,7 @@
       </c>
       <c r="U10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="V10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>40.01</v>
+        <v>45.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10525,7 +10525,7 @@
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>50.005000000000003</v>
+        <v>55.005000000000003</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10577,7 +10577,7 @@
       </c>
       <c r="U11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>70.010999999999996</v>
+        <v>75.010999999999996</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10627,7 +10627,7 @@
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:H11),0))</f>
@@ -10635,7 +10635,7 @@
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>45.006</v>
+        <v>50.006</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10679,7 +10679,7 @@
       </c>
       <c r="U12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="V12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>70.012</v>
+        <v>75.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10729,7 +10729,7 @@
       </c>
       <c r="G13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:G12),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:H12),0))</f>
@@ -10737,7 +10737,7 @@
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>40.01</v>
+        <v>45.01</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10781,7 +10781,7 @@
       </c>
       <c r="U13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>60.012999999999998</v>
+        <v>65.013000000000005</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12233,7 +12233,7 @@
   <dimension ref="A1:AE37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12261,33 +12261,33 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="173">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C1" s="207"/>
       <c r="D1" s="207">
         <f>+A1</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="207"/>
       <c r="G1" s="207">
         <f>+D1+1</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H1" s="207"/>
       <c r="I1" s="207"/>
       <c r="J1" s="207">
         <f t="shared" ref="J1" si="0">+G1+1</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207">
         <f t="shared" ref="M1" si="1">+J1+1</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S1" s="176" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="T1" s="208"/>
       <c r="U1" s="208"/>
@@ -12400,25 +12400,25 @@
       <c r="C5" s="146"/>
       <c r="D5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(D1,Aux!$F:$O,8,0)</f>
-        <v>Grupo A</v>
+        <v>Grupo C</v>
       </c>
       <c r="E5" s="297"/>
       <c r="F5" s="298"/>
       <c r="G5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(G1,Aux!$F:$O,8,0)</f>
-        <v>Grupo A</v>
+        <v>Grupo C</v>
       </c>
       <c r="H5" s="297"/>
       <c r="I5" s="298"/>
       <c r="J5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(J1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo D</v>
       </c>
       <c r="K5" s="297"/>
       <c r="L5" s="298"/>
       <c r="M5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(M1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo D</v>
       </c>
       <c r="N5" s="297"/>
       <c r="O5" s="298"/>
@@ -12426,30 +12426,22 @@
       <c r="R5" s="214"/>
       <c r="S5" s="215"/>
       <c r="T5" s="216" t="str" cm="1">
-        <f t="array" ref="T5:AA5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
-        <v>Cuartos1</v>
+        <f t="array" ref="T5:W5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
+        <v>CampeonG1</v>
       </c>
       <c r="U5" s="216" t="str">
-        <v>Cuartos2</v>
+        <v>CampeonG2</v>
       </c>
       <c r="V5" s="216" t="str">
-        <v>Cuartos3</v>
+        <v>CampeonG3</v>
       </c>
       <c r="W5" s="216" t="str">
-        <v>Cuartos4</v>
-      </c>
-      <c r="X5" s="216" t="str">
-        <v>Cuartos5</v>
-      </c>
-      <c r="Y5" s="216" t="str">
-        <v>Cuartos6</v>
-      </c>
-      <c r="Z5" s="216" t="str">
-        <v>Cuartos7</v>
-      </c>
-      <c r="AA5" s="216" t="str">
-        <v>Cuartos8</v>
-      </c>
+        <v>CampeonG4</v>
+      </c>
+      <c r="X5" s="216"/>
+      <c r="Y5" s="216"/>
+      <c r="Z5" s="216"/>
+      <c r="AA5" s="216"/>
       <c r="AB5" s="123"/>
       <c r="AD5" s="207" t="s">
         <v>94</v>
@@ -12463,51 +12455,51 @@
       <c r="C6" s="146"/>
       <c r="D6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,5,0)</f>
-        <v>Perú</v>
+        <v>Panamá</v>
       </c>
       <c r="E6" s="217">
         <f>VLOOKUP(D1,Aux!$F:$O,3,0)</f>
-        <v>45468.708333333336</v>
+        <v>45470.75</v>
       </c>
       <c r="F6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,6,0)</f>
-        <v>Canadá</v>
+        <v>Estados Unidos</v>
       </c>
       <c r="G6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,5,0)</f>
-        <v>Chile</v>
+        <v>Uruguay</v>
       </c>
       <c r="H6" s="217">
         <f>VLOOKUP(G1,Aux!$F:$O,3,0)</f>
-        <v>45468.875</v>
+        <v>45470.875</v>
       </c>
       <c r="I6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,6,0)</f>
-        <v>Argentina</v>
+        <v>Bolivia</v>
       </c>
       <c r="J6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,5,0)</f>
-        <v>Ecuador</v>
+        <v>Colombia</v>
       </c>
       <c r="K6" s="217">
         <f>VLOOKUP(J1,Aux!$F:$O,3,0)</f>
-        <v>45469.625</v>
+        <v>45471.625</v>
       </c>
       <c r="L6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,6,0)</f>
-        <v>Jamaica</v>
+        <v>Costa Rica</v>
       </c>
       <c r="M6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,5,0)</f>
-        <v>Venezuela</v>
+        <v>Paraguay</v>
       </c>
       <c r="N6" s="217">
         <f>VLOOKUP(M1,Aux!$F:$O,3,0)</f>
-        <v>45469.75</v>
+        <v>45471.75</v>
       </c>
       <c r="O6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,6,0)</f>
-        <v>México</v>
+        <v>Brasil</v>
       </c>
       <c r="P6" s="123"/>
       <c r="R6" s="214"/>
@@ -12521,31 +12513,31 @@
       </c>
       <c r="U6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">IF(OR(U$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">IF(OR(V$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="W6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">IF(OR(W$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Brasil</v>
       </c>
       <c r="X6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">IF(OR(X$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y6" ca="1">IF(OR(Y$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z6" ca="1">IF(OR(Z$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA6" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA6" ca="1">IF(OR(AA$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB6" s="123"/>
       <c r="AD6"/>
@@ -12557,25 +12549,25 @@
       <c r="D7" s="299"/>
       <c r="E7" s="220">
         <f>+E6</f>
-        <v>45468.708333333336</v>
+        <v>45470.75</v>
       </c>
       <c r="F7" s="299"/>
       <c r="G7" s="299"/>
       <c r="H7" s="220">
         <f>+H6</f>
-        <v>45468.875</v>
+        <v>45470.875</v>
       </c>
       <c r="I7" s="299"/>
       <c r="J7" s="299"/>
       <c r="K7" s="220">
         <f>+K6</f>
-        <v>45469.625</v>
+        <v>45471.625</v>
       </c>
       <c r="L7" s="299"/>
       <c r="M7" s="299"/>
       <c r="N7" s="220">
         <f>+N6</f>
-        <v>45469.75</v>
+        <v>45471.75</v>
       </c>
       <c r="O7" s="299"/>
       <c r="P7" s="123"/>
@@ -12590,31 +12582,31 @@
       </c>
       <c r="U7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U7" ca="1">IF(OR(U$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V7" ca="1">IF(OR(V$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Colombia</v>
       </c>
       <c r="X7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">IF(OR(X$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="Y7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y7" ca="1">IF(OR(Y$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z7" ca="1">IF(OR(Z$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA7" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA7" ca="1">IF(OR(AA$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="AB7" s="123"/>
       <c r="AD7"/>
@@ -12627,11 +12619,11 @@
       </c>
       <c r="D8" s="221">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="222">
         <f ca="1">+IF(D8="","",IF(D8&gt;F8,1,IF(D8=F8,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="223">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
@@ -12639,39 +12631,39 @@
       </c>
       <c r="G8" s="221">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="222">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="223">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="221">
+        <v>0</v>
+      </c>
+      <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
-        <v>3</v>
-      </c>
-      <c r="K8" s="222">
+        <v/>
+      </c>
+      <c r="K8" s="222" t="str">
         <f ca="1">+IF(J8="","",IF(J8&gt;L8,1,IF(J8=L8,"X",2)))</f>
-        <v>1</v>
-      </c>
-      <c r="L8" s="223">
+        <v/>
+      </c>
+      <c r="L8" s="223" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,10,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="221">
+        <v/>
+      </c>
+      <c r="M8" s="221" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,9,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N8" s="222">
+        <v/>
+      </c>
+      <c r="N8" s="222" t="str">
         <f ca="1">+IF(M8="","",IF(M8&gt;O8,1,IF(M8=O8,"X",2)))</f>
-        <v>1</v>
-      </c>
-      <c r="O8" s="223">
+        <v/>
+      </c>
+      <c r="O8" s="223" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,10,0)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="P8" s="123"/>
       <c r="R8" s="214"/>
@@ -12685,31 +12677,31 @@
       </c>
       <c r="U8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(OR(U$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">IF(OR(V$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">IF(OR(W$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Brasil</v>
       </c>
       <c r="X8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">IF(OR(X$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y8" ca="1">IF(OR(Y$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z8" ca="1">IF(OR(Z$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA8" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA8" ca="1">IF(OR(AA$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB8" s="123"/>
       <c r="AD8"/>
@@ -12729,31 +12721,31 @@
       </c>
       <c r="U9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U9" ca="1">IF(OR(U$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V9" ca="1">IF(OR(V$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">IF(OR(W$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Brasil</v>
       </c>
       <c r="X9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">IF(OR(X$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y9" ca="1">IF(OR(Y$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z9" ca="1">IF(OR(Z$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA9" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA9" ca="1">IF(OR(AA$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB9" s="123"/>
       <c r="AD9"/>
@@ -12775,23 +12767,23 @@
       </c>
       <c r="F10" s="225" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="226">
         <f t="shared" ref="H10" ca="1" si="3">+IF(G10="","",IF(G10&gt;I10,1,IF(G10=I10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="228" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K10" s="226">
         <f t="shared" ref="K10" ca="1" si="4">+IF(J10="","",IF(J10&gt;L10,1,IF(J10=L10,"X",2)))</f>
@@ -12799,7 +12791,7 @@
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12807,11 +12799,11 @@
       </c>
       <c r="N10" s="226">
         <f t="shared" ref="N10" ca="1" si="5">+IF(M10="","",IF(M10&gt;O10,1,IF(M10=O10,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10" s="123"/>
       <c r="R10" s="214"/>
@@ -12825,31 +12817,31 @@
       </c>
       <c r="U10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(OR(U$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(OR(V$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Colombia</v>
       </c>
       <c r="X10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">IF(OR(X$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="Y10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y10" ca="1">IF(OR(Y$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z10" ca="1">IF(OR(Z$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA10" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA10" ca="1">IF(OR(AA$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="AB10" s="123"/>
       <c r="AD10"/>
@@ -12871,23 +12863,23 @@
       </c>
       <c r="F11" s="230" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="231">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
@@ -12895,19 +12887,19 @@
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="231" t="str">
+        <v>1</v>
+      </c>
+      <c r="N11" s="231">
         <f t="shared" ref="N11:N29" ca="1" si="9">+IF(M11="","",IF(M11&gt;O11,1,IF(M11=O11,"X",2)))</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="O11" s="233" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" s="123"/>
       <c r="R11" s="214"/>
@@ -12921,31 +12913,31 @@
       </c>
       <c r="U11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(OR(U$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(OR(V$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="W11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">IF(OR(W$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Brasil</v>
       </c>
       <c r="X11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">IF(OR(X$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">IF(OR(Y$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">IF(OR(Z$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA11" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">IF(OR(AA$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB11" s="123"/>
       <c r="AD11"/>
@@ -12971,15 +12963,15 @@
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -12995,15 +12987,15 @@
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="233" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P12" s="123"/>
       <c r="R12" s="214"/>
@@ -13017,31 +13009,31 @@
       </c>
       <c r="U12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">IF(OR(U$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">IF(OR(V$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W12" ca="1">IF(OR(W$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Brasil</v>
       </c>
       <c r="X12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">IF(OR(X$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y12" ca="1">IF(OR(Y$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z12" ca="1">IF(OR(Z$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA12" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA12" ca="1">IF(OR(AA$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB12" s="123"/>
       <c r="AD12"/>
@@ -13063,23 +13055,23 @@
       </c>
       <c r="F13" s="230" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="233" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13091,15 +13083,15 @@
       </c>
       <c r="M13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="233" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P13" s="123"/>
       <c r="R13" s="214"/>
@@ -13113,31 +13105,31 @@
       </c>
       <c r="U13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U13" ca="1">IF(OR(U$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V13" ca="1">IF(OR(V$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">IF(OR(W$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Brasil</v>
       </c>
       <c r="X13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">IF(OR(X$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y13" ca="1">IF(OR(Y$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z13" ca="1">IF(OR(Z$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA13" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA13" ca="1">IF(OR(AA$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB13" s="123"/>
       <c r="AD13"/>
@@ -13151,7 +13143,7 @@
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13159,23 +13151,23 @@
       </c>
       <c r="F14" s="230" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H14" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="233" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13187,11 +13179,11 @@
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="233" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13209,31 +13201,31 @@
       </c>
       <c r="U14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">IF(OR(U$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">IF(OR(V$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">IF(OR(W$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Brasil</v>
       </c>
       <c r="X14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X14" ca="1">IF(OR(X$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y14" ca="1">IF(OR(Y$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z14" ca="1">IF(OR(Z$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA14" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA14" ca="1">IF(OR(AA$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB14" s="123"/>
       <c r="AD14"/>
@@ -13247,27 +13239,27 @@
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="231" t="str">
+        <v>1</v>
+      </c>
+      <c r="E15" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H15" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13279,19 +13271,19 @@
       </c>
       <c r="L15" s="230" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P15" s="123"/>
       <c r="R15" s="214"/>
@@ -13351,15 +13343,15 @@
       </c>
       <c r="F16" s="230" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -13367,7 +13359,7 @@
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13375,19 +13367,19 @@
       </c>
       <c r="L16" s="230" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
         <v>2</v>
       </c>
-      <c r="N16" s="231">
+      <c r="N16" s="231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="O16" s="233" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P16" s="123"/>
       <c r="R16" s="214"/>
@@ -13439,27 +13431,27 @@
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="233" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13471,19 +13463,19 @@
       </c>
       <c r="L17" s="230" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="N17" s="231" t="str">
+      <c r="N17" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="123"/>
       <c r="R17" s="214"/>
@@ -13547,15 +13539,15 @@
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13573,13 +13565,13 @@
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="N18" s="231" t="str">
+      <c r="N18" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="O18" s="233" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18" s="123"/>
       <c r="R18" s="214"/>
@@ -19096,29 +19088,29 @@
         <f t="shared" ref="AN3" ca="1" si="10">IF(OR(AL3="",AM3=""),"",IF(AL3&gt;AM3,1,IF(AL3=AM3,"x",2)))</f>
         <v>1</v>
       </c>
-      <c r="AO3" s="191" t="str">
+      <c r="AO3" s="191">
         <f ca="1">VLOOKUP(AO2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AP3" s="191" t="str">
+        <v>2</v>
+      </c>
+      <c r="AP3" s="191">
         <f ca="1">VLOOKUP(AO2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AQ3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="191">
         <f t="shared" ref="AQ3" ca="1" si="11">IF(OR(AO3="",AP3=""),"",IF(AO3&gt;AP3,1,IF(AO3=AP3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="AR3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AR3" s="191">
         <f ca="1">VLOOKUP(AR2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AS3" s="191" t="str">
+        <v>5</v>
+      </c>
+      <c r="AS3" s="191">
         <f ca="1">VLOOKUP(AR2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AT3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="191">
         <f t="shared" ref="AT3" ca="1" si="12">IF(OR(AR3="",AS3=""),"",IF(AR3&gt;AS3,1,IF(AR3=AS3,"x",2)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AU3" s="191" t="str">
         <f ca="1">VLOOKUP(AU2,Aux!$F:$O,9,0)</f>
@@ -20410,7 +20402,7 @@
       </c>
       <c r="AT7">
         <f ca="1">IF($B7=0,0,IF(AND(AR$3=TotalApuestas!AR2,Resultado!AS$3=TotalApuestas!AS2),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT2,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU7">
         <f ca="1">IF($B7=0,0,IF(AU$3=TotalApuestas!AU2,AU$5,0))</f>
@@ -20876,7 +20868,7 @@
       </c>
       <c r="AT8">
         <f ca="1">IF($B8=0,0,IF(AND(AR$3=TotalApuestas!AR3,Resultado!AS$3=TotalApuestas!AS3),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT3,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU8">
         <f ca="1">IF($B8=0,0,IF(AU$3=TotalApuestas!AU3,AU$5,0))</f>
@@ -21342,7 +21334,7 @@
       </c>
       <c r="AT9">
         <f ca="1">IF($B9=0,0,IF(AND(AR$3=TotalApuestas!AR4,Resultado!AS$3=TotalApuestas!AS4),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT4,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU9">
         <f ca="1">IF($B9=0,0,IF(AU$3=TotalApuestas!AU4,AU$5,0))</f>
@@ -21808,7 +21800,7 @@
       </c>
       <c r="AT10">
         <f ca="1">IF($B10=0,0,IF(AND(AR$3=TotalApuestas!AR5,Resultado!AS$3=TotalApuestas!AS5),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT5,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU10">
         <f ca="1">IF($B10=0,0,IF(AU$3=TotalApuestas!AU5,AU$5,0))</f>
@@ -22274,7 +22266,7 @@
       </c>
       <c r="AT11">
         <f ca="1">IF($B11=0,0,IF(AND(AR$3=TotalApuestas!AR6,Resultado!AS$3=TotalApuestas!AS6),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT6,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU11">
         <f ca="1">IF($B11=0,0,IF(AU$3=TotalApuestas!AU6,AU$5,0))</f>
@@ -22740,7 +22732,7 @@
       </c>
       <c r="AT12">
         <f ca="1">IF($B12=0,0,IF(AND(AR$3=TotalApuestas!AR7,Resultado!AS$3=TotalApuestas!AS7),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT7,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU12">
         <f ca="1">IF($B12=0,0,IF(AU$3=TotalApuestas!AU7,AU$5,0))</f>
@@ -23206,7 +23198,7 @@
       </c>
       <c r="AT13">
         <f ca="1">IF($B13=0,0,IF(AND(AR$3=TotalApuestas!AR8,Resultado!AS$3=TotalApuestas!AS8),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT8,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU13">
         <f ca="1">IF($B13=0,0,IF(AU$3=TotalApuestas!AU8,AU$5,0))</f>
@@ -23672,7 +23664,7 @@
       </c>
       <c r="AT14">
         <f ca="1">IF($B14=0,0,IF(AND(AR$3=TotalApuestas!AR9,Resultado!AS$3=TotalApuestas!AS9),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT9,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU14">
         <f ca="1">IF($B14=0,0,IF(AU$3=TotalApuestas!AU9,AU$5,0))</f>
@@ -24138,7 +24130,7 @@
       </c>
       <c r="AT15">
         <f ca="1">IF($B15=0,0,IF(AND(AR$3=TotalApuestas!AR10,Resultado!AS$3=TotalApuestas!AS10),Resultado!AT$5+VLOOKUP(AT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AT$3=TotalApuestas!AT10,AT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU15">
         <f ca="1">IF($B15=0,0,IF(AU$3=TotalApuestas!AU10,AU$5,0))</f>
@@ -41385,29 +41377,29 @@
         <f ca="1">+Resultado!AN3</f>
         <v>1</v>
       </c>
-      <c r="AO1" s="84" t="str">
+      <c r="AO1" s="84">
         <f ca="1">+Resultado!AO3</f>
-        <v/>
-      </c>
-      <c r="AP1" s="84" t="str">
+        <v>2</v>
+      </c>
+      <c r="AP1" s="84">
         <f ca="1">+Resultado!AP3</f>
-        <v/>
-      </c>
-      <c r="AQ1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AQ1" s="84">
         <f ca="1">+Resultado!AQ3</f>
-        <v/>
-      </c>
-      <c r="AR1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AR1" s="84">
         <f ca="1">+Resultado!AR3</f>
-        <v/>
-      </c>
-      <c r="AS1" s="84" t="str">
+        <v>5</v>
+      </c>
+      <c r="AS1" s="84">
         <f ca="1">+Resultado!AS3</f>
-        <v/>
-      </c>
-      <c r="AT1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="AT1" s="84">
         <f ca="1">+Resultado!AT3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AU1" s="84" t="str">
         <f ca="1">+Resultado!AU3</f>
@@ -44929,7 +44921,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -45204,11 +45196,11 @@
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU5" s="245">
         <f>+VLOOKUP(AU7,$AD$9:$AF$15,3,0)</f>
@@ -45471,11 +45463,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -45487,7 +45479,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -45495,7 +45487,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -45509,7 +45501,7 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
@@ -45525,27 +45517,27 @@
       </c>
       <c r="AI9" s="53" cm="1">
         <f t="array" ref="AI9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL9" s="252">
         <f>+SUMIFS($AR9:$AU9,$AR$5:$AU$5,AF9)</f>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="AM9" s="252">
         <f>+AJ9-AK9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN9" s="53">
         <f>+_xlfn.RANK.EQ(AF9,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM9,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ9,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL9,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.1210089999999999</v>
+        <v>2.2240090000000001</v>
       </c>
       <c r="AO9" s="53">
         <f>+_xlfn.RANK.EQ(AN9,$AN$9:$AN$15,1)</f>
@@ -45572,7 +45564,7 @@
 (SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="AU9" s="53" cm="1">
         <f t="array" ref="AU9">(SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -45699,19 +45691,19 @@
       </c>
       <c r="V11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,6,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,7,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,8,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="161">
         <f>+W11-X11</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="60"/>
       <c r="AA11" s="59"/>
@@ -45725,15 +45717,15 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11" si="0">+AG11+AH11+AI11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11" si="1">+AG11*3+AH11</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AG11" s="53" cm="1">
         <f t="array" ref="AG11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11" s="53" cm="1">
         <f t="array" ref="AH11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -45745,7 +45737,7 @@
       </c>
       <c r="AJ11" s="53" cm="1">
         <f t="array" ref="AJ11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)+($K$9:$K$22=$AD11)*($J$9:$J$22))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AK11" s="53" cm="1">
         <f t="array" ref="AK11">SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22))</f>
@@ -45753,15 +45745,15 @@
       </c>
       <c r="AL11" s="252">
         <f>+SUMIFS($AR11:$AU11,$AR$5:$AU$5,AF11)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM11" s="252">
         <f>+AJ11-AK11</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.111011</v>
+        <v>1.1120110000000001</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
@@ -45795,7 +45787,7 @@
 (SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AU$7)))*100
 +SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($J$9:$J$22)*($G$9:$G$22=AU$7))
 -SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22)*($G$9:$G$22=AU$7))</f>
-        <v>100</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="2:47" s="54" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -45869,11 +45861,15 @@
         <f>+VLOOKUP(B13,Aux!F:S,5,0)</f>
         <v>Panamá</v>
       </c>
-      <c r="H13" s="258"/>
+      <c r="H13" s="258">
+        <v>2</v>
+      </c>
       <c r="I13" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="258"/>
+      <c r="J13" s="258">
+        <v>1</v>
+      </c>
       <c r="K13" s="38" t="str">
         <f>+VLOOKUP(B13,Aux!F:S,6,0)</f>
         <v>Estados Unidos</v>
@@ -45899,11 +45895,11 @@
       <c r="R13" s="158"/>
       <c r="S13" s="159">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,5,0)</f>
@@ -45915,15 +45911,15 @@
       </c>
       <c r="W13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,7,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,8,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y13" s="161">
         <f>+W13-X13</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Z13" s="60"/>
       <c r="AA13" s="57"/>
@@ -45937,15 +45933,15 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" ref="AE13" si="3">+AG13+AH13+AI13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" ref="AF13" si="4">+AG13*3+AH13</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG13" s="53" cm="1">
         <f t="array" ref="AG13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="53" cm="1">
         <f t="array" ref="AH13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -45957,23 +45953,23 @@
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.3310129999999996</v>
+        <v>2.3210129999999998</v>
       </c>
       <c r="AO13" s="53">
         <f t="shared" ref="AO13" si="5">+_xlfn.RANK.EQ(AN13,$AN$9:$AN$15,1)</f>
@@ -45986,7 +45982,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AR$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AR$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AR$7))</f>
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="AS13" s="53" cm="1">
         <f t="array" ref="AS13">(SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AS$7)))*300+
@@ -46081,11 +46077,15 @@
         <f>+VLOOKUP(B15,Aux!F:S,5,0)</f>
         <v>Uruguay</v>
       </c>
-      <c r="H15" s="258"/>
+      <c r="H15" s="258">
+        <v>5</v>
+      </c>
       <c r="I15" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="258"/>
+      <c r="J15" s="258">
+        <v>0</v>
+      </c>
       <c r="K15" s="38" t="str">
         <f>+VLOOKUP(B15,Aux!F:S,6,0)</f>
         <v>Bolivia</v>
@@ -46123,7 +46123,7 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
@@ -46131,11 +46131,11 @@
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -46149,7 +46149,7 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" ref="AE15" si="6">+AG15+AH15+AI15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" ref="AF15" si="7">+AG15*3+AH15</f>
@@ -46165,7 +46165,7 @@
       </c>
       <c r="AI15" s="53" cm="1">
         <f t="array" ref="AI15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ15" s="53" cm="1">
         <f t="array" ref="AJ15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)+($K$9:$K$22=$AD15)*($J$9:$J$22))</f>
@@ -46173,19 +46173,19 @@
       </c>
       <c r="AK15" s="53" cm="1">
         <f t="array" ref="AK15">SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.3410149999999996</v>
+        <v>4.4420150000000005</v>
       </c>
       <c r="AO15" s="53">
         <f t="shared" ref="AO15" si="8">+_xlfn.RANK.EQ(AN15,$AN$9:$AN$15,1)</f>
@@ -46205,7 +46205,7 @@
 (SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AS$7)))*100
 +SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($J$9:$J$22)*($G$9:$G$22=AS$7))
 -SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22)*($G$9:$G$22=AS$7))</f>
-        <v>100</v>
+        <v>-5</v>
       </c>
       <c r="AT15" s="53" cm="1">
         <f t="array" ref="AT15">(SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AT$7)))*300+
@@ -50474,13 +50474,13 @@
       <c r="M14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="68" t="str">
+      <c r="N14" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O14" s="68" t="str">
+        <v>2</v>
+      </c>
+      <c r="O14" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>17</v>
@@ -50535,13 +50535,13 @@
       <c r="M15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="68" t="str">
+      <c r="N15" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O15" s="68" t="str">
+        <v>5</v>
+      </c>
+      <c r="O15" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fin de jornada 2 D
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43629719-881A-4DA4-B9DE-906FB5CBF499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3920319A-5367-4941-B328-0D2750E37A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -9917,11 +9917,11 @@
       </c>
       <c r="H5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:H4),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>75.012</v>
+        <v>85.012</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="Q5" s="119">
         <f t="shared" ref="Q5:Q26" ca="1" si="0">+_xlfn.RANK.EQ(AB5,$AB$5:$AB$26)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R5" s="126" t="str">
         <f>Resultado!B7</f>
@@ -9969,11 +9969,11 @@
       </c>
       <c r="V5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>55.005000000000003</v>
+        <v>60.005000000000003</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10019,11 +10019,11 @@
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>75.010999999999996</v>
+        <v>85.010999999999996</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="Q6" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R6" s="126" t="str">
         <f>Resultado!B8</f>
@@ -10071,11 +10071,11 @@
       </c>
       <c r="V6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>50.006</v>
+        <v>60.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10121,11 +10121,11 @@
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>65.013000000000005</v>
+        <v>75.013000000000005</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10173,11 +10173,11 @@
       </c>
       <c r="V7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>60.006999999999998</v>
+        <v>75.007000000000005</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10223,11 +10223,11 @@
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>65.009</v>
+        <v>75.009</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10275,11 +10275,11 @@
       </c>
       <c r="V8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>55.008000000000003</v>
+        <v>65.007999999999996</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10325,11 +10325,11 @@
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>60.006999999999998</v>
+        <v>75.007000000000005</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10377,11 +10377,11 @@
       </c>
       <c r="V9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>65.009</v>
+        <v>75.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10427,11 +10427,11 @@
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>55.008000000000003</v>
+        <v>65.007999999999996</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10479,11 +10479,11 @@
       </c>
       <c r="V10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>45.01</v>
+        <v>55.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10513,7 +10513,7 @@
       </c>
       <c r="D11" s="151" t="str">
         <f ca="1">+VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:D10),0)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
@@ -10521,7 +10521,7 @@
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
@@ -10529,11 +10529,11 @@
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>55.005000000000003</v>
+        <v>60.006</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10581,11 +10581,11 @@
       </c>
       <c r="V11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>75.010999999999996</v>
+        <v>85.010999999999996</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10615,7 +10615,7 @@
       </c>
       <c r="D12" s="151" t="str">
         <f ca="1">+VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:D11),0)</f>
-        <v>Cazaputas69</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="E12" s="197">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:E11),0))</f>
@@ -10623,7 +10623,7 @@
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
@@ -10631,11 +10631,11 @@
       </c>
       <c r="H12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:H11),0))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>50.006</v>
+        <v>60.005000000000003</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10683,11 +10683,11 @@
       </c>
       <c r="V12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>75.012</v>
+        <v>85.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10733,11 +10733,11 @@
       </c>
       <c r="H13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:H12),0))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>45.01</v>
+        <v>55.01</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10785,11 +10785,11 @@
       </c>
       <c r="V13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>65.013000000000005</v>
+        <v>75.013000000000005</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12641,29 +12641,29 @@
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="221" t="str">
+      <c r="J8" s="221">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="K8" s="222" t="str">
+        <v>3</v>
+      </c>
+      <c r="K8" s="222">
         <f ca="1">+IF(J8="","",IF(J8&gt;L8,1,IF(J8=L8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="L8" s="223" t="str">
+        <v>1</v>
+      </c>
+      <c r="L8" s="223">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="M8" s="221" t="str">
+        <v>0</v>
+      </c>
+      <c r="M8" s="221">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="N8" s="222" t="str">
+        <v>1</v>
+      </c>
+      <c r="N8" s="222">
         <f ca="1">+IF(M8="","",IF(M8&gt;O8,1,IF(M8=O8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="O8" s="223" t="str">
+        <v>2</v>
+      </c>
+      <c r="O8" s="223">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="P8" s="123"/>
       <c r="R8" s="214"/>
@@ -13001,7 +13001,7 @@
       <c r="R12" s="214"/>
       <c r="S12" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="T12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">IF(OR(T$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13097,7 +13097,7 @@
       <c r="R13" s="214"/>
       <c r="S13" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Cazaputas69</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="T13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">IF(OR(T$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13331,11 +13331,11 @@
       <c r="B16" s="214"/>
       <c r="C16" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13347,7 +13347,7 @@
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -13355,11 +13355,11 @@
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13371,11 +13371,11 @@
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
+        <v>1</v>
+      </c>
+      <c r="N16" s="231">
+        <f t="shared" ca="1" si="9"/>
         <v>2</v>
-      </c>
-      <c r="N16" s="231" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>X</v>
       </c>
       <c r="O16" s="233" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13427,11 +13427,11 @@
       <c r="B17" s="214"/>
       <c r="C17" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Cazaputas69</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13443,7 +13443,7 @@
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H17" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -13451,11 +13451,11 @@
       </c>
       <c r="I17" s="233" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13467,11 +13467,11 @@
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="N17" s="231">
+        <v>2</v>
+      </c>
+      <c r="N17" s="231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -19112,29 +19112,29 @@
         <f t="shared" ref="AT3" ca="1" si="12">IF(OR(AR3="",AS3=""),"",IF(AR3&gt;AS3,1,IF(AR3=AS3,"x",2)))</f>
         <v>1</v>
       </c>
-      <c r="AU3" s="191" t="str">
+      <c r="AU3" s="191">
         <f ca="1">VLOOKUP(AU2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AV3" s="191" t="str">
+        <v>3</v>
+      </c>
+      <c r="AV3" s="191">
         <f ca="1">VLOOKUP(AU2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AW3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="191">
         <f t="shared" ref="AW3" ca="1" si="13">IF(OR(AU3="",AV3=""),"",IF(AU3&gt;AV3,1,IF(AU3=AV3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="AX3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="191">
         <f ca="1">VLOOKUP(AX2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="AY3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="191">
         <f ca="1">VLOOKUP(AX2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="AZ3" s="191" t="str">
+        <v>4</v>
+      </c>
+      <c r="AZ3" s="191">
         <f t="shared" ref="AZ3" ca="1" si="14">IF(OR(AX3="",AY3=""),"",IF(AX3&gt;AY3,1,IF(AX3=AY3,"x",2)))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="BA3" s="191" t="str">
         <f ca="1">VLOOKUP(BA2,Aux!$F:$O,9,0)</f>
@@ -20414,7 +20414,7 @@
       </c>
       <c r="AW7">
         <f ca="1">IF($B7=0,0,IF(AND(AU$3=TotalApuestas!AU2,Resultado!AV$3=TotalApuestas!AV2),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW2,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX7">
         <f ca="1">IF($B7=0,0,IF(AX$3=TotalApuestas!AX2,AX$5,0))</f>
@@ -20880,7 +20880,7 @@
       </c>
       <c r="AW8">
         <f ca="1">IF($B8=0,0,IF(AND(AU$3=TotalApuestas!AU3,Resultado!AV$3=TotalApuestas!AV3),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW3,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX8">
         <f ca="1">IF($B8=0,0,IF(AX$3=TotalApuestas!AX3,AX$5,0))</f>
@@ -20892,7 +20892,7 @@
       </c>
       <c r="AZ8">
         <f ca="1">IF($B8=0,0,IF(AND(AX$3=TotalApuestas!AX3,Resultado!AY$3=TotalApuestas!AY3),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ3,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA8">
         <f ca="1">IF($B8=0,0,IF(BA$3=TotalApuestas!BA3,BA$5,0))</f>
@@ -21346,7 +21346,7 @@
       </c>
       <c r="AW9">
         <f ca="1">IF($B9=0,0,IF(AND(AU$3=TotalApuestas!AU4,Resultado!AV$3=TotalApuestas!AV4),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW4,AW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AX9">
         <f ca="1">IF($B9=0,0,IF(AX$3=TotalApuestas!AX4,AX$5,0))</f>
@@ -21358,7 +21358,7 @@
       </c>
       <c r="AZ9">
         <f ca="1">IF($B9=0,0,IF(AND(AX$3=TotalApuestas!AX4,Resultado!AY$3=TotalApuestas!AY4),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ4,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA9">
         <f ca="1">IF($B9=0,0,IF(BA$3=TotalApuestas!BA4,BA$5,0))</f>
@@ -21812,7 +21812,7 @@
       </c>
       <c r="AW10">
         <f ca="1">IF($B10=0,0,IF(AND(AU$3=TotalApuestas!AU5,Resultado!AV$3=TotalApuestas!AV5),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW5,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX10">
         <f ca="1">IF($B10=0,0,IF(AX$3=TotalApuestas!AX5,AX$5,0))</f>
@@ -21824,7 +21824,7 @@
       </c>
       <c r="AZ10">
         <f ca="1">IF($B10=0,0,IF(AND(AX$3=TotalApuestas!AX5,Resultado!AY$3=TotalApuestas!AY5),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ5,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA10">
         <f ca="1">IF($B10=0,0,IF(BA$3=TotalApuestas!BA5,BA$5,0))</f>
@@ -22278,7 +22278,7 @@
       </c>
       <c r="AW11">
         <f ca="1">IF($B11=0,0,IF(AND(AU$3=TotalApuestas!AU6,Resultado!AV$3=TotalApuestas!AV6),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW6,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX11">
         <f ca="1">IF($B11=0,0,IF(AX$3=TotalApuestas!AX6,AX$5,0))</f>
@@ -22290,7 +22290,7 @@
       </c>
       <c r="AZ11">
         <f ca="1">IF($B11=0,0,IF(AND(AX$3=TotalApuestas!AX6,Resultado!AY$3=TotalApuestas!AY6),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ6,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA11">
         <f ca="1">IF($B11=0,0,IF(BA$3=TotalApuestas!BA6,BA$5,0))</f>
@@ -22744,7 +22744,7 @@
       </c>
       <c r="AW12">
         <f ca="1">IF($B12=0,0,IF(AND(AU$3=TotalApuestas!AU7,Resultado!AV$3=TotalApuestas!AV7),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW7,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX12">
         <f ca="1">IF($B12=0,0,IF(AX$3=TotalApuestas!AX7,AX$5,0))</f>
@@ -22756,7 +22756,7 @@
       </c>
       <c r="AZ12">
         <f ca="1">IF($B12=0,0,IF(AND(AX$3=TotalApuestas!AX7,Resultado!AY$3=TotalApuestas!AY7),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ7,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA12">
         <f ca="1">IF($B12=0,0,IF(BA$3=TotalApuestas!BA7,BA$5,0))</f>
@@ -23210,7 +23210,7 @@
       </c>
       <c r="AW13">
         <f ca="1">IF($B13=0,0,IF(AND(AU$3=TotalApuestas!AU8,Resultado!AV$3=TotalApuestas!AV8),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW8,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX13">
         <f ca="1">IF($B13=0,0,IF(AX$3=TotalApuestas!AX8,AX$5,0))</f>
@@ -23222,7 +23222,7 @@
       </c>
       <c r="AZ13">
         <f ca="1">IF($B13=0,0,IF(AND(AX$3=TotalApuestas!AX8,Resultado!AY$3=TotalApuestas!AY8),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ8,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA13">
         <f ca="1">IF($B13=0,0,IF(BA$3=TotalApuestas!BA8,BA$5,0))</f>
@@ -23676,7 +23676,7 @@
       </c>
       <c r="AW14">
         <f ca="1">IF($B14=0,0,IF(AND(AU$3=TotalApuestas!AU9,Resultado!AV$3=TotalApuestas!AV9),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW9,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX14">
         <f ca="1">IF($B14=0,0,IF(AX$3=TotalApuestas!AX9,AX$5,0))</f>
@@ -23688,7 +23688,7 @@
       </c>
       <c r="AZ14">
         <f ca="1">IF($B14=0,0,IF(AND(AX$3=TotalApuestas!AX9,Resultado!AY$3=TotalApuestas!AY9),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ9,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA14">
         <f ca="1">IF($B14=0,0,IF(BA$3=TotalApuestas!BA9,BA$5,0))</f>
@@ -24142,7 +24142,7 @@
       </c>
       <c r="AW15">
         <f ca="1">IF($B15=0,0,IF(AND(AU$3=TotalApuestas!AU10,Resultado!AV$3=TotalApuestas!AV10),Resultado!AW$5+VLOOKUP(AW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AW$3=TotalApuestas!AW10,AW$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX15">
         <f ca="1">IF($B15=0,0,IF(AX$3=TotalApuestas!AX10,AX$5,0))</f>
@@ -24154,7 +24154,7 @@
       </c>
       <c r="AZ15">
         <f ca="1">IF($B15=0,0,IF(AND(AX$3=TotalApuestas!AX10,Resultado!AY$3=TotalApuestas!AY10),Resultado!AZ$5+VLOOKUP(AZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(AZ$3=TotalApuestas!AZ10,AZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA15">
         <f ca="1">IF($B15=0,0,IF(BA$3=TotalApuestas!BA10,BA$5,0))</f>
@@ -41401,29 +41401,29 @@
         <f ca="1">+Resultado!AT3</f>
         <v>1</v>
       </c>
-      <c r="AU1" s="84" t="str">
+      <c r="AU1" s="84">
         <f ca="1">+Resultado!AU3</f>
-        <v/>
-      </c>
-      <c r="AV1" s="84" t="str">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="84">
         <f ca="1">+Resultado!AV3</f>
-        <v/>
-      </c>
-      <c r="AW1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="AW1" s="84">
         <f ca="1">+Resultado!AW3</f>
-        <v/>
-      </c>
-      <c r="AX1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AX1" s="84">
         <f ca="1">+Resultado!AX3</f>
-        <v/>
-      </c>
-      <c r="AY1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="AY1" s="84">
         <f ca="1">+Resultado!AY3</f>
-        <v/>
-      </c>
-      <c r="AZ1" s="84" t="str">
+        <v>4</v>
+      </c>
+      <c r="AZ1" s="84">
         <f ca="1">+Resultado!AZ3</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="BA1" s="84" t="str">
         <f ca="1">+Resultado!BA3</f>
@@ -46529,7 +46529,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46800,11 +46800,11 @@
       <c r="AQ5" s="53"/>
       <c r="AR5" s="245">
         <f>+VLOOKUP(AR7,$AD$9:$AF$15,3,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
@@ -47071,11 +47071,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -47087,7 +47087,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -47095,7 +47095,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -47109,15 +47109,15 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG9" s="53" cm="1">
         <f t="array" ref="AG9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9" s="53" cm="1">
         <f t="array" ref="AH9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -47129,23 +47129,23 @@
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL9" s="252">
         <f>+SUMIFS($AR9:$AU9,$AR$5:$AU$5,AF9)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM9" s="252">
         <f>+AJ9-AK9</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN9" s="53">
         <f>+_xlfn.RANK.EQ(AF9,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM9,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ9,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL9,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>2.2310089999999998</v>
+        <v>2.221009</v>
       </c>
       <c r="AO9" s="53">
         <f>+_xlfn.RANK.EQ(AN9,$AN$9:$AN$15,1)</f>
@@ -47172,7 +47172,7 @@
 (SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>303</v>
       </c>
       <c r="AU9" s="53" cm="1">
         <f t="array" ref="AU9">(SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -47287,11 +47287,11 @@
       <c r="R11" s="158"/>
       <c r="S11" s="159">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,3,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,5,0)</f>
@@ -47303,15 +47303,15 @@
       </c>
       <c r="W11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,7,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,8,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="161">
         <f>+W11-X11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z11" s="60"/>
       <c r="AA11" s="59"/>
@@ -47325,15 +47325,15 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11" si="0">+AG11+AH11+AI11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11" si="1">+AG11*3+AH11</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AG11" s="53" cm="1">
         <f t="array" ref="AG11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11" s="53" cm="1">
         <f t="array" ref="AH11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -47345,7 +47345,7 @@
       </c>
       <c r="AJ11" s="53" cm="1">
         <f t="array" ref="AJ11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)+($K$9:$K$22=$AD11)*($J$9:$J$22))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AK11" s="53" cm="1">
         <f t="array" ref="AK11">SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22))</f>
@@ -47357,11 +47357,11 @@
       </c>
       <c r="AM11" s="252">
         <f>+AJ11-AK11</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.113011</v>
+        <v>1.111011</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
@@ -47395,7 +47395,7 @@
 (SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AU$7)))*100
 +SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($J$9:$J$22)*($G$9:$G$22=AU$7))
 -SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD11)*($H$9:$H$22)*($G$9:$G$22=AU$7))</f>
-        <v>100</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="2:47" s="54" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -47469,11 +47469,15 @@
         <f>+VLOOKUP(B13,Aux!F:S,5,0)</f>
         <v>Colombia</v>
       </c>
-      <c r="H13" s="258"/>
+      <c r="H13" s="258">
+        <v>3</v>
+      </c>
       <c r="I13" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="258"/>
+      <c r="J13" s="258">
+        <v>0</v>
+      </c>
       <c r="K13" s="38" t="str">
         <f>+VLOOKUP(B13,Aux!F:S,6,0)</f>
         <v>Costa Rica</v>
@@ -47511,7 +47515,7 @@
       </c>
       <c r="V13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,6,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,7,0)</f>
@@ -47519,11 +47523,11 @@
       </c>
       <c r="X13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,8,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y13" s="161">
         <f>+W13-X13</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="Z13" s="60"/>
       <c r="AA13" s="57"/>
@@ -47537,7 +47541,7 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" ref="AE13" si="3">+AG13+AH13+AI13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" ref="AF13" si="4">+AG13*3+AH13</f>
@@ -47553,15 +47557,15 @@
       </c>
       <c r="AI13" s="53" cm="1">
         <f t="array" ref="AI13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
@@ -47569,11 +47573,11 @@
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>4.4230130000000001</v>
+        <v>4.431013000000001</v>
       </c>
       <c r="AO13" s="53">
         <f t="shared" ref="AO13" si="5">+_xlfn.RANK.EQ(AN13,$AN$9:$AN$15,1)</f>
@@ -47586,7 +47590,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AR$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AR$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AR$7))</f>
-        <v>100</v>
+        <v>-3</v>
       </c>
       <c r="AS13" s="53" cm="1">
         <f t="array" ref="AS13">(SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AS$7)))*300+
@@ -47681,11 +47685,15 @@
         <f>+VLOOKUP(B15,Aux!F:S,5,0)</f>
         <v>Paraguay</v>
       </c>
-      <c r="H15" s="258"/>
+      <c r="H15" s="258">
+        <v>1</v>
+      </c>
       <c r="I15" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="258"/>
+      <c r="J15" s="258">
+        <v>4</v>
+      </c>
       <c r="K15" s="38" t="str">
         <f>+VLOOKUP(B15,Aux!F:S,6,0)</f>
         <v>Brasil</v>
@@ -47723,19 +47731,19 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -47749,7 +47757,7 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" ref="AE15" si="6">+AG15+AH15+AI15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" ref="AF15" si="7">+AG15*3+AH15</f>
@@ -47765,7 +47773,7 @@
       </c>
       <c r="AI15" s="53" cm="1">
         <f t="array" ref="AI15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="53" cm="1">
         <f t="array" ref="AJ15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)+($K$9:$K$22=$AD15)*($J$9:$J$22))</f>
@@ -47773,19 +47781,19 @@
       </c>
       <c r="AK15" s="53" cm="1">
         <f t="array" ref="AK15">SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>2.2310149999999997</v>
+        <v>3.3410149999999996</v>
       </c>
       <c r="AO15" s="53">
         <f t="shared" ref="AO15" si="8">+_xlfn.RANK.EQ(AN15,$AN$9:$AN$15,1)</f>
@@ -47805,7 +47813,7 @@
 (SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AS$7)))*100
 +SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($J$9:$J$22)*($G$9:$G$22=AS$7))
 -SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD15)*($H$9:$H$22)*($G$9:$G$22=AS$7))</f>
-        <v>100</v>
+        <v>-3</v>
       </c>
       <c r="AT15" s="53" cm="1">
         <f t="array" ref="AT15">(SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AT$7)))*300+
@@ -50596,13 +50604,13 @@
       <c r="M16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="68" t="str">
+      <c r="N16" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O16" s="68" t="str">
+        <v>3</v>
+      </c>
+      <c r="O16" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>17</v>
@@ -50657,13 +50665,13 @@
       <c r="M17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="68" t="str">
+      <c r="N17" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O17" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="O17" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fin de la jornada 3 A
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3920319A-5367-4941-B328-0D2750E37A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE389E2-5430-4DC8-8DF8-E1D462DDE37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -9901,11 +9901,11 @@
       </c>
       <c r="D5" s="151" t="str">
         <f ca="1">+VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:D4),0)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="E5" s="197">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:E4),0))</f>
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="F5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:F4),0))</f>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="G5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:G4),0))</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:H4),0))</f>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>85.012</v>
+        <v>110.011</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="Q5" s="119">
         <f t="shared" ref="Q5:Q26" ca="1" si="0">+_xlfn.RANK.EQ(AB5,$AB$5:$AB$26)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R5" s="126" t="str">
         <f>Resultado!B7</f>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="S5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="T5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>60.005000000000003</v>
+        <v>80.004999999999995</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10003,11 +10003,11 @@
       </c>
       <c r="D6" s="151" t="str">
         <f ca="1">+VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:D5),0)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
@@ -10015,7 +10015,7 @@
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>85.010999999999996</v>
+        <v>100.012</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="Q6" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R6" s="126" t="str">
         <f>Resultado!B8</f>
@@ -10059,7 +10059,7 @@
       </c>
       <c r="S6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="T6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>60.006</v>
+        <v>85.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10105,15 +10105,15 @@
       </c>
       <c r="D7" s="151" t="str">
         <f ca="1">+VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:D6),0)</f>
-        <v>Moises</v>
+        <v>YUTA</v>
       </c>
       <c r="E7" s="197">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:E6),0))</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
@@ -10121,11 +10121,11 @@
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>75.013000000000005</v>
+        <v>100.009</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10153,7 +10153,7 @@
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R7" s="126" t="str">
         <f>Resultado!B9</f>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="S7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="T7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>75.007000000000005</v>
+        <v>100.00700000000001</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10207,15 +10207,15 @@
       </c>
       <c r="D8" s="152" t="str">
         <f ca="1">+VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:D7),0)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="E8" s="201">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:E7),0))</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
@@ -10223,11 +10223,11 @@
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>75.009</v>
+        <v>100.00700000000001</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10263,7 +10263,7 @@
       </c>
       <c r="S8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="T8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>65.007999999999996</v>
+        <v>85.007999999999996</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10309,15 +10309,15 @@
       </c>
       <c r="D9" s="153" t="str">
         <f ca="1">+VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:D8),0)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>Moises</v>
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
@@ -10325,11 +10325,11 @@
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>75.007000000000005</v>
+        <v>90.013000000000005</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="Q9" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R9" s="126" t="str">
         <f>Resultado!B11</f>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="S9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="T9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10381,7 +10381,7 @@
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>75.009</v>
+        <v>100.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10411,27 +10411,27 @@
       </c>
       <c r="D10" s="151" t="str">
         <f ca="1">+VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:D9),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>65.007999999999996</v>
+        <v>90.01</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="S10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="T10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>55.01</v>
+        <v>90.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10513,19 +10513,19 @@
       </c>
       <c r="D11" s="151" t="str">
         <f ca="1">+VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:D10),0)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>60.006</v>
+        <v>85.007999999999996</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10561,7 +10561,7 @@
       </c>
       <c r="Q11" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11" s="126" t="str">
         <f>Resultado!B13</f>
@@ -10569,7 +10569,7 @@
       </c>
       <c r="S11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="T11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>85.010999999999996</v>
+        <v>110.011</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10615,15 +10615,15 @@
       </c>
       <c r="D12" s="151" t="str">
         <f ca="1">+VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:D11),0)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="E12" s="197">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:E11),0))</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
@@ -10631,11 +10631,11 @@
       </c>
       <c r="H12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:H11),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>60.005000000000003</v>
+        <v>85.006</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10663,7 +10663,7 @@
       </c>
       <c r="Q12" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="126" t="str">
         <f>Resultado!B14</f>
@@ -10671,7 +10671,7 @@
       </c>
       <c r="S12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="T12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>85.012</v>
+        <v>100.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10717,15 +10717,15 @@
       </c>
       <c r="D13" s="152" t="str">
         <f ca="1">+VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:D12),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="E13" s="201">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:E12),0))</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:F12),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:G12),0))</f>
@@ -10737,7 +10737,7 @@
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>55.01</v>
+        <v>80.004999999999995</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10765,7 +10765,7 @@
       </c>
       <c r="Q13" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R13" s="126" t="str">
         <f>Resultado!B15</f>
@@ -10773,7 +10773,7 @@
       </c>
       <c r="S13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="T13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>75.013000000000005</v>
+        <v>90.013000000000005</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12261,30 +12261,30 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="173">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="207"/>
       <c r="D1" s="207">
         <f>+A1</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="207"/>
       <c r="G1" s="207">
         <f>+D1+1</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H1" s="207"/>
       <c r="I1" s="207"/>
       <c r="J1" s="207">
         <f t="shared" ref="J1" si="0">+G1+1</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207">
         <f t="shared" ref="M1" si="1">+J1+1</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="S1" s="176" t="s">
         <v>174</v>
@@ -12400,25 +12400,25 @@
       <c r="C5" s="146"/>
       <c r="D5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(D1,Aux!$F:$O,8,0)</f>
-        <v>Grupo C</v>
+        <v>Grupo A</v>
       </c>
       <c r="E5" s="297"/>
       <c r="F5" s="298"/>
       <c r="G5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(G1,Aux!$F:$O,8,0)</f>
-        <v>Grupo C</v>
+        <v>Grupo A</v>
       </c>
       <c r="H5" s="297"/>
       <c r="I5" s="298"/>
       <c r="J5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(J1,Aux!$F:$O,8,0)</f>
-        <v>Grupo D</v>
+        <v>Grupo B</v>
       </c>
       <c r="K5" s="297"/>
       <c r="L5" s="298"/>
       <c r="M5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(M1,Aux!$F:$O,8,0)</f>
-        <v>Grupo D</v>
+        <v>Grupo B</v>
       </c>
       <c r="N5" s="297"/>
       <c r="O5" s="298"/>
@@ -12455,57 +12455,57 @@
       <c r="C6" s="146"/>
       <c r="D6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,5,0)</f>
-        <v>Panamá</v>
+        <v>Argentina</v>
       </c>
       <c r="E6" s="217">
         <f>VLOOKUP(D1,Aux!$F:$O,3,0)</f>
-        <v>45470.75</v>
+        <v>45472.833333333336</v>
       </c>
       <c r="F6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,6,0)</f>
-        <v>Estados Unidos</v>
+        <v>Perú</v>
       </c>
       <c r="G6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,5,0)</f>
-        <v>Uruguay</v>
+        <v>Canadá</v>
       </c>
       <c r="H6" s="217">
         <f>VLOOKUP(G1,Aux!$F:$O,3,0)</f>
-        <v>45470.875</v>
+        <v>45472.833333333336</v>
       </c>
       <c r="I6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,6,0)</f>
-        <v>Bolivia</v>
+        <v>Chile</v>
       </c>
       <c r="J6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,5,0)</f>
-        <v>Colombia</v>
+        <v>México</v>
       </c>
       <c r="K6" s="217">
         <f>VLOOKUP(J1,Aux!$F:$O,3,0)</f>
-        <v>45471.625</v>
+        <v>45473.708333333336</v>
       </c>
       <c r="L6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,6,0)</f>
-        <v>Costa Rica</v>
+        <v>Ecuador</v>
       </c>
       <c r="M6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,5,0)</f>
-        <v>Paraguay</v>
+        <v>Jamaica</v>
       </c>
       <c r="N6" s="217">
         <f>VLOOKUP(M1,Aux!$F:$O,3,0)</f>
-        <v>45471.75</v>
+        <v>45473.791666666664</v>
       </c>
       <c r="O6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,6,0)</f>
-        <v>Brasil</v>
+        <v>Venezuela</v>
       </c>
       <c r="P6" s="123"/>
       <c r="R6" s="214"/>
       <c r="S6" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D5=0,"",ClasificaciónPorra!D5)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="T6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">IF(OR(T$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="W6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">IF(OR(W$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Colombia</v>
       </c>
       <c r="X6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">IF(OR(X$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -12549,32 +12549,32 @@
       <c r="D7" s="299"/>
       <c r="E7" s="220">
         <f>+E6</f>
-        <v>45470.75</v>
+        <v>45472.833333333336</v>
       </c>
       <c r="F7" s="299"/>
       <c r="G7" s="299"/>
       <c r="H7" s="220">
         <f>+H6</f>
-        <v>45470.875</v>
+        <v>45472.833333333336</v>
       </c>
       <c r="I7" s="299"/>
       <c r="J7" s="299"/>
       <c r="K7" s="220">
         <f>+K6</f>
-        <v>45471.625</v>
+        <v>45473.708333333336</v>
       </c>
       <c r="L7" s="299"/>
       <c r="M7" s="299"/>
       <c r="N7" s="220">
         <f>+N6</f>
-        <v>45471.75</v>
+        <v>45473.791666666664</v>
       </c>
       <c r="O7" s="299"/>
       <c r="P7" s="123"/>
       <c r="R7" s="214"/>
       <c r="S7" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="T7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">IF(OR(T$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12590,7 +12590,7 @@
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="X7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">IF(OR(X$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -12627,49 +12627,49 @@
       </c>
       <c r="F8" s="223">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="221">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v>5</v>
-      </c>
-      <c r="H8" s="222">
+        <v>0</v>
+      </c>
+      <c r="H8" s="222" t="str">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I8" s="223">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="221">
+      <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
-        <v>3</v>
-      </c>
-      <c r="K8" s="222">
+        <v/>
+      </c>
+      <c r="K8" s="222" t="str">
         <f ca="1">+IF(J8="","",IF(J8&gt;L8,1,IF(J8=L8,"X",2)))</f>
-        <v>1</v>
-      </c>
-      <c r="L8" s="223">
+        <v/>
+      </c>
+      <c r="L8" s="223" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="221">
+        <v/>
+      </c>
+      <c r="M8" s="221" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,9,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N8" s="222">
+        <v/>
+      </c>
+      <c r="N8" s="222" t="str">
         <f ca="1">+IF(M8="","",IF(M8&gt;O8,1,IF(M8=O8,"X",2)))</f>
-        <v>2</v>
-      </c>
-      <c r="O8" s="223">
+        <v/>
+      </c>
+      <c r="O8" s="223" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,10,0)</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="P8" s="123"/>
       <c r="R8" s="214"/>
       <c r="S8" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>Moises</v>
+        <v>YUTA</v>
       </c>
       <c r="T8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">IF(OR(T$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12713,7 +12713,7 @@
       <c r="R9" s="214"/>
       <c r="S9" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="T9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">IF(OR(T$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12729,7 +12729,7 @@
       </c>
       <c r="W9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">IF(OR(W$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Colombia</v>
       </c>
       <c r="X9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">IF(OR(X$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -12755,47 +12755,47 @@
       <c r="B10" s="214"/>
       <c r="C10" s="224" t="str">
         <f ca="1">IF(ClasificaciónPorra!D5=0,"",ClasificaciónPorra!D5)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Leiner</v>
       </c>
       <c r="D10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="226">
         <f t="shared" ref="E10" ca="1" si="2">+IF(D10="","",IF(D10&gt;F10,1,IF(D10=F10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="225" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
-      </c>
-      <c r="H10" s="226">
+        <v>1</v>
+      </c>
+      <c r="H10" s="226" t="str">
         <f t="shared" ref="H10" ca="1" si="3">+IF(G10="","",IF(G10&gt;I10,1,IF(G10=I10,"X",2)))</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I10" s="228" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K10" s="226">
         <f t="shared" ref="K10" ca="1" si="4">+IF(J10="","",IF(J10&gt;L10,1,IF(J10=L10,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="226">
         <f t="shared" ref="N10" ca="1" si="5">+IF(M10="","",IF(M10&gt;O10,1,IF(M10=O10,"X",2)))</f>
@@ -12803,13 +12803,13 @@
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P10" s="123"/>
       <c r="R10" s="214"/>
       <c r="S10" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>Moises</v>
       </c>
       <c r="T10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">IF(OR(T$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12825,7 +12825,7 @@
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="X10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">IF(OR(X$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -12851,19 +12851,19 @@
       <c r="B11" s="214"/>
       <c r="C11" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v>Leiner</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="231">
+        <v>1</v>
+      </c>
+      <c r="E11" s="231" t="str">
         <f t="shared" ref="E11:E29" ca="1" si="6">+IF(D11="","",IF(D11&gt;F11,1,IF(D11=F11,"X",2)))</f>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="F11" s="230" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -12875,19 +12875,19 @@
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12905,7 +12905,7 @@
       <c r="R11" s="214"/>
       <c r="S11" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">IF(OR(T$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12913,7 +12913,7 @@
       </c>
       <c r="U11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(OR(U$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(OR(V$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
@@ -12947,43 +12947,43 @@
       <c r="B12" s="214"/>
       <c r="C12" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>Moises</v>
+        <v>YUTA</v>
       </c>
       <c r="D12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="230" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="K12" s="231">
+      <c r="K12" s="231" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="L12" s="230" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12995,13 +12995,13 @@
       </c>
       <c r="O12" s="233" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P12" s="123"/>
       <c r="R12" s="214"/>
       <c r="S12" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">IF(OR(T$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13009,7 +13009,7 @@
       </c>
       <c r="U12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">IF(OR(U$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">IF(OR(V$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
@@ -13043,43 +13043,43 @@
       <c r="B13" s="214"/>
       <c r="C13" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="D13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="230" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="231">
+        <v>2</v>
+      </c>
+      <c r="H13" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I13" s="233" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="230" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -13097,7 +13097,7 @@
       <c r="R13" s="214"/>
       <c r="S13" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="T13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">IF(OR(T$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13139,23 +13139,23 @@
       <c r="B14" s="214"/>
       <c r="C14" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>Moises</v>
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="E14" s="231">
+      <c r="E14" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="F14" s="230" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -13167,19 +13167,19 @@
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K14" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="230" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13187,13 +13187,13 @@
       </c>
       <c r="O14" s="233" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="123"/>
       <c r="R14" s="214"/>
       <c r="S14" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D13=0,"",ClasificaciónPorra!D13)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="T14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">IF(OR(T$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13235,27 +13235,27 @@
       <c r="B15" s="214"/>
       <c r="C15" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
-      </c>
-      <c r="H15" s="231">
+        <v>0</v>
+      </c>
+      <c r="H15" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -13263,19 +13263,19 @@
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="230" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P15" s="123"/>
       <c r="R15" s="214"/>
@@ -13331,19 +13331,19 @@
       <c r="B16" s="214"/>
       <c r="C16" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Cazaputas69</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="230" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13355,23 +13355,23 @@
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="230" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13427,27 +13427,27 @@
       <c r="B17" s="214"/>
       <c r="C17" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D12=0,"",ClasificaciónPorra!D12)</f>
-        <v>Carlos Hurtado</v>
+        <v>Cazaputas69</v>
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>4</v>
-      </c>
-      <c r="H17" s="231">
+        <v>2</v>
+      </c>
+      <c r="H17" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I17" s="233" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -13455,23 +13455,23 @@
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="230" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="231">
+        <f t="shared" ca="1" si="9"/>
         <v>2</v>
-      </c>
-      <c r="N17" s="231" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>X</v>
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13523,31 +13523,31 @@
       <c r="B18" s="214"/>
       <c r="C18" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D13=0,"",ClasificaciónPorra!D13)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Carlos Hurtado</v>
       </c>
       <c r="D18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="230" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13555,11 +13555,11 @@
       </c>
       <c r="K18" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="230" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -19136,29 +19136,29 @@
         <f t="shared" ref="AZ3" ca="1" si="14">IF(OR(AX3="",AY3=""),"",IF(AX3&gt;AY3,1,IF(AX3=AY3,"x",2)))</f>
         <v>2</v>
       </c>
-      <c r="BA3" s="191" t="str">
+      <c r="BA3" s="191">
         <f ca="1">VLOOKUP(BA2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BB3" s="191" t="str">
+        <v>2</v>
+      </c>
+      <c r="BB3" s="191">
         <f ca="1">VLOOKUP(BA2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="BC3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="191">
         <f t="shared" ref="BC3" ca="1" si="15">IF(OR(BA3="",BB3=""),"",IF(BA3&gt;BB3,1,IF(BA3=BB3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="BD3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="BD3" s="191">
         <f ca="1">VLOOKUP(BD2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BE3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="191">
         <f ca="1">VLOOKUP(BD2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="BF3" s="191" t="str">
         <f t="shared" ref="BF3" ca="1" si="16">IF(OR(BD3="",BE3=""),"",IF(BD3&gt;BE3,1,IF(BD3=BE3,"x",2)))</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="BG3" s="191" t="str">
         <f ca="1">VLOOKUP(BG2,Aux!$F:$O,9,0)</f>
@@ -19234,7 +19234,7 @@
       </c>
       <c r="BY3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="BY3" ca="1">IF(INDIRECT(BY2&amp;"!AE9")&lt;3,"",INDIRECT(BY2&amp;"!P9"))</f>
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="BZ3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="BZ3" ca="1">IF(INDIRECT(BZ2&amp;"!AE9")&lt;3,"",INDIRECT(BZ2&amp;"!P9"))</f>
@@ -20438,7 +20438,7 @@
       </c>
       <c r="BC7">
         <f ca="1">IF($B7=0,0,IF(AND(BA$3=TotalApuestas!BA2,Resultado!BB$3=TotalApuestas!BB2),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC2,BC$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD7">
         <f ca="1">IF($B7=0,0,IF(BD$3=TotalApuestas!BD2,BD$5,0))</f>
@@ -20526,7 +20526,7 @@
       </c>
       <c r="BY7">
         <f ca="1">IF($B7=0,0,IF(BY$3=TotalApuestas!BY2,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ7">
         <f ca="1">IF($B7=0,0,IF(BZ$3=TotalApuestas!BZ2,BZ$5,0))</f>
@@ -20904,7 +20904,7 @@
       </c>
       <c r="BC8">
         <f ca="1">IF($B8=0,0,IF(AND(BA$3=TotalApuestas!BA3,Resultado!BB$3=TotalApuestas!BB3),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC3,BC$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD8">
         <f ca="1">IF($B8=0,0,IF(BD$3=TotalApuestas!BD3,BD$5,0))</f>
@@ -20916,7 +20916,7 @@
       </c>
       <c r="BF8">
         <f ca="1">IF($B8=0,0,IF(AND(BD$3=TotalApuestas!BD3,Resultado!BE$3=TotalApuestas!BE3),Resultado!BF$5+VLOOKUP(BF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BF$3=TotalApuestas!BF3,BF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG8">
         <f ca="1">IF($B8=0,0,IF(BG$3=TotalApuestas!BG3,BG$5,0))</f>
@@ -20992,7 +20992,7 @@
       </c>
       <c r="BY8">
         <f ca="1">IF($B8=0,0,IF(BY$3=TotalApuestas!BY3,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ8">
         <f ca="1">IF($B8=0,0,IF(BZ$3=TotalApuestas!BZ3,BZ$5,0))</f>
@@ -21370,7 +21370,7 @@
       </c>
       <c r="BC9">
         <f ca="1">IF($B9=0,0,IF(AND(BA$3=TotalApuestas!BA4,Resultado!BB$3=TotalApuestas!BB4),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC4,BC$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD9">
         <f ca="1">IF($B9=0,0,IF(BD$3=TotalApuestas!BD4,BD$5,0))</f>
@@ -21382,7 +21382,7 @@
       </c>
       <c r="BF9">
         <f ca="1">IF($B9=0,0,IF(AND(BD$3=TotalApuestas!BD4,Resultado!BE$3=TotalApuestas!BE4),Resultado!BF$5+VLOOKUP(BF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BF$3=TotalApuestas!BF4,BF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG9">
         <f ca="1">IF($B9=0,0,IF(BG$3=TotalApuestas!BG4,BG$5,0))</f>
@@ -21458,7 +21458,7 @@
       </c>
       <c r="BY9">
         <f ca="1">IF($B9=0,0,IF(BY$3=TotalApuestas!BY4,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ9">
         <f ca="1">IF($B9=0,0,IF(BZ$3=TotalApuestas!BZ4,BZ$5,0))</f>
@@ -21836,7 +21836,7 @@
       </c>
       <c r="BC10">
         <f ca="1">IF($B10=0,0,IF(AND(BA$3=TotalApuestas!BA5,Resultado!BB$3=TotalApuestas!BB5),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC5,BC$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD10">
         <f ca="1">IF($B10=0,0,IF(BD$3=TotalApuestas!BD5,BD$5,0))</f>
@@ -21924,7 +21924,7 @@
       </c>
       <c r="BY10">
         <f ca="1">IF($B10=0,0,IF(BY$3=TotalApuestas!BY5,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ10">
         <f ca="1">IF($B10=0,0,IF(BZ$3=TotalApuestas!BZ5,BZ$5,0))</f>
@@ -22302,7 +22302,7 @@
       </c>
       <c r="BC11">
         <f ca="1">IF($B11=0,0,IF(AND(BA$3=TotalApuestas!BA6,Resultado!BB$3=TotalApuestas!BB6),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC6,BC$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BD11">
         <f ca="1">IF($B11=0,0,IF(BD$3=TotalApuestas!BD6,BD$5,0))</f>
@@ -22390,7 +22390,7 @@
       </c>
       <c r="BY11">
         <f ca="1">IF($B11=0,0,IF(BY$3=TotalApuestas!BY6,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ11">
         <f ca="1">IF($B11=0,0,IF(BZ$3=TotalApuestas!BZ6,BZ$5,0))</f>
@@ -22768,7 +22768,7 @@
       </c>
       <c r="BC12">
         <f ca="1">IF($B12=0,0,IF(AND(BA$3=TotalApuestas!BA7,Resultado!BB$3=TotalApuestas!BB7),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC7,BC$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BD12">
         <f ca="1">IF($B12=0,0,IF(BD$3=TotalApuestas!BD7,BD$5,0))</f>
@@ -22780,7 +22780,7 @@
       </c>
       <c r="BF12">
         <f ca="1">IF($B12=0,0,IF(AND(BD$3=TotalApuestas!BD7,Resultado!BE$3=TotalApuestas!BE7),Resultado!BF$5+VLOOKUP(BF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BF$3=TotalApuestas!BF7,BF$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BG12">
         <f ca="1">IF($B12=0,0,IF(BG$3=TotalApuestas!BG7,BG$5,0))</f>
@@ -22856,7 +22856,7 @@
       </c>
       <c r="BY12">
         <f ca="1">IF($B12=0,0,IF(BY$3=TotalApuestas!BY7,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ12">
         <f ca="1">IF($B12=0,0,IF(BZ$3=TotalApuestas!BZ7,BZ$5,0))</f>
@@ -23234,7 +23234,7 @@
       </c>
       <c r="BC13">
         <f ca="1">IF($B13=0,0,IF(AND(BA$3=TotalApuestas!BA8,Resultado!BB$3=TotalApuestas!BB8),Resultado!BC$5+VLOOKUP(BC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BC$3=TotalApuestas!BC8,BC$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD13">
         <f ca="1">IF($B13=0,0,IF(BD$3=TotalApuestas!BD8,BD$5,0))</f>
@@ -23246,7 +23246,7 @@
       </c>
       <c r="BF13">
         <f ca="1">IF($B13=0,0,IF(AND(BD$3=TotalApuestas!BD8,Resultado!BE$3=TotalApuestas!BE8),Resultado!BF$5+VLOOKUP(BF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BF$3=TotalApuestas!BF8,BF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG13">
         <f ca="1">IF($B13=0,0,IF(BG$3=TotalApuestas!BG8,BG$5,0))</f>
@@ -23322,7 +23322,7 @@
       </c>
       <c r="BY13">
         <f ca="1">IF($B13=0,0,IF(BY$3=TotalApuestas!BY8,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ13">
         <f ca="1">IF($B13=0,0,IF(BZ$3=TotalApuestas!BZ8,BZ$5,0))</f>
@@ -23788,7 +23788,7 @@
       </c>
       <c r="BY14">
         <f ca="1">IF($B14=0,0,IF(BY$3=TotalApuestas!BY9,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ14">
         <f ca="1">IF($B14=0,0,IF(BZ$3=TotalApuestas!BZ9,BZ$5,0))</f>
@@ -24254,7 +24254,7 @@
       </c>
       <c r="BY15">
         <f ca="1">IF($B15=0,0,IF(BY$3=TotalApuestas!BY10,BY$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BZ15">
         <f ca="1">IF($B15=0,0,IF(BZ$3=TotalApuestas!BZ10,BZ$5,0))</f>
@@ -41425,29 +41425,29 @@
         <f ca="1">+Resultado!AZ3</f>
         <v>2</v>
       </c>
-      <c r="BA1" s="84" t="str">
+      <c r="BA1" s="84">
         <f ca="1">+Resultado!BA3</f>
-        <v/>
-      </c>
-      <c r="BB1" s="84" t="str">
+        <v>2</v>
+      </c>
+      <c r="BB1" s="84">
         <f ca="1">+Resultado!BB3</f>
-        <v/>
-      </c>
-      <c r="BC1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="BC1" s="84">
         <f ca="1">+Resultado!BC3</f>
-        <v/>
-      </c>
-      <c r="BD1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="BD1" s="84">
         <f ca="1">+Resultado!BD3</f>
-        <v/>
-      </c>
-      <c r="BE1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="BE1" s="84">
         <f ca="1">+Resultado!BE3</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="BF1" s="84" t="str">
         <f ca="1">+Resultado!BF3</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="BG1" s="84" t="str">
         <f ca="1">+Resultado!BG3</f>
@@ -41523,7 +41523,7 @@
       </c>
       <c r="BY1" s="84" t="str">
         <f ca="1">+Resultado!BY3</f>
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="BZ1" s="84" t="str">
         <f ca="1">+Resultado!BZ3</f>
@@ -41705,7 +41705,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -41976,7 +41976,7 @@
       <c r="AQ5" s="53"/>
       <c r="AR5" s="245">
         <f>+VLOOKUP(AR7,$AD$9:$AF$15,3,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
@@ -41984,11 +41984,11 @@
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU5" s="245">
         <f>+VLOOKUP(AU7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:47" s="54" customFormat="1" ht="22.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -42247,11 +42247,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -42263,7 +42263,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -42271,7 +42271,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -42285,15 +42285,15 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AG9" s="53" cm="1">
         <f t="array" ref="AG9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH9" s="53" cm="1">
         <f t="array" ref="AH9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -42305,7 +42305,7 @@
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
@@ -42317,11 +42317,11 @@
       </c>
       <c r="AM9" s="252">
         <f>+AJ9-AK9</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN9" s="53">
         <f>+_xlfn.RANK.EQ(AF9,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM9,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ9,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL9,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.1130089999999999</v>
+        <v>1.1110089999999999</v>
       </c>
       <c r="AO9" s="53">
         <f>+_xlfn.RANK.EQ(AN9,$AN$9:$AN$15,1)</f>
@@ -42341,7 +42341,7 @@
 (SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AS$7)))*100
 +SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD9)*($J$9:$J$22)*($G$9:$G$22=AS$7))
 -SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD9)*($H$9:$H$22)*($G$9:$G$22=AS$7))</f>
-        <v>100</v>
+        <v>302</v>
       </c>
       <c r="AT9" s="53" cm="1">
         <f t="array" ref="AT9">(SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AT$7)))*300+
@@ -42463,7 +42463,7 @@
       <c r="R11" s="158"/>
       <c r="S11" s="159">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,4,0)</f>
@@ -42471,7 +42471,7 @@
       </c>
       <c r="U11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,6,0)</f>
@@ -42501,7 +42501,7 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11:AE15" si="0">+AG11+AH11+AI11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11:AF15" si="1">+AG11*3+AH11</f>
@@ -42517,7 +42517,7 @@
       </c>
       <c r="AI11" s="53" cm="1">
         <f t="array" ref="AI11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11" s="53" cm="1">
         <f t="array" ref="AJ11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)+($K$9:$K$22=$AD11)*($J$9:$J$22))</f>
@@ -42525,23 +42525,23 @@
       </c>
       <c r="AK11" s="53" cm="1">
         <f t="array" ref="AK11">SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL11" s="252">
         <f>+SUMIFS($AR11:$AU11,$AR$5:$AU$5,AF11)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM11" s="252">
         <f>+AJ11-AK11</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>3.2310110000000001</v>
+        <v>4.4310110000000007</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11:AO15" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AP11" s="53"/>
       <c r="AQ11" s="53"/>
@@ -42550,7 +42550,7 @@
 (SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AR$7)))*100
 +SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD11)*($J$9:$J$22)*($G$9:$G$22=AR$7))
 -SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)*($K$9:$K$22=AR$7)+($K$9:$K$22=$AD11)*($H$9:$H$22)*($G$9:$G$22=AR$7))</f>
-        <v>100</v>
+        <v>-2</v>
       </c>
       <c r="AS11" s="53" cm="1">
         <f t="array" ref="AS11">(SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AS$7)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AS$7)))*300+
@@ -42670,16 +42670,16 @@
       <c r="O13"/>
       <c r="P13" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(3,$AO$9:$AO$15,0))</f>
-        <v>Perú</v>
-      </c>
-      <c r="Q13" s="157" t="e" vm="3">
+        <v>Chile</v>
+      </c>
+      <c r="Q13" s="157" t="e" vm="4">
         <f>IFERROR(VLOOKUP(P13,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
       <c r="R13" s="158"/>
       <c r="S13" s="159">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,3,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,4,0)</f>
@@ -42687,7 +42687,7 @@
       </c>
       <c r="U13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,6,0)</f>
@@ -42717,11 +42717,11 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG13" s="53" cm="1">
         <f t="array" ref="AG13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -42729,7 +42729,7 @@
       </c>
       <c r="AH13" s="53" cm="1">
         <f t="array" ref="AH13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI13" s="53" cm="1">
         <f t="array" ref="AI13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -42745,7 +42745,7 @@
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
@@ -42757,7 +42757,7 @@
       </c>
       <c r="AO13" s="53">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AP13" s="53"/>
       <c r="AQ13" s="53"/>
@@ -42886,9 +42886,9 @@
       <c r="O15"/>
       <c r="P15" s="156" t="str">
         <f>+INDEX($AD$9:$AD$16,MATCH(4,$AO$9:$AO$15,0))</f>
-        <v>Chile</v>
-      </c>
-      <c r="Q15" s="157" t="e" vm="4">
+        <v>Perú</v>
+      </c>
+      <c r="Q15" s="157" t="e" vm="3">
         <f>IFERROR(VLOOKUP(P15,Aux!A:C,3,0),"")</f>
         <v>#VALUE!</v>
       </c>
@@ -42907,7 +42907,7 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
@@ -42915,11 +42915,11 @@
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -42933,11 +42933,11 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG15" s="53" cm="1">
         <f t="array" ref="AG15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -42945,7 +42945,7 @@
       </c>
       <c r="AH15" s="53" cm="1">
         <f t="array" ref="AH15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15" s="53" cm="1">
         <f t="array" ref="AI15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -42969,7 +42969,7 @@
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>2.2230150000000002</v>
+        <v>2.221015</v>
       </c>
       <c r="AO15" s="53">
         <f t="shared" si="2"/>
@@ -43077,11 +43077,15 @@
         <f>+VLOOKUP(B17,Aux!F:S,5,0)</f>
         <v>Argentina</v>
       </c>
-      <c r="H17" s="258"/>
+      <c r="H17" s="258">
+        <v>2</v>
+      </c>
       <c r="I17" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="258"/>
+      <c r="J17" s="258">
+        <v>0</v>
+      </c>
       <c r="K17" s="38" t="str">
         <f>+VLOOKUP(B17,Aux!F:S,6,0)</f>
         <v>Perú</v>
@@ -43176,11 +43180,15 @@
         <f>+VLOOKUP(B19,Aux!F:S,5,0)</f>
         <v>Canadá</v>
       </c>
-      <c r="H19" s="258"/>
+      <c r="H19" s="258">
+        <v>0</v>
+      </c>
       <c r="I19" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="258"/>
+      <c r="J19" s="258">
+        <v>0</v>
+      </c>
       <c r="K19" s="38" t="str">
         <f>+VLOOKUP(B19,Aux!F:S,6,0)</f>
         <v>Chile</v>
@@ -50719,13 +50727,13 @@
       <c r="M18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N18" s="68" t="str">
+      <c r="N18" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O18" s="68" t="str">
+        <v>2</v>
+      </c>
+      <c r="O18" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="2"/>
@@ -50767,13 +50775,13 @@
       <c r="M19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N19" s="68" t="str">
+      <c r="N19" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O19" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O19" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="2"/>

</xml_diff>

<commit_message>
fin jornada 3 B
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE389E2-5430-4DC8-8DF8-E1D462DDE37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5B87A-00CC-4F95-94AA-CC2B662EAAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9204,7 +9204,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="F5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:F4),0))</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:G4),0))</f>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>110.011</v>
+        <v>130.011</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="T5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>80.004999999999995</v>
+        <v>85.004999999999995</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
@@ -10023,7 +10023,7 @@
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>100.012</v>
+        <v>120.012</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10063,7 +10063,7 @@
       </c>
       <c r="T6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="U6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>85.006</v>
+        <v>90.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10113,7 +10113,7 @@
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
@@ -10125,7 +10125,7 @@
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>100.009</v>
+        <v>110.009</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10153,7 +10153,7 @@
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" s="126" t="str">
         <f>Resultado!B9</f>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="T7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>100.00700000000001</v>
+        <v>105.00700000000001</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10207,15 +10207,15 @@
       </c>
       <c r="D8" s="152" t="str">
         <f ca="1">+VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:D7),0)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E8" s="201">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:E7),0))</f>
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
@@ -10223,11 +10223,11 @@
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>100.00700000000001</v>
+        <v>105.008</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="T8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>85.007999999999996</v>
+        <v>105.008</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10309,11 +10309,11 @@
       </c>
       <c r="D9" s="153" t="str">
         <f ca="1">+VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:D8),0)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
@@ -10325,11 +10325,11 @@
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>90.013000000000005</v>
+        <v>105.00700000000001</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10369,7 +10369,7 @@
       </c>
       <c r="T9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="U9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10381,7 +10381,7 @@
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>100.009</v>
+        <v>110.009</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10411,27 +10411,27 @@
       </c>
       <c r="D10" s="151" t="str">
         <f ca="1">+VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:D9),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Moises</v>
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>90.01</v>
+        <v>95.013000000000005</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10471,7 +10471,7 @@
       </c>
       <c r="T10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>90.01</v>
+        <v>95.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10513,27 +10513,27 @@
       </c>
       <c r="D11" s="151" t="str">
         <f ca="1">+VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:D10),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>85.007999999999996</v>
+        <v>95.01</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10573,7 +10573,7 @@
       </c>
       <c r="T11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="U11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>110.011</v>
+        <v>130.011</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
@@ -10635,7 +10635,7 @@
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>85.006</v>
+        <v>90.006</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10675,7 +10675,7 @@
       </c>
       <c r="T12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="U12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>100.012</v>
+        <v>120.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10725,7 +10725,7 @@
       </c>
       <c r="F13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:F12),0))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:G12),0))</f>
@@ -10737,7 +10737,7 @@
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>80.004999999999995</v>
+        <v>85.004999999999995</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10765,7 +10765,7 @@
       </c>
       <c r="Q13" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="126" t="str">
         <f>Resultado!B15</f>
@@ -10777,7 +10777,7 @@
       </c>
       <c r="T13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>90.013000000000005</v>
+        <v>95.013000000000005</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12261,33 +12261,33 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="173">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" s="207"/>
       <c r="D1" s="207">
         <f>+A1</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="207"/>
       <c r="G1" s="207">
         <f>+D1+1</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H1" s="207"/>
       <c r="I1" s="207"/>
       <c r="J1" s="207">
         <f t="shared" ref="J1" si="0">+G1+1</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207">
         <f t="shared" ref="M1" si="1">+J1+1</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="S1" s="176" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="T1" s="208"/>
       <c r="U1" s="208"/>
@@ -12400,25 +12400,25 @@
       <c r="C5" s="146"/>
       <c r="D5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(D1,Aux!$F:$O,8,0)</f>
-        <v>Grupo A</v>
+        <v>Grupo C</v>
       </c>
       <c r="E5" s="297"/>
       <c r="F5" s="298"/>
       <c r="G5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(G1,Aux!$F:$O,8,0)</f>
-        <v>Grupo A</v>
+        <v>Grupo D</v>
       </c>
       <c r="H5" s="297"/>
       <c r="I5" s="298"/>
       <c r="J5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(J1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo D</v>
       </c>
       <c r="K5" s="297"/>
       <c r="L5" s="298"/>
       <c r="M5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(M1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo Cuartos</v>
       </c>
       <c r="N5" s="297"/>
       <c r="O5" s="298"/>
@@ -12426,22 +12426,30 @@
       <c r="R5" s="214"/>
       <c r="S5" s="215"/>
       <c r="T5" s="216" t="str" cm="1">
-        <f t="array" ref="T5:W5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
-        <v>CampeonG1</v>
+        <f t="array" ref="T5:AA5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
+        <v>Cuartos1</v>
       </c>
       <c r="U5" s="216" t="str">
-        <v>CampeonG2</v>
+        <v>Cuartos2</v>
       </c>
       <c r="V5" s="216" t="str">
-        <v>CampeonG3</v>
+        <v>Cuartos3</v>
       </c>
       <c r="W5" s="216" t="str">
-        <v>CampeonG4</v>
-      </c>
-      <c r="X5" s="216"/>
-      <c r="Y5" s="216"/>
-      <c r="Z5" s="216"/>
-      <c r="AA5" s="216"/>
+        <v>Cuartos4</v>
+      </c>
+      <c r="X5" s="216" t="str">
+        <v>Cuartos5</v>
+      </c>
+      <c r="Y5" s="216" t="str">
+        <v>Cuartos6</v>
+      </c>
+      <c r="Z5" s="216" t="str">
+        <v>Cuartos7</v>
+      </c>
+      <c r="AA5" s="216" t="str">
+        <v>Cuartos8</v>
+      </c>
       <c r="AB5" s="123"/>
       <c r="AD5" s="207" t="s">
         <v>94</v>
@@ -12455,51 +12463,51 @@
       <c r="C6" s="146"/>
       <c r="D6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,5,0)</f>
-        <v>Argentina</v>
+        <v>Bolivia</v>
       </c>
       <c r="E6" s="217">
         <f>VLOOKUP(D1,Aux!$F:$O,3,0)</f>
-        <v>45472.833333333336</v>
+        <v>45474.875</v>
       </c>
       <c r="F6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,6,0)</f>
-        <v>Perú</v>
+        <v>Panamá</v>
       </c>
       <c r="G6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,5,0)</f>
-        <v>Canadá</v>
+        <v>Brasil</v>
       </c>
       <c r="H6" s="217">
         <f>VLOOKUP(G1,Aux!$F:$O,3,0)</f>
-        <v>45472.833333333336</v>
+        <v>45475.75</v>
       </c>
       <c r="I6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,6,0)</f>
-        <v>Chile</v>
+        <v>Colombia</v>
       </c>
       <c r="J6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,5,0)</f>
-        <v>México</v>
+        <v>Costa Rica</v>
       </c>
       <c r="K6" s="217">
         <f>VLOOKUP(J1,Aux!$F:$O,3,0)</f>
-        <v>45473.708333333336</v>
+        <v>45475.833333333336</v>
       </c>
       <c r="L6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,6,0)</f>
-        <v>Ecuador</v>
+        <v>Paraguay</v>
       </c>
       <c r="M6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,5,0)</f>
-        <v>Jamaica</v>
+        <v>1A</v>
       </c>
       <c r="N6" s="217">
         <f>VLOOKUP(M1,Aux!$F:$O,3,0)</f>
-        <v>45473.791666666664</v>
+        <v>45477.833333333336</v>
       </c>
       <c r="O6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,6,0)</f>
-        <v>Venezuela</v>
+        <v>2B</v>
       </c>
       <c r="P6" s="123"/>
       <c r="R6" s="214"/>
@@ -12513,31 +12521,31 @@
       </c>
       <c r="U6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">IF(OR(U$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">IF(OR(V$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Venezuela</v>
       </c>
       <c r="W6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">IF(OR(W$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Chile</v>
       </c>
       <c r="X6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">IF(OR(X$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="Y6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y6" ca="1">IF(OR(Y$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z6" ca="1">IF(OR(Z$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA6" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA6" ca="1">IF(OR(AA$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="AB6" s="123"/>
       <c r="AD6"/>
@@ -12549,25 +12557,25 @@
       <c r="D7" s="299"/>
       <c r="E7" s="220">
         <f>+E6</f>
-        <v>45472.833333333336</v>
+        <v>45474.875</v>
       </c>
       <c r="F7" s="299"/>
       <c r="G7" s="299"/>
       <c r="H7" s="220">
         <f>+H6</f>
-        <v>45472.833333333336</v>
+        <v>45475.75</v>
       </c>
       <c r="I7" s="299"/>
       <c r="J7" s="299"/>
       <c r="K7" s="220">
         <f>+K6</f>
-        <v>45473.708333333336</v>
+        <v>45475.833333333336</v>
       </c>
       <c r="L7" s="299"/>
       <c r="M7" s="299"/>
       <c r="N7" s="220">
         <f>+N6</f>
-        <v>45473.791666666664</v>
+        <v>45477.833333333336</v>
       </c>
       <c r="O7" s="299"/>
       <c r="P7" s="123"/>
@@ -12582,31 +12590,31 @@
       </c>
       <c r="U7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U7" ca="1">IF(OR(U$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V7" ca="1">IF(OR(V$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Venezuela</v>
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Canadá</v>
       </c>
       <c r="X7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">IF(OR(X$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y7" ca="1">IF(OR(Y$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z7" ca="1">IF(OR(Z$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA7" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA7" ca="1">IF(OR(AA$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB7" s="123"/>
       <c r="AD7"/>
@@ -12617,29 +12625,29 @@
       <c r="C8" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="221">
+      <c r="D8" s="221" t="str">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,9,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E8" s="222">
+        <v/>
+      </c>
+      <c r="E8" s="222" t="str">
         <f ca="1">+IF(D8="","",IF(D8&gt;F8,1,IF(D8=F8,"X",2)))</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="223">
+        <v/>
+      </c>
+      <c r="F8" s="223" t="str">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="221">
+        <v/>
+      </c>
+      <c r="G8" s="221" t="str">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H8" s="222" t="str">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v>X</v>
-      </c>
-      <c r="I8" s="223">
+        <v/>
+      </c>
+      <c r="I8" s="223" t="str">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
@@ -12677,31 +12685,31 @@
       </c>
       <c r="U8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(OR(U$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">IF(OR(V$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">IF(OR(W$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Chile</v>
       </c>
       <c r="X8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">IF(OR(X$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y8" ca="1">IF(OR(Y$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z8" ca="1">IF(OR(Z$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA8" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA8" ca="1">IF(OR(AA$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB8" s="123"/>
       <c r="AD8"/>
@@ -12713,7 +12721,7 @@
       <c r="R9" s="214"/>
       <c r="S9" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">IF(OR(T$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12725,27 +12733,27 @@
       </c>
       <c r="V9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V9" ca="1">IF(OR(V$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Venezuela</v>
       </c>
       <c r="W9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">IF(OR(W$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Canadá</v>
       </c>
       <c r="X9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">IF(OR(X$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y9" ca="1">IF(OR(Y$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z9" ca="1">IF(OR(Z$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA9" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA9" ca="1">IF(OR(AA$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB9" s="123"/>
       <c r="AD9"/>
@@ -12759,7 +12767,7 @@
       </c>
       <c r="D10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="226">
         <f t="shared" ref="E10" ca="1" si="2">+IF(D10="","",IF(D10&gt;F10,1,IF(D10=F10,"X",2)))</f>
@@ -12791,15 +12799,15 @@
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="226">
         <f t="shared" ref="N10" ca="1" si="5">+IF(M10="","",IF(M10&gt;O10,1,IF(M10=O10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -12809,7 +12817,7 @@
       <c r="R10" s="214"/>
       <c r="S10" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="T10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">IF(OR(T$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12817,31 +12825,31 @@
       </c>
       <c r="U10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(OR(U$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(OR(V$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Chile</v>
       </c>
       <c r="X10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">IF(OR(X$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="Y10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y10" ca="1">IF(OR(Y$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z10" ca="1">IF(OR(Z$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA10" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA10" ca="1">IF(OR(AA$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="AB10" s="123"/>
       <c r="AD10"/>
@@ -12855,11 +12863,11 @@
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="E11" s="231">
         <f t="shared" ref="E11:E29" ca="1" si="6">+IF(D11="","",IF(D11&gt;F11,1,IF(D11=F11,"X",2)))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="F11" s="230" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
@@ -12867,15 +12875,15 @@
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
-      </c>
-      <c r="H11" s="231">
+        <v>1</v>
+      </c>
+      <c r="H11" s="231" t="str">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -12887,25 +12895,25 @@
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="231">
         <f t="shared" ref="N11:N29" ca="1" si="9">+IF(M11="","",IF(M11&gt;O11,1,IF(M11=O11,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O11" s="233" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" s="123"/>
       <c r="R11" s="214"/>
       <c r="S11" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Moises</v>
       </c>
       <c r="T11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">IF(OR(T$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12913,31 +12921,31 @@
       </c>
       <c r="U11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(OR(U$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(OR(V$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">IF(OR(W$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Canadá</v>
       </c>
       <c r="X11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">IF(OR(X$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">IF(OR(Y$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">IF(OR(Z$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA11" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">IF(OR(AA$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB11" s="123"/>
       <c r="AD11"/>
@@ -12959,19 +12967,19 @@
       </c>
       <c r="F12" s="230" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -12987,21 +12995,21 @@
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O12" s="233" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="123"/>
       <c r="R12" s="214"/>
       <c r="S12" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">IF(OR(T$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13013,27 +13021,27 @@
       </c>
       <c r="V12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">IF(OR(V$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W12" ca="1">IF(OR(W$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Canadá</v>
       </c>
       <c r="X12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">IF(OR(X$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y12" ca="1">IF(OR(Y$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z12" ca="1">IF(OR(Z$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA12" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA12" ca="1">IF(OR(AA$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB12" s="123"/>
       <c r="AD12"/>
@@ -13043,15 +13051,15 @@
       <c r="B13" s="214"/>
       <c r="C13" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="231">
+        <v>0</v>
+      </c>
+      <c r="E13" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="F13" s="230" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
@@ -13073,21 +13081,21 @@
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
         <v>0</v>
       </c>
-      <c r="K13" s="231">
+      <c r="K13" s="231" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="L13" s="230" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="231">
+        <v>2</v>
+      </c>
+      <c r="N13" s="231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="O13" s="233" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13105,31 +13113,31 @@
       </c>
       <c r="U13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U13" ca="1">IF(OR(U$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V13" ca="1">IF(OR(V$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">IF(OR(W$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Chile</v>
       </c>
       <c r="X13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">IF(OR(X$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y13" ca="1">IF(OR(Y$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z13" ca="1">IF(OR(Z$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA13" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA13" ca="1">IF(OR(AA$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB13" s="123"/>
       <c r="AD13"/>
@@ -13139,15 +13147,15 @@
       <c r="B14" s="214"/>
       <c r="C14" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="E14" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="F14" s="230" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
@@ -13159,35 +13167,35 @@
       </c>
       <c r="H14" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="233" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="231">
+        <v>1</v>
+      </c>
+      <c r="K14" s="231" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="L14" s="230" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="233" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="123"/>
       <c r="R14" s="214"/>
@@ -13201,31 +13209,31 @@
       </c>
       <c r="U14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">IF(OR(U$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">IF(OR(V$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Ecuador</v>
       </c>
       <c r="W14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">IF(OR(W$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Chile</v>
       </c>
       <c r="X14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X14" ca="1">IF(OR(X$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="Y14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y14" ca="1">IF(OR(Y$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v/>
+        <v>Estados Unidos</v>
       </c>
       <c r="Z14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z14" ca="1">IF(OR(Z$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="AA14" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA14" ca="1">IF(OR(AA$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="AB14" s="123"/>
       <c r="AD14"/>
@@ -13235,15 +13243,15 @@
       <c r="B15" s="214"/>
       <c r="C15" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>Moises</v>
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
-      </c>
-      <c r="E15" s="231">
+        <v>0</v>
+      </c>
+      <c r="E15" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
@@ -13251,15 +13259,15 @@
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="231" t="str">
+        <v>3</v>
+      </c>
+      <c r="H15" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13271,19 +13279,19 @@
       </c>
       <c r="L15" s="230" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="123"/>
       <c r="R15" s="214"/>
@@ -13331,31 +13339,31 @@
       <c r="B16" s="214"/>
       <c r="C16" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="E16" s="231">
+      <c r="E16" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="F16" s="230" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
         <v>2</v>
       </c>
-      <c r="H16" s="231">
+      <c r="H16" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13371,15 +13379,15 @@
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O16" s="233" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P16" s="123"/>
       <c r="R16" s="214"/>
@@ -13431,7 +13439,7 @@
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13439,7 +13447,7 @@
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13455,27 +13463,27 @@
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="231">
+        <v>1</v>
+      </c>
+      <c r="K17" s="231" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="L17" s="230" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" s="123"/>
       <c r="R17" s="214"/>
@@ -13527,7 +13535,7 @@
       </c>
       <c r="D18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13535,15 +13543,15 @@
       </c>
       <c r="F18" s="230" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H18" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -13551,27 +13559,27 @@
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
-      </c>
-      <c r="K18" s="231">
+        <v>0</v>
+      </c>
+      <c r="K18" s="231" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="L18" s="230" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O18" s="233" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P18" s="123"/>
       <c r="R18" s="214"/>
@@ -19160,29 +19168,29 @@
         <f t="shared" ref="BF3" ca="1" si="16">IF(OR(BD3="",BE3=""),"",IF(BD3&gt;BE3,1,IF(BD3=BE3,"x",2)))</f>
         <v>x</v>
       </c>
-      <c r="BG3" s="191" t="str">
+      <c r="BG3" s="191">
         <f ca="1">VLOOKUP(BG2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BH3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="191">
         <f ca="1">VLOOKUP(BG2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="BI3" s="191" t="str">
         <f t="shared" ref="BI3" ca="1" si="17">IF(OR(BG3="",BH3=""),"",IF(BG3&gt;BH3,1,IF(BG3=BH3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="BJ3" s="191" t="str">
+        <v>x</v>
+      </c>
+      <c r="BJ3" s="191">
         <f ca="1">VLOOKUP(BJ2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BK3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="191">
         <f ca="1">VLOOKUP(BJ2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="BL3" s="191" t="str">
+        <v>3</v>
+      </c>
+      <c r="BL3" s="191">
         <f t="shared" ref="BL3" ca="1" si="18">IF(OR(BJ3="",BK3=""),"",IF(BJ3&gt;BK3,1,IF(BJ3=BK3,"x",2)))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="BM3" s="191" t="str">
         <f ca="1">VLOOKUP(BM2,Aux!$F:$O,9,0)</f>
@@ -19238,7 +19246,7 @@
       </c>
       <c r="BZ3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="BZ3" ca="1">IF(INDIRECT(BZ2&amp;"!AE9")&lt;3,"",INDIRECT(BZ2&amp;"!P9"))</f>
-        <v/>
+        <v>Venezuela</v>
       </c>
       <c r="CA3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="CA3" ca="1">IF(INDIRECT(CA2&amp;"!AE9")&lt;3,"",INDIRECT(CA2&amp;"!P9"))</f>
@@ -20474,7 +20482,7 @@
       </c>
       <c r="BL7">
         <f ca="1">IF($B7=0,0,IF(AND(BJ$3=TotalApuestas!BJ2,Resultado!BK$3=TotalApuestas!BK2),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL2,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM7">
         <f ca="1">IF($B7=0,0,IF(BM$3=TotalApuestas!BM2,BM$5,0))</f>
@@ -20940,7 +20948,7 @@
       </c>
       <c r="BL8">
         <f ca="1">IF($B8=0,0,IF(AND(BJ$3=TotalApuestas!BJ3,Resultado!BK$3=TotalApuestas!BK3),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL3,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM8">
         <f ca="1">IF($B8=0,0,IF(BM$3=TotalApuestas!BM3,BM$5,0))</f>
@@ -21406,7 +21414,7 @@
       </c>
       <c r="BL9">
         <f ca="1">IF($B9=0,0,IF(AND(BJ$3=TotalApuestas!BJ4,Resultado!BK$3=TotalApuestas!BK4),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL4,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM9">
         <f ca="1">IF($B9=0,0,IF(BM$3=TotalApuestas!BM4,BM$5,0))</f>
@@ -21872,7 +21880,7 @@
       </c>
       <c r="BL10">
         <f ca="1">IF($B10=0,0,IF(AND(BJ$3=TotalApuestas!BJ5,Resultado!BK$3=TotalApuestas!BK5),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL5,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM10">
         <f ca="1">IF($B10=0,0,IF(BM$3=TotalApuestas!BM5,BM$5,0))</f>
@@ -21928,7 +21936,7 @@
       </c>
       <c r="BZ10">
         <f ca="1">IF($B10=0,0,IF(BZ$3=TotalApuestas!BZ5,BZ$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="CA10">
         <f ca="1">IF($B10=0,0,IF(CA$3=TotalApuestas!CA5,CA$5,0))</f>
@@ -22326,7 +22334,7 @@
       </c>
       <c r="BI11">
         <f ca="1">IF($B11=0,0,IF(AND(BG$3=TotalApuestas!BG6,Resultado!BH$3=TotalApuestas!BH6),Resultado!BI$5+VLOOKUP(BI$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BI$3=TotalApuestas!BI6,BI$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BJ11">
         <f ca="1">IF($B11=0,0,IF(BJ$3=TotalApuestas!BJ6,BJ$5,0))</f>
@@ -22338,7 +22346,7 @@
       </c>
       <c r="BL11">
         <f ca="1">IF($B11=0,0,IF(AND(BJ$3=TotalApuestas!BJ6,Resultado!BK$3=TotalApuestas!BK6),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL6,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM11">
         <f ca="1">IF($B11=0,0,IF(BM$3=TotalApuestas!BM6,BM$5,0))</f>
@@ -22804,7 +22812,7 @@
       </c>
       <c r="BL12">
         <f ca="1">IF($B12=0,0,IF(AND(BJ$3=TotalApuestas!BJ7,Resultado!BK$3=TotalApuestas!BK7),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL7,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM12">
         <f ca="1">IF($B12=0,0,IF(BM$3=TotalApuestas!BM7,BM$5,0))</f>
@@ -23270,7 +23278,7 @@
       </c>
       <c r="BL13">
         <f ca="1">IF($B13=0,0,IF(AND(BJ$3=TotalApuestas!BJ8,Resultado!BK$3=TotalApuestas!BK8),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL8,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM13">
         <f ca="1">IF($B13=0,0,IF(BM$3=TotalApuestas!BM8,BM$5,0))</f>
@@ -23326,7 +23334,7 @@
       </c>
       <c r="BZ13">
         <f ca="1">IF($B13=0,0,IF(BZ$3=TotalApuestas!BZ8,BZ$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="CA13">
         <f ca="1">IF($B13=0,0,IF(CA$3=TotalApuestas!CA8,CA$5,0))</f>
@@ -23736,7 +23744,7 @@
       </c>
       <c r="BL14">
         <f ca="1">IF($B14=0,0,IF(AND(BJ$3=TotalApuestas!BJ9,Resultado!BK$3=TotalApuestas!BK9),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL9,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM14">
         <f ca="1">IF($B14=0,0,IF(BM$3=TotalApuestas!BM9,BM$5,0))</f>
@@ -23792,7 +23800,7 @@
       </c>
       <c r="BZ14">
         <f ca="1">IF($B14=0,0,IF(BZ$3=TotalApuestas!BZ9,BZ$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="CA14">
         <f ca="1">IF($B14=0,0,IF(CA$3=TotalApuestas!CA9,CA$5,0))</f>
@@ -24202,7 +24210,7 @@
       </c>
       <c r="BL15">
         <f ca="1">IF($B15=0,0,IF(AND(BJ$3=TotalApuestas!BJ10,Resultado!BK$3=TotalApuestas!BK10),Resultado!BL$5+VLOOKUP(BL$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BL$3=TotalApuestas!BL10,BL$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BM15">
         <f ca="1">IF($B15=0,0,IF(BM$3=TotalApuestas!BM10,BM$5,0))</f>
@@ -41449,29 +41457,29 @@
         <f ca="1">+Resultado!BF3</f>
         <v>x</v>
       </c>
-      <c r="BG1" s="84" t="str">
+      <c r="BG1" s="84">
         <f ca="1">+Resultado!BG3</f>
-        <v/>
-      </c>
-      <c r="BH1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="BH1" s="84">
         <f ca="1">+Resultado!BH3</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="BI1" s="84" t="str">
         <f ca="1">+Resultado!BI3</f>
-        <v/>
-      </c>
-      <c r="BJ1" s="84" t="str">
+        <v>x</v>
+      </c>
+      <c r="BJ1" s="84">
         <f ca="1">+Resultado!BJ3</f>
-        <v/>
-      </c>
-      <c r="BK1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="BK1" s="84">
         <f ca="1">+Resultado!BK3</f>
-        <v/>
-      </c>
-      <c r="BL1" s="84" t="str">
+        <v>3</v>
+      </c>
+      <c r="BL1" s="84">
         <f ca="1">+Resultado!BL3</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="BM1" s="84" t="str">
         <f ca="1">+Resultado!BM3</f>
@@ -41527,7 +41535,7 @@
       </c>
       <c r="BZ1" s="84" t="str">
         <f ca="1">+Resultado!BZ3</f>
-        <v/>
+        <v>Venezuela</v>
       </c>
       <c r="CA1" s="84" t="str">
         <f ca="1">+Resultado!CA3</f>
@@ -43321,7 +43329,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43592,15 +43600,15 @@
       <c r="AQ5" s="53"/>
       <c r="AR5" s="245">
         <f>+VLOOKUP(AR7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AU5" s="245">
         <f>+VLOOKUP(AU7,$AD$9:$AF$15,3,0)</f>
@@ -43863,11 +43871,11 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
@@ -43879,7 +43887,7 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
@@ -43887,7 +43895,7 @@
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z9" s="60"/>
       <c r="AA9" s="57"/>
@@ -43901,11 +43909,11 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG9" s="53" cm="1">
         <f t="array" ref="AG9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -43913,7 +43921,7 @@
       </c>
       <c r="AH9" s="53" cm="1">
         <f t="array" ref="AH9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" s="53" cm="1">
         <f t="array" ref="AI9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -44079,7 +44087,7 @@
       <c r="R11" s="158"/>
       <c r="S11" s="159">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,4,0)</f>
@@ -44087,7 +44095,7 @@
       </c>
       <c r="U11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,6,0)</f>
@@ -44117,11 +44125,11 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11" si="0">+AG11+AH11+AI11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11" si="1">+AG11*3+AH11</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG11" s="53" cm="1">
         <f t="array" ref="AG11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -44129,7 +44137,7 @@
       </c>
       <c r="AH11" s="53" cm="1">
         <f t="array" ref="AH11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" s="53" cm="1">
         <f t="array" ref="AI11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -44153,7 +44161,7 @@
       </c>
       <c r="AN11" s="53">
         <f>+_xlfn.RANK.EQ(AF11,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM11,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ11,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL11,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>2.2110110000000001</v>
+        <v>2.2210110000000003</v>
       </c>
       <c r="AO11" s="53">
         <f t="shared" ref="AO11" si="2">+_xlfn.RANK.EQ(AN11,$AN$9:$AN$15,1)</f>
@@ -44295,7 +44303,7 @@
       <c r="R13" s="158"/>
       <c r="S13" s="159">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,3,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,4,0)</f>
@@ -44303,7 +44311,7 @@
       </c>
       <c r="U13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,6,0)</f>
@@ -44333,15 +44341,15 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" ref="AE13" si="3">+AG13+AH13+AI13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" ref="AF13" si="4">+AG13*3+AH13</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AG13" s="53" cm="1">
         <f t="array" ref="AG13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH13" s="53" cm="1">
         <f t="array" ref="AH13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -44353,7 +44361,7 @@
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
@@ -44365,11 +44373,11 @@
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
-        <v>1.123013</v>
+        <v>1.113013</v>
       </c>
       <c r="AO13" s="53">
         <f t="shared" ref="AO13" si="5">+_xlfn.RANK.EQ(AN13,$AN$9:$AN$15,1)</f>
@@ -44403,7 +44411,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AU$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AU$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AU$7))</f>
-        <v>100</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="2:47" s="54" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -44523,7 +44531,7 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
@@ -44531,11 +44539,11 @@
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -44549,7 +44557,7 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" ref="AE15" si="6">+AG15+AH15+AI15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" ref="AF15" si="7">+AG15*3+AH15</f>
@@ -44565,7 +44573,7 @@
       </c>
       <c r="AI15" s="53" cm="1">
         <f t="array" ref="AI15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ15" s="53" cm="1">
         <f t="array" ref="AJ15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)+($K$9:$K$22=$AD15)*($J$9:$J$22))</f>
@@ -44573,7 +44581,7 @@
       </c>
       <c r="AK15" s="53" cm="1">
         <f t="array" ref="AK15">SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
@@ -44581,7 +44589,7 @@
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
@@ -44612,7 +44620,7 @@
 (SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>-3</v>
       </c>
       <c r="AU15" s="53" cm="1">
         <f t="array" ref="AU15">(SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -44693,11 +44701,15 @@
         <f>+VLOOKUP(B17,Aux!F:S,5,0)</f>
         <v>México</v>
       </c>
-      <c r="H17" s="258"/>
+      <c r="H17" s="258">
+        <v>0</v>
+      </c>
       <c r="I17" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="258"/>
+      <c r="J17" s="258">
+        <v>0</v>
+      </c>
       <c r="K17" s="38" t="str">
         <f>+VLOOKUP(B17,Aux!F:S,6,0)</f>
         <v>Ecuador</v>
@@ -44792,11 +44804,15 @@
         <f>+VLOOKUP(B19,Aux!F:S,5,0)</f>
         <v>Jamaica</v>
       </c>
-      <c r="H19" s="258"/>
+      <c r="H19" s="258">
+        <v>0</v>
+      </c>
       <c r="I19" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="258"/>
+      <c r="J19" s="258">
+        <v>3</v>
+      </c>
       <c r="K19" s="38" t="str">
         <f>+VLOOKUP(B19,Aux!F:S,6,0)</f>
         <v>Venezuela</v>
@@ -50816,13 +50832,13 @@
       <c r="M20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="68" t="str">
+      <c r="N20" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O20" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O20" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="2"/>
@@ -50857,13 +50873,13 @@
       <c r="M21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="68" t="str">
+      <c r="N21" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O21" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O21" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="2"/>

</xml_diff>

<commit_message>
fin fase de grupos
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79865A85-F37B-4B98-8062-EA261CC5560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6FB72-5239-44BD-BE4B-5CB1B19407D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -9905,23 +9905,23 @@
       </c>
       <c r="E5" s="197">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:E4),0))</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:F4),0))</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:G4),0))</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H5" s="198">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:H4),0))</f>
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="I5" s="199">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:I4),0))</f>
-        <v>150</v>
+        <v>295</v>
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>150.011</v>
+        <v>295.01100000000002</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
@@ -9957,23 +9957,23 @@
       </c>
       <c r="S5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="T5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="V5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="W5" s="120">
         <f t="shared" ref="W5:W26" ca="1" si="1">+SUM(S5:V5)</f>
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>110.005</v>
+        <v>230.005</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10007,23 +10007,23 @@
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>140</v>
+        <v>290</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>140.012</v>
+        <v>290.012</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
@@ -10059,23 +10059,23 @@
       </c>
       <c r="S6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="T6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="U6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="V6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="W6" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>110.006</v>
+        <v>235.006</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10105,27 +10105,27 @@
       </c>
       <c r="D7" s="151" t="str">
         <f ca="1">+VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:D6),0)</f>
-        <v>YUTA</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E7" s="197">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:E6),0))</f>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>130</v>
+        <v>270</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>130.00899999999999</v>
+        <v>270.00799999999998</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10161,23 +10161,23 @@
       </c>
       <c r="S7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="T7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="V7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="W7" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>130</v>
+        <v>265</v>
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>130.00700000000001</v>
+        <v>265.00700000000001</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10211,23 +10211,23 @@
       </c>
       <c r="E8" s="201">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:E7),0))</f>
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>130</v>
+        <v>265</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>130.00700000000001</v>
+        <v>265.00700000000001</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10263,23 +10263,23 @@
       </c>
       <c r="S8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="T8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="U8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="V8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="W8" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>125</v>
+        <v>270</v>
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>125.008</v>
+        <v>270.00799999999998</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10309,27 +10309,27 @@
       </c>
       <c r="D9" s="153" t="str">
         <f ca="1">+VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:D8),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>125</v>
+        <v>260</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>125.008</v>
+        <v>260.01</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="Q9" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R9" s="126" t="str">
         <f>Resultado!B11</f>
@@ -10365,23 +10365,23 @@
       </c>
       <c r="S9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="T9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="U9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="V9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="W9" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>130.00899999999999</v>
+        <v>250.00899999999999</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10415,23 +10415,23 @@
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>115.01300000000001</v>
+        <v>255.01300000000001</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10467,23 +10467,23 @@
       </c>
       <c r="S10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="T10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="U10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="V10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="W10" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>115</v>
+        <v>260</v>
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>115.01</v>
+        <v>260.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10513,27 +10513,27 @@
       </c>
       <c r="D11" s="151" t="str">
         <f ca="1">+VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:D10),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>115</v>
+        <v>250</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
@@ -10553,7 +10553,7 @@
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>115.01</v>
+        <v>250.00899999999999</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10569,23 +10569,23 @@
       </c>
       <c r="S11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="T11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="U11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="V11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="W11" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>150</v>
+        <v>295</v>
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>150.011</v>
+        <v>295.01100000000002</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10619,23 +10619,23 @@
       </c>
       <c r="E12" s="197">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:E11),0))</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:F11),0))</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:G11),0))</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H12" s="198">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:H11),0))</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="I12" s="200">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:I11),0))</f>
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>110.006</v>
+        <v>235.006</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10671,23 +10671,23 @@
       </c>
       <c r="S12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="T12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="U12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="V12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="W12" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>140</v>
+        <v>290</v>
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>140.012</v>
+        <v>290.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10721,23 +10721,23 @@
       </c>
       <c r="E13" s="201">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:E12),0))</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:F12),0))</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:G12),0))</f>
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="H13" s="202">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:H12),0))</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="I13" s="203">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:I12),0))</f>
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>110.005</v>
+        <v>230.005</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
@@ -10773,23 +10773,23 @@
       </c>
       <c r="S13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!S$4)</f>
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="T13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!T$4)</f>
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="U13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!U$4)</f>
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="V13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!V$4)</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="W13" s="120">
         <f t="shared" ca="1" si="1"/>
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>115.01300000000001</v>
+        <v>255.01300000000001</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12261,30 +12261,30 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="173">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" s="207"/>
       <c r="D1" s="207">
         <f>+A1</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="207"/>
       <c r="G1" s="207">
         <f>+D1+1</f>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H1" s="207"/>
       <c r="I1" s="207"/>
       <c r="J1" s="207">
         <f t="shared" ref="J1" si="0">+G1+1</f>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207">
         <f t="shared" ref="M1" si="1">+J1+1</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="S1" s="176" t="s">
         <v>60</v>
@@ -12400,25 +12400,25 @@
       <c r="C5" s="146"/>
       <c r="D5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(D1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo Cuartos</v>
       </c>
       <c r="E5" s="297"/>
       <c r="F5" s="298"/>
       <c r="G5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(G1,Aux!$F:$O,8,0)</f>
-        <v>Grupo B</v>
+        <v>Grupo Cuartos</v>
       </c>
       <c r="H5" s="297"/>
       <c r="I5" s="298"/>
       <c r="J5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(J1,Aux!$F:$O,8,0)</f>
-        <v>Grupo C</v>
+        <v>Grupo Cuartos</v>
       </c>
       <c r="K5" s="297"/>
       <c r="L5" s="298"/>
       <c r="M5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(M1,Aux!$F:$O,8,0)</f>
-        <v>Grupo C</v>
+        <v>Grupo Cuartos</v>
       </c>
       <c r="N5" s="297"/>
       <c r="O5" s="298"/>
@@ -12463,51 +12463,51 @@
       <c r="C6" s="146"/>
       <c r="D6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,5,0)</f>
-        <v>México</v>
+        <v>1A</v>
       </c>
       <c r="E6" s="217">
         <f>VLOOKUP(D1,Aux!$F:$O,3,0)</f>
-        <v>45473.708333333336</v>
+        <v>45477.833333333336</v>
       </c>
       <c r="F6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,6,0)</f>
-        <v>Ecuador</v>
+        <v>2B</v>
       </c>
       <c r="G6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,5,0)</f>
-        <v>Jamaica</v>
+        <v>1B</v>
       </c>
       <c r="H6" s="217">
         <f>VLOOKUP(G1,Aux!$F:$O,3,0)</f>
-        <v>45473.791666666664</v>
+        <v>45478.833333333336</v>
       </c>
       <c r="I6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,6,0)</f>
-        <v>Venezuela</v>
+        <v>2A</v>
       </c>
       <c r="J6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,5,0)</f>
-        <v>Estados Unidos</v>
+        <v>1D</v>
       </c>
       <c r="K6" s="217">
         <f>VLOOKUP(J1,Aux!$F:$O,3,0)</f>
-        <v>45474.833333333336</v>
+        <v>45480.625</v>
       </c>
       <c r="L6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,6,0)</f>
-        <v>Uruguay</v>
+        <v>2C</v>
       </c>
       <c r="M6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,5,0)</f>
-        <v>Bolivia</v>
+        <v>1C</v>
       </c>
       <c r="N6" s="217">
         <f>VLOOKUP(M1,Aux!$F:$O,3,0)</f>
-        <v>45474.875</v>
+        <v>45480.75</v>
       </c>
       <c r="O6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,6,0)</f>
-        <v>Panamá</v>
+        <v>2D</v>
       </c>
       <c r="P6" s="123"/>
       <c r="R6" s="214"/>
@@ -12557,25 +12557,25 @@
       <c r="D7" s="299"/>
       <c r="E7" s="220">
         <f>+E6</f>
-        <v>45473.708333333336</v>
+        <v>45477.833333333336</v>
       </c>
       <c r="F7" s="299"/>
       <c r="G7" s="299"/>
       <c r="H7" s="220">
         <f>+H6</f>
-        <v>45473.791666666664</v>
+        <v>45478.833333333336</v>
       </c>
       <c r="I7" s="299"/>
       <c r="J7" s="299"/>
       <c r="K7" s="220">
         <f>+K6</f>
-        <v>45474.833333333336</v>
+        <v>45480.625</v>
       </c>
       <c r="L7" s="299"/>
       <c r="M7" s="299"/>
       <c r="N7" s="220">
         <f>+N6</f>
-        <v>45474.875</v>
+        <v>45480.75</v>
       </c>
       <c r="O7" s="299"/>
       <c r="P7" s="123"/>
@@ -12625,59 +12625,59 @@
       <c r="C8" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="221">
+      <c r="D8" s="221" t="str">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="E8" s="222" t="str">
         <f ca="1">+IF(D8="","",IF(D8&gt;F8,1,IF(D8=F8,"X",2)))</f>
-        <v>X</v>
-      </c>
-      <c r="F8" s="223">
+        <v/>
+      </c>
+      <c r="F8" s="223" t="str">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="221">
+        <v/>
+      </c>
+      <c r="G8" s="221" t="str">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="222">
+        <v/>
+      </c>
+      <c r="H8" s="222" t="str">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v>2</v>
-      </c>
-      <c r="I8" s="223">
+        <v/>
+      </c>
+      <c r="I8" s="223" t="str">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
-        <v>3</v>
-      </c>
-      <c r="J8" s="221">
+        <v/>
+      </c>
+      <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="222">
+        <v/>
+      </c>
+      <c r="K8" s="222" t="str">
         <f ca="1">+IF(J8="","",IF(J8&gt;L8,1,IF(J8=L8,"X",2)))</f>
-        <v>2</v>
-      </c>
-      <c r="L8" s="223">
+        <v/>
+      </c>
+      <c r="L8" s="223" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,10,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="221">
+        <v/>
+      </c>
+      <c r="M8" s="221" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,9,0)</f>
-        <v>1</v>
-      </c>
-      <c r="N8" s="222">
+        <v/>
+      </c>
+      <c r="N8" s="222" t="str">
         <f ca="1">+IF(M8="","",IF(M8&gt;O8,1,IF(M8=O8,"X",2)))</f>
-        <v>2</v>
-      </c>
-      <c r="O8" s="223">
+        <v/>
+      </c>
+      <c r="O8" s="223" t="str">
         <f ca="1">VLOOKUP(M1,Aux!$F:$O,10,0)</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="P8" s="123"/>
       <c r="R8" s="214"/>
       <c r="S8" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>YUTA</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">IF(OR(T$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12685,15 +12685,15 @@
       </c>
       <c r="U8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(OR(U$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="V8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">IF(OR(V$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="W8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">IF(OR(W$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v>Canadá</v>
       </c>
       <c r="X8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">IF(OR(X$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -12767,43 +12767,43 @@
       </c>
       <c r="D10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="226">
         <f t="shared" ref="E10" ca="1" si="2">+IF(D10="","",IF(D10&gt;F10,1,IF(D10=F10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="225" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="226">
         <f t="shared" ref="H10" ca="1" si="3">+IF(G10="","",IF(G10&gt;I10,1,IF(G10=I10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="228" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K10" s="226">
         <f t="shared" ref="K10" ca="1" si="4">+IF(J10="","",IF(J10&gt;L10,1,IF(J10=L10,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N10" s="226">
         <f t="shared" ref="N10" ca="1" si="5">+IF(M10="","",IF(M10&gt;O10,1,IF(M10=O10,"X",2)))</f>
@@ -12811,13 +12811,13 @@
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="123"/>
       <c r="R10" s="214"/>
       <c r="S10" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">IF(OR(T$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12825,11 +12825,11 @@
       </c>
       <c r="U10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(OR(U$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Venezuela</v>
       </c>
       <c r="V10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(OR(V$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Ecuador</v>
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
@@ -12863,39 +12863,39 @@
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="231">
         <f t="shared" ref="E11:E29" ca="1" si="6">+IF(D11="","",IF(D11&gt;F11,1,IF(D11=F11,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="230" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="231">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12955,11 +12955,11 @@
       <c r="B12" s="214"/>
       <c r="C12" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>YUTA</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="231" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -12967,15 +12967,15 @@
       </c>
       <c r="F12" s="230" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="231">
+        <v>1</v>
+      </c>
+      <c r="H12" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -12983,19 +12983,19 @@
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="230" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N12" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13003,13 +13003,13 @@
       </c>
       <c r="O12" s="233" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="123"/>
       <c r="R12" s="214"/>
       <c r="S12" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="T12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">IF(OR(T$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -13025,7 +13025,7 @@
       </c>
       <c r="W12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W12" ca="1">IF(OR(W$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v>Chile</v>
       </c>
       <c r="X12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">IF(OR(X$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
@@ -13055,35 +13055,35 @@
       </c>
       <c r="D13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="230" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="233" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K13" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="230" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
@@ -13147,55 +13147,55 @@
       <c r="B14" s="214"/>
       <c r="C14" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="230" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="231">
+        <v>1</v>
+      </c>
+      <c r="H14" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I14" s="233" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K14" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="230" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O14" s="233" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="123"/>
       <c r="R14" s="214"/>
@@ -13247,47 +13247,47 @@
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="H15" s="231">
+      <c r="H15" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="230" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13339,51 +13339,51 @@
       <c r="B16" s="214"/>
       <c r="C16" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="230" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
         <v>1</v>
       </c>
-      <c r="H16" s="231">
+      <c r="H16" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" s="230" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="N16" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="N16" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O16" s="233" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13439,43 +13439,43 @@
       </c>
       <c r="D17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="231">
+        <v>1</v>
+      </c>
+      <c r="H17" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I17" s="233" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17" s="230" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N17" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13483,7 +13483,7 @@
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="123"/>
       <c r="R17" s="214"/>
@@ -13539,11 +13539,11 @@
       </c>
       <c r="E18" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="230" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13551,35 +13551,35 @@
       </c>
       <c r="H18" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K18" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" s="230" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
-      </c>
-      <c r="N18" s="231">
+        <v>0</v>
+      </c>
+      <c r="N18" s="231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="O18" s="233" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="123"/>
       <c r="R18" s="214"/>
@@ -19216,29 +19216,29 @@
         <f t="shared" ref="BR3" ca="1" si="20">IF(OR(BP3="",BQ3=""),"",IF(BP3&gt;BQ3,1,IF(BP3=BQ3,"x",2)))</f>
         <v>2</v>
       </c>
-      <c r="BS3" s="191" t="str">
+      <c r="BS3" s="191">
         <f ca="1">VLOOKUP(BS2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BT3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="BT3" s="191">
         <f ca="1">VLOOKUP(BS2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="BU3" s="191" t="str">
         <f t="shared" ref="BU3" ca="1" si="21">IF(OR(BS3="",BT3=""),"",IF(BS3&gt;BT3,1,IF(BS3=BT3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="BV3" s="191" t="str">
+        <v>x</v>
+      </c>
+      <c r="BV3" s="191">
         <f ca="1">VLOOKUP(BV2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="BW3" s="191" t="str">
+        <v>2</v>
+      </c>
+      <c r="BW3" s="191">
         <f ca="1">VLOOKUP(BV2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="BX3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="BX3" s="191">
         <f t="shared" ref="BX3" ca="1" si="22">IF(OR(BV3="",BW3=""),"",IF(BV3&gt;BW3,1,IF(BV3=BW3,"x",2)))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="BY3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="BY3" ca="1">IF(INDIRECT(BY2&amp;"!AE9")&lt;3,"",INDIRECT(BY2&amp;"!P9"))</f>
@@ -19254,39 +19254,39 @@
       </c>
       <c r="CB3" s="191" t="str" cm="1">
         <f t="array" aca="1" ref="CB3" ca="1">IF(INDIRECT(CB2&amp;"!AE9")&lt;3,"",INDIRECT(CB2&amp;"!P9"))</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="CC3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!H9)</f>
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="CD3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!N9)</f>
-        <v/>
+        <v>Ecuador</v>
       </c>
       <c r="CE3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!H12)</f>
-        <v/>
+        <v>Venezuela</v>
       </c>
       <c r="CF3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!N12)</f>
-        <v/>
+        <v>Canadá</v>
       </c>
       <c r="CG3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!H15)</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="CH3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!N15)</f>
-        <v/>
+        <v>Panamá</v>
       </c>
       <c r="CI3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!H18)</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="CJ3" s="191" t="str">
         <f ca="1">IF(CB3="","",Cuartos!N18)</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="CK3" s="191" t="str">
         <f>Semis!H9</f>
@@ -20550,15 +20550,15 @@
       </c>
       <c r="CC7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC2)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD2)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE2)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF2)=1,CF$5,0))</f>
@@ -20566,7 +20566,7 @@
       </c>
       <c r="CG7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG2)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH2)=1,CH$5,0))</f>
@@ -20574,11 +20574,11 @@
       </c>
       <c r="CI7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI2)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ7">
         <f ca="1">IF($B7=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ2)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK7">
         <f>IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK2)=1,CK$5,0))</f>
@@ -20984,7 +20984,7 @@
       </c>
       <c r="BU8">
         <f ca="1">IF($B8=0,0,IF(AND(BS$3=TotalApuestas!BS3,Resultado!BT$3=TotalApuestas!BT3),Resultado!BU$5+VLOOKUP(BU$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BU$3=TotalApuestas!BU3,BU$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BV8">
         <f ca="1">IF($B8=0,0,IF(BV$3=TotalApuestas!BV3,BV$5,0))</f>
@@ -21016,15 +21016,15 @@
       </c>
       <c r="CC8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC3)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD3)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE3)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF3)=1,CF$5,0))</f>
@@ -21032,7 +21032,7 @@
       </c>
       <c r="CG8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG3)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH3)=1,CH$5,0))</f>
@@ -21040,11 +21040,11 @@
       </c>
       <c r="CI8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI3)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ8">
         <f ca="1">IF($B8=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ3)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK8">
         <f>IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK3)=1,CK$5,0))</f>
@@ -21478,19 +21478,19 @@
       </c>
       <c r="CB9">
         <f ca="1">IF($B9=0,0,IF(CB$3=TotalApuestas!CB4,CB$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="CC9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC4)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD4)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE4)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF4)=1,CF$5,0))</f>
@@ -21498,7 +21498,7 @@
       </c>
       <c r="CG9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG4)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH4)=1,CH$5,0))</f>
@@ -21506,11 +21506,11 @@
       </c>
       <c r="CI9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI4)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ9">
         <f ca="1">IF($B9=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ4)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK9">
         <f>IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK4)=1,CK$5,0))</f>
@@ -21916,7 +21916,7 @@
       </c>
       <c r="BU10">
         <f ca="1">IF($B10=0,0,IF(AND(BS$3=TotalApuestas!BS5,Resultado!BT$3=TotalApuestas!BT5),Resultado!BU$5+VLOOKUP(BU$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BU$3=TotalApuestas!BU5,BU$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BV10">
         <f ca="1">IF($B10=0,0,IF(BV$3=TotalApuestas!BV5,BV$5,0))</f>
@@ -21948,23 +21948,23 @@
       </c>
       <c r="CC10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC5)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD5)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE5)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF5)=1,CF$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CG10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG5)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH5)=1,CH$5,0))</f>
@@ -21972,11 +21972,11 @@
       </c>
       <c r="CI10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI5)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ10">
         <f ca="1">IF($B10=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ5)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK10">
         <f>IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK5)=1,CK$5,0))</f>
@@ -22414,15 +22414,15 @@
       </c>
       <c r="CC11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC6)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD6)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE6)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF6)=1,CF$5,0))</f>
@@ -22430,7 +22430,7 @@
       </c>
       <c r="CG11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG6)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH6)=1,CH$5,0))</f>
@@ -22438,11 +22438,11 @@
       </c>
       <c r="CI11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI6)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ11">
         <f ca="1">IF($B11=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ6)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK11">
         <f>IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK6)=1,CK$5,0))</f>
@@ -22848,7 +22848,7 @@
       </c>
       <c r="BU12">
         <f ca="1">IF($B12=0,0,IF(AND(BS$3=TotalApuestas!BS7,Resultado!BT$3=TotalApuestas!BT7),Resultado!BU$5+VLOOKUP(BU$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BU$3=TotalApuestas!BU7,BU$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BV12">
         <f ca="1">IF($B12=0,0,IF(BV$3=TotalApuestas!BV7,BV$5,0))</f>
@@ -22880,23 +22880,23 @@
       </c>
       <c r="CC12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC7)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD7)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE7)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF7)=1,CF$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CG12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG7)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH7)=1,CH$5,0))</f>
@@ -22904,11 +22904,11 @@
       </c>
       <c r="CI12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI7)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ12">
         <f ca="1">IF($B12=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ7)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK12">
         <f>IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK7)=1,CK$5,0))</f>
@@ -23314,7 +23314,7 @@
       </c>
       <c r="BU13">
         <f ca="1">IF($B13=0,0,IF(AND(BS$3=TotalApuestas!BS8,Resultado!BT$3=TotalApuestas!BT8),Resultado!BU$5+VLOOKUP(BU$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BU$3=TotalApuestas!BU8,BU$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BV13">
         <f ca="1">IF($B13=0,0,IF(BV$3=TotalApuestas!BV8,BV$5,0))</f>
@@ -23342,19 +23342,19 @@
       </c>
       <c r="CB13">
         <f ca="1">IF($B13=0,0,IF(CB$3=TotalApuestas!CB8,CB$5,0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="CC13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC8)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD8)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE8)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF8)=1,CF$5,0))</f>
@@ -23362,7 +23362,7 @@
       </c>
       <c r="CG13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG8)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH8)=1,CH$5,0))</f>
@@ -23370,11 +23370,11 @@
       </c>
       <c r="CI13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI8)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ13">
         <f ca="1">IF($B13=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ8)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK13">
         <f>IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK8)=1,CK$5,0))</f>
@@ -23780,7 +23780,7 @@
       </c>
       <c r="BU14">
         <f ca="1">IF($B14=0,0,IF(AND(BS$3=TotalApuestas!BS9,Resultado!BT$3=TotalApuestas!BT9),Resultado!BU$5+VLOOKUP(BU$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(BU$3=TotalApuestas!BU9,BU$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BV14">
         <f ca="1">IF($B14=0,0,IF(BV$3=TotalApuestas!BV9,BV$5,0))</f>
@@ -23812,23 +23812,23 @@
       </c>
       <c r="CC14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC9)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD9)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE9)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF9)=1,CF$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CG14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG9)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH9)=1,CH$5,0))</f>
@@ -23836,11 +23836,11 @@
       </c>
       <c r="CI14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI9)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ14">
         <f ca="1">IF($B14=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ9)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK14">
         <f>IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK9)=1,CK$5,0))</f>
@@ -24278,23 +24278,23 @@
       </c>
       <c r="CC15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CC10)=1,CC$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CD15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CD10)=1,CD$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CE15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CE10)=1,CE$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CF15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CF10)=1,CF$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CG15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CG10)=1,CG$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CH15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CH10)=1,CH$5,0))</f>
@@ -24302,11 +24302,11 @@
       </c>
       <c r="CI15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CI10)=1,CI$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CJ15">
         <f ca="1">IF($B15=0,0,IF(COUNTIF($CC$3:$CJ$3,TotalApuestas!CJ10)=1,CJ$5,0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="CK15">
         <f>IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK10)=1,CK$5,0))</f>
@@ -41505,29 +41505,29 @@
         <f ca="1">+Resultado!BR3</f>
         <v>2</v>
       </c>
-      <c r="BS1" s="84" t="str">
+      <c r="BS1" s="84">
         <f ca="1">+Resultado!BS3</f>
-        <v/>
-      </c>
-      <c r="BT1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="BT1" s="84">
         <f ca="1">+Resultado!BT3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="BU1" s="84" t="str">
         <f ca="1">+Resultado!BU3</f>
-        <v/>
-      </c>
-      <c r="BV1" s="84" t="str">
+        <v>x</v>
+      </c>
+      <c r="BV1" s="84">
         <f ca="1">+Resultado!BV3</f>
-        <v/>
-      </c>
-      <c r="BW1" s="84" t="str">
+        <v>2</v>
+      </c>
+      <c r="BW1" s="84">
         <f ca="1">+Resultado!BW3</f>
-        <v/>
-      </c>
-      <c r="BX1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="BX1" s="84">
         <f ca="1">+Resultado!BX3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="BY1" s="84" t="str">
         <f ca="1">+Resultado!BY3</f>
@@ -41543,39 +41543,39 @@
       </c>
       <c r="CB1" s="84" t="str">
         <f ca="1">+Resultado!CB3</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="CC1" s="84" t="str">
         <f ca="1">+Resultado!CC3</f>
-        <v/>
+        <v>Argentina</v>
       </c>
       <c r="CD1" s="84" t="str">
         <f ca="1">+Resultado!CD3</f>
-        <v/>
+        <v>Ecuador</v>
       </c>
       <c r="CE1" s="84" t="str">
         <f ca="1">+Resultado!CE3</f>
-        <v/>
+        <v>Venezuela</v>
       </c>
       <c r="CF1" s="84" t="str">
         <f ca="1">+Resultado!CF3</f>
-        <v/>
+        <v>Canadá</v>
       </c>
       <c r="CG1" s="84" t="str">
         <f ca="1">+Resultado!CG3</f>
-        <v/>
+        <v>Colombia</v>
       </c>
       <c r="CH1" s="84" t="str">
         <f ca="1">+Resultado!CH3</f>
-        <v/>
+        <v>Panamá</v>
       </c>
       <c r="CI1" s="84" t="str">
         <f ca="1">+Resultado!CI3</f>
-        <v/>
+        <v>Uruguay</v>
       </c>
       <c r="CJ1" s="84" t="str">
         <f ca="1">+Resultado!CJ3</f>
-        <v/>
+        <v>Brasil</v>
       </c>
       <c r="CK1" s="84" t="str">
         <f>+Resultado!CK3</f>
@@ -46561,7 +46561,7 @@
   <dimension ref="B1:AU26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46832,11 +46832,11 @@
       <c r="AQ5" s="53"/>
       <c r="AR5" s="245">
         <f>+VLOOKUP(AR7,$AD$9:$AF$15,3,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AS5" s="245">
         <f>+VLOOKUP(AS7,$AD$9:$AF$15,3,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AT5" s="245">
         <f>+VLOOKUP(AT7,$AD$9:$AF$15,3,0)</f>
@@ -46844,7 +46844,7 @@
       </c>
       <c r="AU5" s="245">
         <f>+VLOOKUP(AU7,$AD$9:$AF$15,3,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:47" s="54" customFormat="1" ht="22.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -47103,7 +47103,7 @@
       <c r="R9" s="158"/>
       <c r="S9" s="159">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,3,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,4,0)</f>
@@ -47111,7 +47111,7 @@
       </c>
       <c r="U9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,5,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="160">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,6,0)</f>
@@ -47119,11 +47119,11 @@
       </c>
       <c r="W9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,7,0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X9" s="161">
         <f>+VLOOKUP($P9,$AD$9:$AK$15,8,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y9" s="161">
         <f>+W9-X9</f>
@@ -47141,11 +47141,11 @@
       </c>
       <c r="AE9" s="53">
         <f>+AG9+AH9+AI9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="53">
         <f>+AG9*3+AH9</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG9" s="53" cm="1">
         <f t="array" ref="AG9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -47153,7 +47153,7 @@
       </c>
       <c r="AH9" s="53" cm="1">
         <f t="array" ref="AH9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD9)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI9" s="53" cm="1">
         <f t="array" ref="AI9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -47161,11 +47161,11 @@
       </c>
       <c r="AJ9" s="53" cm="1">
         <f t="array" ref="AJ9">SUM(($G$9:$G$22=$AD9)*($H$9:$H$22)+($K$9:$K$22=$AD9)*($J$9:$J$22))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AK9" s="53" cm="1">
         <f t="array" ref="AK9">SUM(($G$9:$G$22=$AD9)*($J$9:$J$22)+($K$9:$K$22=$AD9)*($H$9:$H$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL9" s="252">
         <f>+SUMIFS($AR9:$AU9,$AR$5:$AU$5,AF9)</f>
@@ -47319,7 +47319,7 @@
       <c r="R11" s="158"/>
       <c r="S11" s="159">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,3,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,4,0)</f>
@@ -47327,7 +47327,7 @@
       </c>
       <c r="U11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,5,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11" s="160">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,6,0)</f>
@@ -47335,11 +47335,11 @@
       </c>
       <c r="W11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,7,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X11" s="161">
         <f>+VLOOKUP($P11,$AD$9:$AK$15,8,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="161">
         <f>+W11-X11</f>
@@ -47357,11 +47357,11 @@
       </c>
       <c r="AE11" s="53">
         <f t="shared" ref="AE11" si="0">+AG11+AH11+AI11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF11" s="53">
         <f t="shared" ref="AF11" si="1">+AG11*3+AH11</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG11" s="53" cm="1">
         <f t="array" ref="AG11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22))</f>
@@ -47369,7 +47369,7 @@
       </c>
       <c r="AH11" s="53" cm="1">
         <f t="array" ref="AH11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD11)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" s="53" cm="1">
         <f t="array" ref="AI11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22&gt;$J$9:$J$22))</f>
@@ -47377,11 +47377,11 @@
       </c>
       <c r="AJ11" s="53" cm="1">
         <f t="array" ref="AJ11">SUM(($G$9:$G$22=$AD11)*($H$9:$H$22)+($K$9:$K$22=$AD11)*($J$9:$J$22))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AK11" s="53" cm="1">
         <f t="array" ref="AK11">SUM(($G$9:$G$22=$AD11)*($J$9:$J$22)+($K$9:$K$22=$AD11)*($H$9:$H$22))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL11" s="252">
         <f>+SUMIFS($AR11:$AU11,$AR$5:$AU$5,AF11)</f>
@@ -47535,11 +47535,11 @@
       <c r="R13" s="158"/>
       <c r="S13" s="159">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,3,0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="160">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,5,0)</f>
@@ -47551,15 +47551,15 @@
       </c>
       <c r="W13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,7,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X13" s="161">
         <f>+VLOOKUP($P13,$AD$9:$AK$15,8,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y13" s="161">
         <f>+W13-X13</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="Z13" s="60"/>
       <c r="AA13" s="57"/>
@@ -47573,7 +47573,7 @@
       </c>
       <c r="AE13" s="53">
         <f t="shared" ref="AE13" si="3">+AG13+AH13+AI13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF13" s="53">
         <f t="shared" ref="AF13" si="4">+AG13*3+AH13</f>
@@ -47589,15 +47589,15 @@
       </c>
       <c r="AI13" s="53" cm="1">
         <f t="array" ref="AI13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22&lt;$J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22&gt;$J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ13" s="53" cm="1">
         <f t="array" ref="AJ13">SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)+($K$9:$K$22=$AD13)*($J$9:$J$22))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK13" s="53" cm="1">
         <f t="array" ref="AK13">SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)+($K$9:$K$22=$AD13)*($H$9:$H$22))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AL13" s="252">
         <f>+SUMIFS($AR13:$AU13,$AR$5:$AU$5,AF13)</f>
@@ -47605,7 +47605,7 @@
       </c>
       <c r="AM13" s="252">
         <f>+AJ13-AK13</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="AN13" s="53">
         <f>+_xlfn.RANK.EQ(AF13,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM13,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ13,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL13,$AL$9:$AL$15)/1000+ROW()/1000000</f>
@@ -47643,7 +47643,7 @@
 (SUM(($G$9:$G$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AU$7)))*100
 +SUM(($G$9:$G$22=$AD13)*($H$9:$H$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($J$9:$J$22)*($G$9:$G$22=AU$7))
 -SUM(($G$9:$G$22=$AD13)*($J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD13)*($H$9:$H$22)*($G$9:$G$22=AU$7))</f>
-        <v>100</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="2:47" s="54" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -47763,19 +47763,19 @@
       </c>
       <c r="V15" s="160">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,6,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,7,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X15" s="161">
         <f>+VLOOKUP($P15,$AD$9:$AK$15,8,0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y15" s="161">
         <f>+W15-X15</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="Z15" s="60"/>
       <c r="AA15" s="59"/>
@@ -47789,15 +47789,15 @@
       </c>
       <c r="AE15" s="53">
         <f t="shared" ref="AE15" si="6">+AG15+AH15+AI15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF15" s="53">
         <f t="shared" ref="AF15" si="7">+AG15*3+AH15</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG15" s="53" cm="1">
         <f t="array" ref="AG15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15" s="53" cm="1">
         <f t="array" ref="AH15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;"")+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($H$9:$H$22&lt;&gt;""))</f>
@@ -47809,11 +47809,11 @@
       </c>
       <c r="AJ15" s="53" cm="1">
         <f t="array" ref="AJ15">SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)+($K$9:$K$22=$AD15)*($J$9:$J$22))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK15" s="53" cm="1">
         <f t="array" ref="AK15">SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)+($K$9:$K$22=$AD15)*($H$9:$H$22))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL15" s="252">
         <f>+SUMIFS($AR15:$AU15,$AR$5:$AU$5,AF15)</f>
@@ -47821,7 +47821,7 @@
       </c>
       <c r="AM15" s="252">
         <f>+AJ15-AK15</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="AN15" s="53">
         <f>+_xlfn.RANK.EQ(AF15,$AF$9:$AF$15)+_xlfn.RANK.EQ(AM15,$AM$9:$AM$15)/10+_xlfn.RANK.EQ(AJ15,$AJ$9:$AJ$15)/100+_xlfn.RANK.EQ(AL15,$AL$9:$AL$15)/1000+ROW()/1000000</f>
@@ -47852,7 +47852,7 @@
 (SUM(($G$9:$G$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22=$J$9:$J$22)*($G$9:$G$22=AT$7)))*100
 +SUM(($G$9:$G$22=$AD15)*($H$9:$H$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($J$9:$J$22)*($G$9:$G$22=AT$7))
 -SUM(($G$9:$G$22=$AD15)*($J$9:$J$22)*($K$9:$K$22=AT$7)+($K$9:$K$22=$AD15)*($H$9:$H$22)*($G$9:$G$22=AT$7))</f>
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="AU15" s="53" cm="1">
         <f t="array" ref="AU15">(SUM(($G$9:$G$22=$AD15)*($H$9:$H$22&gt;$J$9:$J$22)*($K$9:$K$22=AU$7)+($K$9:$K$22=$AD15)*($H$9:$H$22&lt;$J$9:$J$22)*($G$9:$G$22=AU$7)))*300+
@@ -47933,11 +47933,15 @@
         <f>+VLOOKUP(B17,Aux!F:S,5,0)</f>
         <v>Brasil</v>
       </c>
-      <c r="H17" s="258"/>
+      <c r="H17" s="258">
+        <v>1</v>
+      </c>
       <c r="I17" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="258"/>
+      <c r="J17" s="258">
+        <v>1</v>
+      </c>
       <c r="K17" s="38" t="str">
         <f>+VLOOKUP(B17,Aux!F:S,6,0)</f>
         <v>Colombia</v>
@@ -48032,11 +48036,15 @@
         <f>+VLOOKUP(B19,Aux!F:S,5,0)</f>
         <v>Costa Rica</v>
       </c>
-      <c r="H19" s="258"/>
+      <c r="H19" s="258">
+        <v>2</v>
+      </c>
       <c r="I19" s="257" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="258"/>
+      <c r="J19" s="258">
+        <v>1</v>
+      </c>
       <c r="K19" s="38" t="str">
         <f>+VLOOKUP(B19,Aux!F:S,6,0)</f>
         <v>Paraguay</v>
@@ -48169,7 +48177,7 @@
   <dimension ref="A7:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -51002,13 +51010,13 @@
       <c r="M24" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="N24" s="68" t="str">
+      <c r="N24" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O24" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="O24" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="2"/>
@@ -51043,13 +51051,13 @@
       <c r="M25" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="68" t="str">
+      <c r="N25" s="68">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="O25" s="68" t="str">
+        <v>2</v>
+      </c>
+      <c r="O25" s="68">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="2"/>

</xml_diff>

<commit_message>
termino los cuartos de final
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6FB72-5239-44BD-BE4B-5CB1B19407D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCE558-BFCB-47BB-ADBC-7AD0D02E3494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -9925,11 +9925,11 @@
       </c>
       <c r="J5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:J4),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:K4),0))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:L4),0))</f>
@@ -9937,15 +9937,15 @@
       </c>
       <c r="M5" s="128">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:M4),0))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>295.01100000000002</v>
+        <v>375.01100000000002</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
-        <v>-5.0000000000000001E-4</v>
+        <v>79.999499999999998</v>
       </c>
       <c r="Q5" s="119">
         <f t="shared" ref="Q5:Q26" ca="1" si="0">+_xlfn.RANK.EQ(AB5,$AB$5:$AB$26)</f>
@@ -9977,11 +9977,11 @@
       </c>
       <c r="X5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -9989,11 +9989,11 @@
       </c>
       <c r="AA5" s="122">
         <f t="shared" ref="AA5:AA26" ca="1" si="2">+SUM(X5:Z5)</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>230.005</v>
+        <v>295.005</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10003,35 +10003,35 @@
       </c>
       <c r="D6" s="151" t="str">
         <f ca="1">+VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:D5),0)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:K5),0))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:L5),0))</f>
@@ -10039,15 +10039,15 @@
       </c>
       <c r="M6" s="128">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:M5),0))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>290.012</v>
+        <v>345.01299999999998</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
-        <v>-5.9999999999999995E-4</v>
+        <v>89.999399999999994</v>
       </c>
       <c r="Q6" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10079,11 +10079,11 @@
       </c>
       <c r="X6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10091,11 +10091,11 @@
       </c>
       <c r="AA6" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>235.006</v>
+        <v>300.00599999999997</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10105,35 +10105,35 @@
       </c>
       <c r="D7" s="151" t="str">
         <f ca="1">+VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:D6),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="E7" s="197">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:E6),0))</f>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:K6),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:L6),0))</f>
@@ -10141,15 +10141,15 @@
       </c>
       <c r="M7" s="128">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:M6),0))</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>270.00799999999998</v>
+        <v>345.012</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-6.9999999999999999E-4</v>
+        <v>54.999299999999998</v>
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10181,11 +10181,11 @@
       </c>
       <c r="X7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Z7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10193,11 +10193,11 @@
       </c>
       <c r="AA7" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>265.00700000000001</v>
+        <v>345.00700000000001</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10231,11 +10231,11 @@
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:K7),0))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:L7),0))</f>
@@ -10243,19 +10243,19 @@
       </c>
       <c r="M8" s="131">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:M7),0))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>265.00700000000001</v>
+        <v>345.00700000000001</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-8.0000000000000004E-4</v>
+        <v>79.999200000000002</v>
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10283,11 +10283,11 @@
       </c>
       <c r="X8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10295,11 +10295,11 @@
       </c>
       <c r="AA8" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>270.00799999999998</v>
+        <v>340.00799999999998</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10309,35 +10309,35 @@
       </c>
       <c r="D9" s="153" t="str">
         <f ca="1">+VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:D8),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:K8),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:L8),0))</f>
@@ -10345,15 +10345,15 @@
       </c>
       <c r="M9" s="134">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:M8),0))</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>260.01</v>
+        <v>340.00799999999998</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-8.9999999999999998E-4</v>
+        <v>69.999099999999999</v>
       </c>
       <c r="Q9" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10385,11 +10385,11 @@
       </c>
       <c r="X9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10397,11 +10397,11 @@
       </c>
       <c r="AA9" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>250.00899999999999</v>
+        <v>315.00900000000001</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10411,35 +10411,35 @@
       </c>
       <c r="D10" s="151" t="str">
         <f ca="1">+VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:D9),0)</f>
-        <v>Moises</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:K9),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:L9),0))</f>
@@ -10447,19 +10447,19 @@
       </c>
       <c r="M10" s="128">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:M9),0))</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>255.01300000000001</v>
+        <v>325.01</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-1E-3</v>
+        <v>64.998999999999995</v>
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10487,11 +10487,11 @@
       </c>
       <c r="X10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10499,11 +10499,11 @@
       </c>
       <c r="AA10" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>260.01</v>
+        <v>325.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10537,11 +10537,11 @@
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:K10),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:L10),0))</f>
@@ -10549,15 +10549,15 @@
       </c>
       <c r="M11" s="128">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:M10),0))</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>250.00899999999999</v>
+        <v>315.00900000000001</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.1000000000000001E-3</v>
+        <v>64.998900000000006</v>
       </c>
       <c r="Q11" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10589,11 +10589,11 @@
       </c>
       <c r="X11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Z11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10601,11 +10601,11 @@
       </c>
       <c r="AA11" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>295.01100000000002</v>
+        <v>375.01100000000002</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10639,11 +10639,11 @@
       </c>
       <c r="J12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:J11),0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:K11),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:L11),0))</f>
@@ -10651,19 +10651,19 @@
       </c>
       <c r="M12" s="128">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:M11),0))</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>235.006</v>
+        <v>300.00599999999997</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.1999999999999999E-3</v>
+        <v>64.998800000000003</v>
       </c>
       <c r="Q12" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="126" t="str">
         <f>Resultado!B14</f>
@@ -10691,11 +10691,11 @@
       </c>
       <c r="X12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Z12" s="120">
         <f ca="1">+SUMIFS(Resultado!14:14,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10703,11 +10703,11 @@
       </c>
       <c r="AA12" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="AB12" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>290.012</v>
+        <v>345.012</v>
       </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
@@ -10741,11 +10741,11 @@
       </c>
       <c r="J13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:J12),0))</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:K12),0))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:L12),0))</f>
@@ -10753,19 +10753,19 @@
       </c>
       <c r="M13" s="131">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:M12),0))</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>230.005</v>
+        <v>295.005</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.2999999999999999E-3</v>
+        <v>64.998699999999999</v>
       </c>
       <c r="Q13" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R13" s="126" t="str">
         <f>Resultado!B15</f>
@@ -10793,11 +10793,11 @@
       </c>
       <c r="X13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!X$4)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Y13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Z13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
@@ -10805,11 +10805,11 @@
       </c>
       <c r="AA13" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>255.01300000000001</v>
+        <v>345.01299999999998</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12233,7 +12233,7 @@
   <dimension ref="A1:AE37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V37" sqref="V37"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12261,33 +12261,33 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="173">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C1" s="207"/>
       <c r="D1" s="207">
         <f>+A1</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="207"/>
       <c r="G1" s="207">
         <f>+D1+1</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H1" s="207"/>
       <c r="I1" s="207"/>
       <c r="J1" s="207">
         <f t="shared" ref="J1" si="0">+G1+1</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K1" s="207"/>
       <c r="L1" s="207"/>
       <c r="M1" s="207">
         <f t="shared" ref="M1" si="1">+J1+1</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="S1" s="176" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="T1" s="208"/>
       <c r="U1" s="208"/>
@@ -12400,25 +12400,25 @@
       <c r="C5" s="146"/>
       <c r="D5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(D1,Aux!$F:$O,8,0)</f>
-        <v>Grupo Cuartos</v>
+        <v>Grupo Semis</v>
       </c>
       <c r="E5" s="297"/>
       <c r="F5" s="298"/>
       <c r="G5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(G1,Aux!$F:$O,8,0)</f>
-        <v>Grupo Cuartos</v>
+        <v>Grupo Semis</v>
       </c>
       <c r="H5" s="297"/>
       <c r="I5" s="298"/>
       <c r="J5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(J1,Aux!$F:$O,8,0)</f>
-        <v>Grupo Cuartos</v>
+        <v>Grupo Final</v>
       </c>
       <c r="K5" s="297"/>
       <c r="L5" s="298"/>
       <c r="M5" s="296" t="str">
         <f>"Grupo "&amp;VLOOKUP(M1,Aux!$F:$O,8,0)</f>
-        <v>Grupo Cuartos</v>
+        <v>Grupo Final</v>
       </c>
       <c r="N5" s="297"/>
       <c r="O5" s="298"/>
@@ -12426,30 +12426,20 @@
       <c r="R5" s="214"/>
       <c r="S5" s="215"/>
       <c r="T5" s="216" t="str" cm="1">
-        <f t="array" ref="T5:AA5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
-        <v>Cuartos1</v>
+        <f t="array" ref="T5:V5">S1&amp;_xlfn.SEQUENCE(1,VLOOKUP(S1,$AD$1:$AE$5,2,0))</f>
+        <v>Final1</v>
       </c>
       <c r="U5" s="216" t="str">
-        <v>Cuartos2</v>
+        <v>Final2</v>
       </c>
       <c r="V5" s="216" t="str">
-        <v>Cuartos3</v>
-      </c>
-      <c r="W5" s="216" t="str">
-        <v>Cuartos4</v>
-      </c>
-      <c r="X5" s="216" t="str">
-        <v>Cuartos5</v>
-      </c>
-      <c r="Y5" s="216" t="str">
-        <v>Cuartos6</v>
-      </c>
-      <c r="Z5" s="216" t="str">
-        <v>Cuartos7</v>
-      </c>
-      <c r="AA5" s="216" t="str">
-        <v>Cuartos8</v>
-      </c>
+        <v>Final3</v>
+      </c>
+      <c r="W5" s="216"/>
+      <c r="X5" s="216"/>
+      <c r="Y5" s="216"/>
+      <c r="Z5" s="216"/>
+      <c r="AA5" s="216"/>
       <c r="AB5" s="123"/>
       <c r="AD5" s="207" t="s">
         <v>94</v>
@@ -12463,51 +12453,51 @@
       <c r="C6" s="146"/>
       <c r="D6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,5,0)</f>
-        <v>1A</v>
+        <v>Ganador cuartos de final 1</v>
       </c>
       <c r="E6" s="217">
         <f>VLOOKUP(D1,Aux!$F:$O,3,0)</f>
-        <v>45477.833333333336</v>
+        <v>45482.833333333336</v>
       </c>
       <c r="F6" s="299" t="str">
         <f>VLOOKUP(D1,Aux!$F:$O,6,0)</f>
-        <v>2B</v>
+        <v>Ganador cuartos de final 2</v>
       </c>
       <c r="G6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,5,0)</f>
-        <v>1B</v>
+        <v>Ganador cuartos de final 3</v>
       </c>
       <c r="H6" s="217">
         <f>VLOOKUP(G1,Aux!$F:$O,3,0)</f>
-        <v>45478.833333333336</v>
+        <v>45483.833333333336</v>
       </c>
       <c r="I6" s="299" t="str">
         <f>VLOOKUP(G1,Aux!$F:$O,6,0)</f>
-        <v>2A</v>
+        <v>Ganador cuartos de final 4</v>
       </c>
       <c r="J6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,5,0)</f>
-        <v>1D</v>
+        <v>Perdedor semifinal 1</v>
       </c>
       <c r="K6" s="217">
         <f>VLOOKUP(J1,Aux!$F:$O,3,0)</f>
-        <v>45480.625</v>
+        <v>45486.833333333336</v>
       </c>
       <c r="L6" s="299" t="str">
         <f>VLOOKUP(J1,Aux!$F:$O,6,0)</f>
-        <v>2C</v>
+        <v>Perdedor semifinal 2</v>
       </c>
       <c r="M6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,5,0)</f>
-        <v>1C</v>
+        <v>Ganador semifinal 1</v>
       </c>
       <c r="N6" s="217">
         <f>VLOOKUP(M1,Aux!$F:$O,3,0)</f>
-        <v>45480.75</v>
+        <v>45487.833333333336</v>
       </c>
       <c r="O6" s="299" t="str">
         <f>VLOOKUP(M1,Aux!$F:$O,6,0)</f>
-        <v>2D</v>
+        <v>Ganador semifinal 2</v>
       </c>
       <c r="P6" s="123"/>
       <c r="R6" s="214"/>
@@ -12521,31 +12511,31 @@
       </c>
       <c r="U6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">IF(OR(U$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="V6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">IF(OR(V$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Argentina</v>
       </c>
       <c r="W6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">IF(OR(W$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v/>
       </c>
       <c r="X6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">IF(OR(X$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="Y6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y6" ca="1">IF(OR(Y$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z6" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z6" ca="1">IF(OR(Z$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA6" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA6" ca="1">IF(OR(AA$5="",$S6=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S6,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="AB6" s="123"/>
       <c r="AD6"/>
@@ -12557,32 +12547,32 @@
       <c r="D7" s="299"/>
       <c r="E7" s="220">
         <f>+E6</f>
-        <v>45477.833333333336</v>
+        <v>45482.833333333336</v>
       </c>
       <c r="F7" s="299"/>
       <c r="G7" s="299"/>
       <c r="H7" s="220">
         <f>+H6</f>
-        <v>45478.833333333336</v>
+        <v>45483.833333333336</v>
       </c>
       <c r="I7" s="299"/>
       <c r="J7" s="299"/>
       <c r="K7" s="220">
         <f>+K6</f>
-        <v>45480.625</v>
+        <v>45486.833333333336</v>
       </c>
       <c r="L7" s="299"/>
       <c r="M7" s="299"/>
       <c r="N7" s="220">
         <f>+N6</f>
-        <v>45480.75</v>
+        <v>45487.833333333336</v>
       </c>
       <c r="O7" s="299"/>
       <c r="P7" s="123"/>
       <c r="R7" s="214"/>
       <c r="S7" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="T7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">IF(OR(T$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12590,31 +12580,31 @@
       </c>
       <c r="U7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U7" ca="1">IF(OR(U$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="V7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V7" ca="1">IF(OR(V$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v/>
       </c>
       <c r="X7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">IF(OR(X$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y7" ca="1">IF(OR(Y$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z7" ca="1">IF(OR(Z$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA7" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA7" ca="1">IF(OR(AA$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB7" s="123"/>
       <c r="AD7"/>
@@ -12677,39 +12667,39 @@
       <c r="R8" s="214"/>
       <c r="S8" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="T8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">IF(OR(T$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
-        <v>Argentina</v>
+        <v>Venezuela</v>
       </c>
       <c r="U8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(OR(U$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="V8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">IF(OR(V$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="W8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">IF(OR(W$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v/>
       </c>
       <c r="X8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">IF(OR(X$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y8" ca="1">IF(OR(Y$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z8" ca="1">IF(OR(Z$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA8" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA8" ca="1">IF(OR(AA$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB8" s="123"/>
       <c r="AD8"/>
@@ -12729,31 +12719,31 @@
       </c>
       <c r="U9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U9" ca="1">IF(OR(U$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Colombia</v>
       </c>
       <c r="V9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V9" ca="1">IF(OR(V$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Colombia</v>
       </c>
       <c r="W9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">IF(OR(W$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v/>
       </c>
       <c r="X9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">IF(OR(X$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="Y9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y9" ca="1">IF(OR(Y$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z9" ca="1">IF(OR(Z$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA9" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA9" ca="1">IF(OR(AA$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="AB9" s="123"/>
       <c r="AD9"/>
@@ -12775,11 +12765,11 @@
       </c>
       <c r="F10" s="225" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="226">
         <f t="shared" ref="H10" ca="1" si="3">+IF(G10="","",IF(G10&gt;I10,1,IF(G10=I10,"X",2)))</f>
@@ -12787,11 +12777,11 @@
       </c>
       <c r="I10" s="228" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="225">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K10" s="226">
         <f t="shared" ref="K10" ca="1" si="4">+IF(J10="","",IF(J10&gt;L10,1,IF(J10=L10,"X",2)))</f>
@@ -12799,7 +12789,7 @@
       </c>
       <c r="L10" s="225" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="227">
         <f ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12811,13 +12801,13 @@
       </c>
       <c r="O10" s="228" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">IF($C10="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C10,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="123"/>
       <c r="R10" s="214"/>
       <c r="S10" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">IF(OR(T$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12825,31 +12815,31 @@
       </c>
       <c r="U10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(OR(U$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Brasil</v>
       </c>
       <c r="V10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(OR(V$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Brasil</v>
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v/>
       </c>
       <c r="X10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">IF(OR(X$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y10" ca="1">IF(OR(Y$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z10" ca="1">IF(OR(Z$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA10" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA10" ca="1">IF(OR(AA$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB10" s="123"/>
       <c r="AD10"/>
@@ -12859,7 +12849,7 @@
       <c r="B11" s="214"/>
       <c r="C11" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
@@ -12875,7 +12865,7 @@
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="231">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
@@ -12883,37 +12873,37 @@
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" s="231">
         <f t="shared" ref="N11:N29" ca="1" si="9">+IF(M11="","",IF(M11&gt;O11,1,IF(M11=O11,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="233" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="123"/>
       <c r="R11" s="214"/>
       <c r="S11" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Moises</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">IF(OR(T$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12921,31 +12911,31 @@
       </c>
       <c r="U11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(OR(U$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="V11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(OR(V$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">IF(OR(W$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Canadá</v>
+        <v/>
       </c>
       <c r="X11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">IF(OR(X$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">IF(OR(Y$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">IF(OR(Z$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA11" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">IF(OR(AA$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB11" s="123"/>
       <c r="AD11"/>
@@ -12955,27 +12945,27 @@
       <c r="B12" s="214"/>
       <c r="C12" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="D12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="231">
+        <f t="shared" ca="1" si="6"/>
         <v>2</v>
-      </c>
-      <c r="E12" s="231" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>X</v>
       </c>
       <c r="F12" s="230" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="231" t="str">
+        <v>2</v>
+      </c>
+      <c r="H12" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
@@ -12983,7 +12973,7 @@
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -12991,15 +12981,15 @@
       </c>
       <c r="L12" s="230" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N12" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="233" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13017,31 +13007,31 @@
       </c>
       <c r="U12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">IF(OR(U$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="V12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">IF(OR(V$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Uruguay</v>
       </c>
       <c r="W12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W12" ca="1">IF(OR(W$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v/>
       </c>
       <c r="X12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">IF(OR(X$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y12" ca="1">IF(OR(Y$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z12" ca="1">IF(OR(Z$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA12" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA12" ca="1">IF(OR(AA$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB12" s="123"/>
       <c r="AD12"/>
@@ -13055,7 +13045,7 @@
       </c>
       <c r="D13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13071,31 +13061,31 @@
       </c>
       <c r="H13" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="233" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K13" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="230" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="233" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -13113,31 +13103,31 @@
       </c>
       <c r="U13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U13" ca="1">IF(OR(U$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="V13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V13" ca="1">IF(OR(V$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Argentina</v>
       </c>
       <c r="W13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">IF(OR(W$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v/>
       </c>
       <c r="X13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">IF(OR(X$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y13" ca="1">IF(OR(Y$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z13" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z13" ca="1">IF(OR(Z$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA13" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA13" ca="1">IF(OR(AA$5="",$S13=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S13,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB13" s="123"/>
       <c r="AD13"/>
@@ -13147,11 +13137,11 @@
       <c r="B14" s="214"/>
       <c r="C14" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13163,7 +13153,7 @@
       </c>
       <c r="G14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -13171,11 +13161,11 @@
       </c>
       <c r="I14" s="233" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K14" s="231">
         <f t="shared" ca="1" si="8"/>
@@ -13187,15 +13177,15 @@
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="233" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="123"/>
       <c r="R14" s="214"/>
@@ -13209,31 +13199,31 @@
       </c>
       <c r="U14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">IF(OR(U$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Uruguay</v>
       </c>
       <c r="V14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">IF(OR(V$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Ecuador</v>
+        <v>Argentina</v>
       </c>
       <c r="W14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">IF(OR(W$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
-        <v>Chile</v>
+        <v/>
       </c>
       <c r="X14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="X14" ca="1">IF(OR(X$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:X$1)-1),0))</f>
-        <v>Brasil</v>
+        <v/>
       </c>
       <c r="Y14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Y14" ca="1">IF(OR(Y$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Y$1)-1),0))</f>
-        <v>Estados Unidos</v>
+        <v/>
       </c>
       <c r="Z14" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="Z14" ca="1">IF(OR(Z$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:Z$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v/>
       </c>
       <c r="AA14" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="AA14" ca="1">IF(OR(AA$5="",$S14=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S14,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:AA$1)-1),0))</f>
-        <v>Colombia</v>
+        <v/>
       </c>
       <c r="AB14" s="123"/>
       <c r="AD14"/>
@@ -13243,11 +13233,11 @@
       <c r="B15" s="214"/>
       <c r="C15" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Moises</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13255,7 +13245,7 @@
       </c>
       <c r="F15" s="230" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
@@ -13283,15 +13273,15 @@
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="233" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="123"/>
       <c r="R15" s="214"/>
@@ -13343,7 +13333,7 @@
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13355,39 +13345,39 @@
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="231" t="str">
+        <v>3</v>
+      </c>
+      <c r="H16" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="230" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" s="233" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P16" s="123"/>
       <c r="R16" s="214"/>
@@ -13447,11 +13437,11 @@
       </c>
       <c r="F17" s="230" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -13459,23 +13449,23 @@
       </c>
       <c r="I17" s="233" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="230">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K17" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="230" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="232">
         <f ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13483,7 +13473,7 @@
       </c>
       <c r="O17" s="233" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">IF($C17="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C17,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="123"/>
       <c r="R17" s="214"/>
@@ -13543,11 +13533,11 @@
       </c>
       <c r="F18" s="230" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -13555,27 +13545,27 @@
       </c>
       <c r="I18" s="233" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="230">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K18" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="230" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M18" s="232">
         <f ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="231" t="str">
+        <v>1</v>
+      </c>
+      <c r="N18" s="231">
         <f t="shared" ca="1" si="9"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="O18" s="233" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">IF($C18="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C18,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
@@ -14676,7 +14666,7 @@
       <selection activeCell="AA17" sqref="AA17"/>
       <selection pane="topRight" activeCell="AA17" sqref="AA17"/>
       <selection pane="bottomLeft" activeCell="AA17" sqref="AA17"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19289,20 +19279,20 @@
         <v>Brasil</v>
       </c>
       <c r="CK3" s="191" t="str">
-        <f>Semis!H9</f>
-        <v/>
+        <f ca="1">Semis!H9</f>
+        <v>Argentina</v>
       </c>
       <c r="CL3" s="191" t="str">
-        <f>Semis!N9</f>
-        <v/>
+        <f ca="1">Semis!N9</f>
+        <v>Canadá</v>
       </c>
       <c r="CM3" s="191" t="str">
-        <f>Semis!H12</f>
-        <v/>
+        <f ca="1">Semis!H12</f>
+        <v>Uruguay</v>
       </c>
       <c r="CN3" s="191" t="str">
-        <f>Semis!N12</f>
-        <v/>
+        <f ca="1">Semis!N12</f>
+        <v>Colombia</v>
       </c>
       <c r="CO3" s="191" t="str">
         <f>Final!H15</f>
@@ -19316,53 +19306,53 @@
         <f>Final!H22</f>
         <v/>
       </c>
-      <c r="CR3" s="191" t="str">
+      <c r="CR3" s="191">
         <f ca="1">VLOOKUP(CR2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="CS3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="CS3" s="191">
         <f ca="1">VLOOKUP(CR2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="CT3" s="191" t="str">
         <f t="shared" ref="CT3" ca="1" si="23">IF(OR(CR3="",CS3=""),"",IF(CR3&gt;CS3,1,IF(CR3=CS3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="CU3" s="191" t="str">
+        <v>x</v>
+      </c>
+      <c r="CU3" s="191">
         <f ca="1">VLOOKUP(CU2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="CV3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="CV3" s="191">
         <f ca="1">VLOOKUP(CU2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="CW3" s="191" t="str">
         <f t="shared" ref="CW3" ca="1" si="24">IF(OR(CU3="",CV3=""),"",IF(CU3&gt;CV3,1,IF(CU3=CV3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="CX3" s="191" t="str">
+        <v>x</v>
+      </c>
+      <c r="CX3" s="191">
         <f ca="1">VLOOKUP(CX2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="CY3" s="191" t="str">
+        <v>5</v>
+      </c>
+      <c r="CY3" s="191">
         <f ca="1">VLOOKUP(CX2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="CZ3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="CZ3" s="191">
         <f t="shared" ref="CZ3" ca="1" si="25">IF(OR(CX3="",CY3=""),"",IF(CX3&gt;CY3,1,IF(CX3=CY3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="DA3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="DA3" s="191">
         <f ca="1">VLOOKUP(DA2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="DB3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="DB3" s="191">
         <f ca="1">VLOOKUP(DA2,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="DC3" s="191" t="str">
         <f t="shared" ref="DC3" ca="1" si="26">IF(OR(DA3="",DB3=""),"",IF(DA3&gt;DB3,1,IF(DA3=DB3,"x",2)))</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="DD3" s="191" t="str">
         <f ca="1">VLOOKUP(DD2,Aux!$F:$O,9,0)</f>
@@ -20581,19 +20571,19 @@
         <v>20</v>
       </c>
       <c r="CK7">
-        <f>IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK2)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK2)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL7">
-        <f>IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL2)=1,CL$5,0))</f>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL2)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM7">
-        <f>IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM2)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM2)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN7">
-        <f>IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN2)=1,CN$5,0))</f>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN2)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO7">
@@ -20642,7 +20632,7 @@
       </c>
       <c r="CZ7">
         <f ca="1">IF($B7=0,0,IF(AND(CX$3=TotalApuestas!CX2,Resultado!CY$3=TotalApuestas!CY2),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ2,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA7">
         <f ca="1">IF($B7=0,0,IF(DA$3=TotalApuestas!DA2,DA$5,0))</f>
@@ -20654,7 +20644,7 @@
       </c>
       <c r="DC7">
         <f ca="1">IF($B7=0,0,IF(AND(DA$3=TotalApuestas!DA2,Resultado!DB$3=TotalApuestas!DB2),Resultado!DC$5+VLOOKUP(DC$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DC$3=TotalApuestas!DC2,DC$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DD7">
         <f ca="1">IF($B7=0,0,IF(DD$3=TotalApuestas!DD2,DD$5,0))</f>
@@ -21047,19 +21037,19 @@
         <v>20</v>
       </c>
       <c r="CK8">
-        <f>IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK3)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK3)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL8">
-        <f>IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL3)=1,CL$5,0))</f>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL3)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM8">
-        <f>IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM3)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM3)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN8">
-        <f>IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN3)=1,CN$5,0))</f>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN3)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO8">
@@ -21096,7 +21086,7 @@
       </c>
       <c r="CW8">
         <f ca="1">IF($B8=0,0,IF(AND(CU$3=TotalApuestas!CU3,Resultado!CV$3=TotalApuestas!CV3),Resultado!CW$5+VLOOKUP(CW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CW$3=TotalApuestas!CW3,CW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CX8">
         <f ca="1">IF($B8=0,0,IF(CX$3=TotalApuestas!CX3,CX$5,0))</f>
@@ -21108,7 +21098,7 @@
       </c>
       <c r="CZ8">
         <f ca="1">IF($B8=0,0,IF(AND(CX$3=TotalApuestas!CX3,Resultado!CY$3=TotalApuestas!CY3),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ3,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA8">
         <f ca="1">IF($B8=0,0,IF(DA$3=TotalApuestas!DA3,DA$5,0))</f>
@@ -21513,20 +21503,20 @@
         <v>20</v>
       </c>
       <c r="CK9">
-        <f>IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK4)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK4)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL9">
-        <f>IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL4)=1,CL$5,0))</f>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL4)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM9">
-        <f>IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM4)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM4)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN9">
-        <f>IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN4)=1,CN$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN4)=1,CN$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CO9">
         <f>IF($B9=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO4)=1,CO$5,0))</f>
@@ -21574,7 +21564,7 @@
       </c>
       <c r="CZ9">
         <f ca="1">IF($B9=0,0,IF(AND(CX$3=TotalApuestas!CX4,Resultado!CY$3=TotalApuestas!CY4),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ4,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA9">
         <f ca="1">IF($B9=0,0,IF(DA$3=TotalApuestas!DA4,DA$5,0))</f>
@@ -21979,19 +21969,19 @@
         <v>20</v>
       </c>
       <c r="CK10">
-        <f>IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK5)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK5)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL10">
-        <f>IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL5)=1,CL$5,0))</f>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL5)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM10">
-        <f>IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM5)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM5)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN10">
-        <f>IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN5)=1,CN$5,0))</f>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN5)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO10">
@@ -22016,7 +22006,7 @@
       </c>
       <c r="CT10">
         <f ca="1">IF($B10=0,0,IF(AND(CR$3=TotalApuestas!CR5,Resultado!CS$3=TotalApuestas!CS5),Resultado!CT$5+VLOOKUP(CT$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CT$3=TotalApuestas!CT5,CT$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="CU10">
         <f ca="1">IF($B10=0,0,IF(CU$3=TotalApuestas!CU5,CU$5,0))</f>
@@ -22028,7 +22018,7 @@
       </c>
       <c r="CW10">
         <f ca="1">IF($B10=0,0,IF(AND(CU$3=TotalApuestas!CU5,Resultado!CV$3=TotalApuestas!CV5),Resultado!CW$5+VLOOKUP(CW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CW$3=TotalApuestas!CW5,CW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CX10">
         <f ca="1">IF($B10=0,0,IF(CX$3=TotalApuestas!CX5,CX$5,0))</f>
@@ -22040,7 +22030,7 @@
       </c>
       <c r="CZ10">
         <f ca="1">IF($B10=0,0,IF(AND(CX$3=TotalApuestas!CX5,Resultado!CY$3=TotalApuestas!CY5),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ5,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA10">
         <f ca="1">IF($B10=0,0,IF(DA$3=TotalApuestas!DA5,DA$5,0))</f>
@@ -22445,19 +22435,19 @@
         <v>20</v>
       </c>
       <c r="CK11">
-        <f>IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK6)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK6)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL11">
-        <f>IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL6)=1,CL$5,0))</f>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL6)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM11">
-        <f>IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM6)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM6)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN11">
-        <f>IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN6)=1,CN$5,0))</f>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN6)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO11">
@@ -22494,7 +22484,7 @@
       </c>
       <c r="CW11">
         <f ca="1">IF($B11=0,0,IF(AND(CU$3=TotalApuestas!CU6,Resultado!CV$3=TotalApuestas!CV6),Resultado!CW$5+VLOOKUP(CW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CW$3=TotalApuestas!CW6,CW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CX11">
         <f ca="1">IF($B11=0,0,IF(CX$3=TotalApuestas!CX6,CX$5,0))</f>
@@ -22506,7 +22496,7 @@
       </c>
       <c r="CZ11">
         <f ca="1">IF($B11=0,0,IF(AND(CX$3=TotalApuestas!CX6,Resultado!CY$3=TotalApuestas!CY6),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ6,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA11">
         <f ca="1">IF($B11=0,0,IF(DA$3=TotalApuestas!DA6,DA$5,0))</f>
@@ -22911,19 +22901,19 @@
         <v>20</v>
       </c>
       <c r="CK12">
-        <f>IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK7)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK7)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL12">
-        <f>IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL7)=1,CL$5,0))</f>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL7)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM12">
-        <f>IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM7)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM7)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN12">
-        <f>IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN7)=1,CN$5,0))</f>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN7)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO12">
@@ -22960,7 +22950,7 @@
       </c>
       <c r="CW12">
         <f ca="1">IF($B12=0,0,IF(AND(CU$3=TotalApuestas!CU7,Resultado!CV$3=TotalApuestas!CV7),Resultado!CW$5+VLOOKUP(CW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CW$3=TotalApuestas!CW7,CW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CX12">
         <f ca="1">IF($B12=0,0,IF(CX$3=TotalApuestas!CX7,CX$5,0))</f>
@@ -22972,7 +22962,7 @@
       </c>
       <c r="CZ12">
         <f ca="1">IF($B12=0,0,IF(AND(CX$3=TotalApuestas!CX7,Resultado!CY$3=TotalApuestas!CY7),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ7,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA12">
         <f ca="1">IF($B12=0,0,IF(DA$3=TotalApuestas!DA7,DA$5,0))</f>
@@ -23377,20 +23367,20 @@
         <v>20</v>
       </c>
       <c r="CK13">
-        <f>IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK8)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK8)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL13">
-        <f>IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL8)=1,CL$5,0))</f>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL8)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM13">
-        <f>IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM8)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM8)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN13">
-        <f>IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN8)=1,CN$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN8)=1,CN$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CO13">
         <f>IF($B13=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO8)=1,CO$5,0))</f>
@@ -23438,7 +23428,7 @@
       </c>
       <c r="CZ13">
         <f ca="1">IF($B13=0,0,IF(AND(CX$3=TotalApuestas!CX8,Resultado!CY$3=TotalApuestas!CY8),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ8,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA13">
         <f ca="1">IF($B13=0,0,IF(DA$3=TotalApuestas!DA8,DA$5,0))</f>
@@ -23843,19 +23833,19 @@
         <v>20</v>
       </c>
       <c r="CK14">
-        <f>IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK9)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK9)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL14">
-        <f>IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL9)=1,CL$5,0))</f>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL9)=1,CL$5,0))</f>
         <v>0</v>
       </c>
       <c r="CM14">
-        <f>IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM9)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM9)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN14">
-        <f>IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN9)=1,CN$5,0))</f>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN9)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO14">
@@ -23904,7 +23894,7 @@
       </c>
       <c r="CZ14">
         <f ca="1">IF($B14=0,0,IF(AND(CX$3=TotalApuestas!CX9,Resultado!CY$3=TotalApuestas!CY9),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ9,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA14">
         <f ca="1">IF($B14=0,0,IF(DA$3=TotalApuestas!DA9,DA$5,0))</f>
@@ -24309,19 +24299,19 @@
         <v>20</v>
       </c>
       <c r="CK15">
-        <f>IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK10)=1,CK$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CK10)=1,CK$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CL15">
-        <f>IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL10)=1,CL$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CL10)=1,CL$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CM15">
-        <f>IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM10)=1,CM$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CM10)=1,CM$5,0))</f>
+        <v>25</v>
       </c>
       <c r="CN15">
-        <f>IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN10)=1,CN$5,0))</f>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CK$3:$CN$3,TotalApuestas!CN10)=1,CN$5,0))</f>
         <v>0</v>
       </c>
       <c r="CO15">
@@ -24358,7 +24348,7 @@
       </c>
       <c r="CW15">
         <f ca="1">IF($B15=0,0,IF(AND(CU$3=TotalApuestas!CU10,Resultado!CV$3=TotalApuestas!CV10),Resultado!CW$5+VLOOKUP(CW$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CW$3=TotalApuestas!CW10,CW$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CX15">
         <f ca="1">IF($B15=0,0,IF(CX$3=TotalApuestas!CX10,CX$5,0))</f>
@@ -24370,7 +24360,7 @@
       </c>
       <c r="CZ15">
         <f ca="1">IF($B15=0,0,IF(AND(CX$3=TotalApuestas!CX10,Resultado!CY$3=TotalApuestas!CY10),Resultado!CZ$5+VLOOKUP(CZ$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(CZ$3=TotalApuestas!CZ10,CZ$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DA15">
         <f ca="1">IF($B15=0,0,IF(DA$3=TotalApuestas!DA10,DA$5,0))</f>
@@ -41578,20 +41568,20 @@
         <v>Brasil</v>
       </c>
       <c r="CK1" s="84" t="str">
-        <f>+Resultado!CK3</f>
-        <v/>
+        <f ca="1">+Resultado!CK3</f>
+        <v>Argentina</v>
       </c>
       <c r="CL1" s="84" t="str">
-        <f>+Resultado!CL3</f>
-        <v/>
+        <f ca="1">+Resultado!CL3</f>
+        <v>Canadá</v>
       </c>
       <c r="CM1" s="84" t="str">
-        <f>+Resultado!CM3</f>
-        <v/>
+        <f ca="1">+Resultado!CM3</f>
+        <v>Uruguay</v>
       </c>
       <c r="CN1" s="84" t="str">
-        <f>+Resultado!CN3</f>
-        <v/>
+        <f ca="1">+Resultado!CN3</f>
+        <v>Colombia</v>
       </c>
       <c r="CO1" s="84" t="str">
         <f>+Resultado!CO3</f>
@@ -41605,53 +41595,53 @@
         <f>+Resultado!CQ3</f>
         <v/>
       </c>
-      <c r="CR1" s="84" t="str">
+      <c r="CR1" s="84">
         <f ca="1">+Resultado!CR3</f>
-        <v/>
-      </c>
-      <c r="CS1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="CS1" s="84">
         <f ca="1">+Resultado!CS3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="CT1" s="84" t="str">
         <f ca="1">+Resultado!CT3</f>
-        <v/>
-      </c>
-      <c r="CU1" s="84" t="str">
+        <v>x</v>
+      </c>
+      <c r="CU1" s="84">
         <f ca="1">+Resultado!CU3</f>
-        <v/>
-      </c>
-      <c r="CV1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="CV1" s="84">
         <f ca="1">+Resultado!CV3</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="CW1" s="84" t="str">
         <f ca="1">+Resultado!CW3</f>
-        <v/>
-      </c>
-      <c r="CX1" s="84" t="str">
+        <v>x</v>
+      </c>
+      <c r="CX1" s="84">
         <f ca="1">+Resultado!CX3</f>
-        <v/>
-      </c>
-      <c r="CY1" s="84" t="str">
+        <v>5</v>
+      </c>
+      <c r="CY1" s="84">
         <f ca="1">+Resultado!CY3</f>
-        <v/>
-      </c>
-      <c r="CZ1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="CZ1" s="84">
         <f ca="1">+Resultado!CZ3</f>
-        <v/>
-      </c>
-      <c r="DA1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="DA1" s="84">
         <f ca="1">+Resultado!DA3</f>
-        <v/>
-      </c>
-      <c r="DB1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="DB1" s="84">
         <f ca="1">+Resultado!DB3</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="DC1" s="84" t="str">
         <f ca="1">+Resultado!DC3</f>
-        <v/>
+        <v>x</v>
       </c>
       <c r="DD1" s="84" t="str">
         <f ca="1">+Resultado!DD3</f>
@@ -48177,7 +48167,7 @@
   <dimension ref="A7:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48278,11 +48268,15 @@
         <v>Argentina</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="16">
+        <v>1</v>
+      </c>
       <c r="K9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="16"/>
+      <c r="L9" s="16">
+        <v>1</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="N9" ca="1">INDIRECT(RIGHT(B9,1)&amp;"!P"&amp;7+LEFT(B9,1)*2)</f>
@@ -48298,8 +48292,8 @@
         <v>NRG Stadium - HOUSTON, TX</v>
       </c>
       <c r="S9" s="18" t="str">
-        <f>IF(OR(J9="",L9=""),"",IF(J9&gt;L9,H9,IF(J9&lt;L9,N9,IF(OR(J10="",L10=""),"",IF(J10&gt;L10,H9,N9)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J9="",L9=""),"",IF(J9&gt;L9,H9,IF(J9&lt;L9,N9,IF(OR(J10="",L10=""),"",IF(J10&gt;L10,H9,N9)))))</f>
+        <v>Argentina</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48312,11 +48306,15 @@
         <v>51</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9">
+        <v>4</v>
+      </c>
       <c r="K10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="9"/>
+      <c r="L10" s="9">
+        <v>2</v>
+      </c>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
@@ -48371,11 +48369,15 @@
         <v>Venezuela</v>
       </c>
       <c r="I12" s="25"/>
-      <c r="J12" s="16"/>
+      <c r="J12" s="16">
+        <v>1</v>
+      </c>
       <c r="K12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="L12" s="16">
+        <v>1</v>
+      </c>
       <c r="M12" s="6"/>
       <c r="N12" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="N12" ca="1">INDIRECT(RIGHT(B12,1)&amp;"!P"&amp;7+LEFT(B12,1)*2)</f>
@@ -48391,8 +48393,8 @@
         <v>AT&amp;T Stadium - ARLINGTON, TX</v>
       </c>
       <c r="S12" s="18" t="str">
-        <f>IF(OR(J12="",L12=""),"",IF(J12&gt;L12,H12,IF(J12&lt;L12,N12,IF(OR(J13="",L13=""),"",IF(J13&gt;L13,H12,N12)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J12="",L12=""),"",IF(J12&gt;L12,H12,IF(J12&lt;L12,N12,IF(OR(J13="",L13=""),"",IF(J13&gt;L13,H12,N12)))))</f>
+        <v>Canadá</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48405,11 +48407,15 @@
         <v>51</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9">
+        <v>3</v>
+      </c>
       <c r="K13" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="9"/>
+      <c r="L13" s="9">
+        <v>4</v>
+      </c>
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
@@ -48464,11 +48470,15 @@
         <v>Colombia</v>
       </c>
       <c r="I15" s="25"/>
-      <c r="J15" s="16"/>
+      <c r="J15" s="16">
+        <v>5</v>
+      </c>
       <c r="K15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="16"/>
+      <c r="L15" s="16">
+        <v>0</v>
+      </c>
       <c r="M15" s="6"/>
       <c r="N15" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="N15" ca="1">INDIRECT(RIGHT(B15,1)&amp;"!P"&amp;7+LEFT(B15,1)*2)</f>
@@ -48484,8 +48494,8 @@
         <v>Allegiant Stadium - LAS VEGAS, NV</v>
       </c>
       <c r="S15" s="18" t="str">
-        <f>IF(OR(J15="",L15=""),"",IF(J15&gt;L15,H15,IF(J15&lt;L15,N15,IF(OR(J16="",L16=""),"",IF(J16&gt;L16,H15,N15)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J15="",L15=""),"",IF(J15&gt;L15,H15,IF(J15&lt;L15,N15,IF(OR(J16="",L16=""),"",IF(J16&gt;L16,H15,N15)))))</f>
+        <v>Colombia</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48557,11 +48567,15 @@
         <v>Uruguay</v>
       </c>
       <c r="I18" s="25"/>
-      <c r="J18" s="16"/>
+      <c r="J18" s="16">
+        <v>0</v>
+      </c>
       <c r="K18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="16">
+        <v>0</v>
+      </c>
       <c r="M18" s="6"/>
       <c r="N18" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="N18" ca="1">INDIRECT(RIGHT(B18,1)&amp;"!P"&amp;7+LEFT(B18,1)*2)</f>
@@ -48577,8 +48591,8 @@
         <v>State Farm Stadium - GLENDALE, AZ</v>
       </c>
       <c r="S18" s="18" t="str">
-        <f>IF(OR(J18="",L18=""),"",IF(J18&gt;L18,H18,IF(J18&lt;L18,N18,IF(OR(J19="",L19=""),"",IF(J19&gt;L19,H18,N18)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J18="",L18=""),"",IF(J18&gt;L18,H18,IF(J18&lt;L18,N18,IF(OR(J19="",L19=""),"",IF(J19&gt;L19,H18,N18)))))</f>
+        <v>Uruguay</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48591,11 +48605,15 @@
         <v>51</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9">
+        <v>4</v>
+      </c>
       <c r="K19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="9"/>
+      <c r="L19" s="9">
+        <v>2</v>
+      </c>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
@@ -48880,13 +48898,13 @@
         <v>45482.833333333336</v>
       </c>
       <c r="F9" s="180"/>
-      <c r="G9" s="180" t="str">
-        <f>IFERROR(VLOOKUP(H9,Aux!$A:$C,3,0),"")</f>
-        <v/>
+      <c r="G9" s="180" t="e" vm="1">
+        <f ca="1">IFERROR(VLOOKUP(H9,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H9" s="7" t="str">
-        <f>+Cuartos!S9</f>
-        <v/>
+        <f ca="1">+Cuartos!S9</f>
+        <v>Argentina</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="16"/>
@@ -48896,12 +48914,12 @@
       <c r="L9" s="16"/>
       <c r="M9" s="6"/>
       <c r="N9" s="17" t="str">
-        <f>+Cuartos!S12</f>
-        <v/>
-      </c>
-      <c r="O9" s="180" t="str">
-        <f>IFERROR(VLOOKUP(N9,Aux!$A:$C,3,0),"")</f>
-        <v/>
+        <f ca="1">+Cuartos!S12</f>
+        <v>Canadá</v>
+      </c>
+      <c r="O9" s="180" t="e" vm="2">
+        <f ca="1">IFERROR(VLOOKUP(N9,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="175" t="str">
@@ -48967,13 +48985,13 @@
         <v>45483.833333333336</v>
       </c>
       <c r="F12" s="180"/>
-      <c r="G12" s="180" t="str">
-        <f>IFERROR(VLOOKUP(H12,Aux!$A:$C,3,0),"")</f>
-        <v/>
+      <c r="G12" s="180" t="e" vm="11">
+        <f ca="1">IFERROR(VLOOKUP(H12,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H12" s="7" t="str">
-        <f>+Cuartos!S18</f>
-        <v/>
+        <f ca="1">+Cuartos!S18</f>
+        <v>Uruguay</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="16"/>
@@ -48983,12 +49001,12 @@
       <c r="L12" s="16"/>
       <c r="M12" s="6"/>
       <c r="N12" s="17" t="str">
-        <f>+Cuartos!S15</f>
-        <v/>
-      </c>
-      <c r="O12" s="180" t="str">
-        <f>IFERROR(VLOOKUP(N12,Aux!$A:$C,3,0),"")</f>
-        <v/>
+        <f ca="1">+Cuartos!S15</f>
+        <v>Colombia</v>
+      </c>
+      <c r="O12" s="180" t="e" vm="13">
+        <f ca="1">IFERROR(VLOOKUP(N12,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="P12" s="17"/>
       <c r="Q12" s="175" t="str">
@@ -51090,13 +51108,13 @@
       <c r="M26" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="68" t="str">
+      <c r="N26" s="68">
         <f ca="1">IF(VLOOKUP(F26,INDIRECT(M26&amp;"!C:M"),8,0)="","",VLOOKUP(F26,INDIRECT(M26&amp;"!C:M"),8,0))</f>
-        <v/>
-      </c>
-      <c r="O26" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="O26" s="68">
         <f ca="1">IF(VLOOKUP(F26,INDIRECT(M26&amp;"!C:M"),10,0)="","",VLOOKUP(F26,INDIRECT(M26&amp;"!C:M"),10,0))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="2"/>
@@ -51128,13 +51146,13 @@
       <c r="M27" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="68" t="str">
+      <c r="N27" s="68">
         <f t="shared" ref="N27:N33" ca="1" si="4">IF(VLOOKUP(F27,INDIRECT(M27&amp;"!C:M"),8,0)="","",VLOOKUP(F27,INDIRECT(M27&amp;"!C:M"),8,0))</f>
-        <v/>
-      </c>
-      <c r="O27" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="O27" s="68">
         <f t="shared" ref="O27:O33" ca="1" si="5">IF(VLOOKUP(F27,INDIRECT(M27&amp;"!C:M"),10,0)="","",VLOOKUP(F27,INDIRECT(M27&amp;"!C:M"),10,0))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="2"/>
@@ -51165,13 +51183,13 @@
       <c r="M28" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="N28" s="68" t="str">
+      <c r="N28" s="68">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O28" s="68" t="str">
+        <v>5</v>
+      </c>
+      <c r="O28" s="68">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="2"/>
@@ -51202,13 +51220,13 @@
       <c r="M29" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="N29" s="68" t="str">
+      <c r="N29" s="68">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O29" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O29" s="68">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="2"/>

</xml_diff>

<commit_message>
final de las semis
</commit_message>
<xml_diff>
--- a/Main.xlsx
+++ b/Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leine\Documentos\QUINIELA-VENECA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCE558-BFCB-47BB-ADBC-7AD0D02E3494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD308069-27DE-4651-AF0E-C51D7C7041AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" firstSheet="6" activeTab="10" xr2:uid="{A1A07F19-1258-4827-8AF7-173CDFEC396E}"/>
   </bookViews>
   <sheets>
     <sheet name="Normas" sheetId="23" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B88681C-FA4B-4A27-91BB-760B20935DE2}">
   <dimension ref="C1:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -9929,23 +9929,23 @@
       </c>
       <c r="K5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:K4),0))</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="L5" s="127">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:L4),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M5" s="128">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:M4),0))</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N5" s="129">
         <f ca="1">+IF($D5=0,"",VLOOKUP($C5,$Q:$AB,COLUMNS($C$4:N4),0))</f>
-        <v>375.01100000000002</v>
+        <v>415.01100000000002</v>
       </c>
       <c r="P5" s="196">
         <f ca="1">IFERROR(M5-ROW()/10000,"")</f>
-        <v>79.999499999999998</v>
+        <v>119.9995</v>
       </c>
       <c r="Q5" s="119">
         <f t="shared" ref="Q5:Q26" ca="1" si="0">+_xlfn.RANK.EQ(AB5,$AB$5:$AB$26)</f>
@@ -9981,19 +9981,19 @@
       </c>
       <c r="Y5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="Z5" s="120">
         <f ca="1">+SUMIFS(Resultado!7:7,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA5" s="122">
         <f t="shared" ref="AA5:AA26" ca="1" si="2">+SUM(X5:Z5)</f>
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="AB5" s="121">
         <f t="shared" ref="AB5:AB26" ca="1" si="3">+IF(R5=0,0+ROW()/10000,AA5+W5+ROW()/1000)</f>
-        <v>295.005</v>
+        <v>335.005</v>
       </c>
     </row>
     <row r="6" spans="3:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10003,51 +10003,51 @@
       </c>
       <c r="D6" s="151" t="str">
         <f ca="1">+VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:D5),0)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="E6" s="197">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:E5),0))</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:F5),0))</f>
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:G5),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H6" s="198">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:H5),0))</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I6" s="200">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:I5),0))</f>
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="J6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:J5),0))</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:K5),0))</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="L6" s="127">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:L5),0))</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M6" s="128">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:M5),0))</f>
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="N6" s="129">
         <f ca="1">+IF($D6=0,"",VLOOKUP($C6,$Q:$AB,COLUMNS($C$4:N5),0))</f>
-        <v>345.01299999999998</v>
+        <v>415.00700000000001</v>
       </c>
       <c r="P6" s="196">
         <f t="shared" ref="P6:P26" ca="1" si="5">IFERROR(M6-ROW()/10000,"")</f>
-        <v>89.999399999999994</v>
+        <v>149.99940000000001</v>
       </c>
       <c r="Q6" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10083,19 +10083,19 @@
       </c>
       <c r="Y6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="Z6" s="120">
         <f ca="1">+SUMIFS(Resultado!8:8,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA6" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="AB6" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>300.00599999999997</v>
+        <v>335.00599999999997</v>
       </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
@@ -10105,55 +10105,55 @@
       </c>
       <c r="D7" s="151" t="str">
         <f ca="1">+VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:D6),0)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="E7" s="197">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:E6),0))</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:F6),0))</f>
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:G6),0))</f>
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H7" s="198">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:H6),0))</f>
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I7" s="200">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:I6),0))</f>
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="J7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:J6),0))</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:K6),0))</f>
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="L7" s="127">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:L6),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M7" s="128">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:M6),0))</f>
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="N7" s="129">
         <f ca="1">+IF($D7=0,"",VLOOKUP($C7,$Q:$AB,COLUMNS($C$4:N6),0))</f>
-        <v>345.012</v>
+        <v>385.01299999999998</v>
       </c>
       <c r="P7" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>54.999299999999998</v>
+        <v>129.99930000000001</v>
       </c>
       <c r="Q7" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R7" s="126" t="str">
         <f>Resultado!B9</f>
@@ -10185,19 +10185,19 @@
       </c>
       <c r="Y7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Z7" s="120">
         <f ca="1">+SUMIFS(Resultado!9:9,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AA7" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="AB7" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>345.00700000000001</v>
+        <v>415.00700000000001</v>
       </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
@@ -10207,55 +10207,55 @@
       </c>
       <c r="D8" s="152" t="str">
         <f ca="1">+VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:D7),0)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="E8" s="201">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:E7),0))</f>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:F7),0))</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:G7),0))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H8" s="202">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:H7),0))</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I8" s="203">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:I7),0))</f>
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="J8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:J7),0))</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:K7),0))</f>
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="L8" s="130">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:L7),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M8" s="131">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:M7),0))</f>
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="N8" s="132">
         <f ca="1">+IF($D8=0,"",VLOOKUP($C8,$Q:$AB,COLUMNS($C$4:N7),0))</f>
-        <v>345.00700000000001</v>
+        <v>375.00799999999998</v>
       </c>
       <c r="P8" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>79.999200000000002</v>
+        <v>104.9992</v>
       </c>
       <c r="Q8" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R8" s="126" t="str">
         <f>Resultado!B10</f>
@@ -10287,19 +10287,19 @@
       </c>
       <c r="Y8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="Z8" s="120">
         <f ca="1">+SUMIFS(Resultado!10:10,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA8" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="AB8" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>340.00799999999998</v>
+        <v>375.00799999999998</v>
       </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
@@ -10309,55 +10309,55 @@
       </c>
       <c r="D9" s="153" t="str">
         <f ca="1">+VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:D8),0)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="E9" s="204">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:E8),0))</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="F9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:F8),0))</f>
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:G8),0))</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H9" s="205">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:H8),0))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I9" s="206">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:I8),0))</f>
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="J9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:J8),0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:K8),0))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L9" s="133">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:L8),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M9" s="134">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:M8),0))</f>
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="N9" s="135">
         <f ca="1">+IF($D9=0,"",VLOOKUP($C9,$Q:$AB,COLUMNS($C$4:N8),0))</f>
-        <v>340.00799999999998</v>
+        <v>365.01</v>
       </c>
       <c r="P9" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>69.999099999999999</v>
+        <v>104.9991</v>
       </c>
       <c r="Q9" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R9" s="126" t="str">
         <f>Resultado!B11</f>
@@ -10389,19 +10389,19 @@
       </c>
       <c r="Y9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="Z9" s="120">
         <f ca="1">+SUMIFS(Resultado!11:11,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA9" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="AB9" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>315.00900000000001</v>
+        <v>350.00900000000001</v>
       </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
@@ -10411,19 +10411,19 @@
       </c>
       <c r="D10" s="151" t="str">
         <f ca="1">+VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:D9),0)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="E10" s="197">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:E9),0))</f>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:F9),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:G9),0))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H10" s="198">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:H9),0))</f>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="I10" s="200">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:I9),0))</f>
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="J10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:J9),0))</f>
@@ -10439,27 +10439,27 @@
       </c>
       <c r="K10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:K9),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L10" s="127">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:L9),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M10" s="128">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:M9),0))</f>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="N10" s="129">
         <f ca="1">+IF($D10=0,"",VLOOKUP($C10,$Q:$AB,COLUMNS($C$4:N9),0))</f>
-        <v>325.01</v>
+        <v>350.00900000000001</v>
       </c>
       <c r="P10" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>64.998999999999995</v>
+        <v>99.998999999999995</v>
       </c>
       <c r="Q10" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R10" s="126" t="str">
         <f>Resultado!B12</f>
@@ -10491,19 +10491,19 @@
       </c>
       <c r="Y10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="Z10" s="120">
         <f ca="1">+SUMIFS(Resultado!12:12,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA10" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="AB10" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>325.01</v>
+        <v>365.01</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
@@ -10513,31 +10513,31 @@
       </c>
       <c r="D11" s="151" t="str">
         <f ca="1">+VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:D10),0)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="E11" s="197">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:E10),0))</f>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:F10),0))</f>
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:G10),0))</f>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H11" s="198">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:H10),0))</f>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I11" s="200">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:I10),0))</f>
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="J11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:J10),0))</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K11" s="127">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:K10),0))</f>
@@ -10549,15 +10549,15 @@
       </c>
       <c r="M11" s="128">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:M10),0))</f>
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="N11" s="129">
         <f ca="1">+IF($D11=0,"",VLOOKUP($C11,$Q:$AB,COLUMNS($C$4:N10),0))</f>
-        <v>315.00900000000001</v>
+        <v>345.012</v>
       </c>
       <c r="P11" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>64.998900000000006</v>
+        <v>54.998899999999999</v>
       </c>
       <c r="Q11" s="119">
         <f t="shared" ca="1" si="0"/>
@@ -10593,19 +10593,19 @@
       </c>
       <c r="Y11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Z11" s="120">
         <f ca="1">+SUMIFS(Resultado!13:13,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA11" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="AB11" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>375.01100000000002</v>
+        <v>415.01100000000002</v>
       </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
@@ -10643,27 +10643,27 @@
       </c>
       <c r="K12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:K11),0))</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L12" s="127">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:L11),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M12" s="128">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:M11),0))</f>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="N12" s="129">
         <f ca="1">+IF($D12=0,"",VLOOKUP($C12,$Q:$AB,COLUMNS($C$4:N11),0))</f>
-        <v>300.00599999999997</v>
+        <v>335.00599999999997</v>
       </c>
       <c r="P12" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>64.998800000000003</v>
+        <v>99.998800000000003</v>
       </c>
       <c r="Q12" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R12" s="126" t="str">
         <f>Resultado!B14</f>
@@ -10745,27 +10745,27 @@
       </c>
       <c r="K13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:K12),0))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L13" s="130">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:L12),0))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M13" s="131">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:M12),0))</f>
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="N13" s="132">
         <f ca="1">+IF($D13=0,"",VLOOKUP($C13,$Q:$AB,COLUMNS($C$4:N12),0))</f>
-        <v>295.005</v>
+        <v>335.005</v>
       </c>
       <c r="P13" s="196">
         <f t="shared" ca="1" si="5"/>
-        <v>64.998699999999999</v>
+        <v>104.9987</v>
       </c>
       <c r="Q13" s="119">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R13" s="126" t="str">
         <f>Resultado!B15</f>
@@ -10797,19 +10797,19 @@
       </c>
       <c r="Y13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!Y$4)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="Z13" s="120">
         <f ca="1">+SUMIFS(Resultado!15:15,Resultado!$1:$1,ClasificaciónPorra!Z$4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AA13" s="122">
         <f t="shared" ca="1" si="2"/>
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="AB13" s="121">
         <f t="shared" ca="1" si="3"/>
-        <v>345.01299999999998</v>
+        <v>385.01299999999998</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
@@ -12232,7 +12232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC332C9-1E43-4D20-B8E8-89E7F565F63E}">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
@@ -12572,7 +12572,7 @@
       <c r="R7" s="214"/>
       <c r="S7" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="T7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">IF(OR(T$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12580,11 +12580,11 @@
       </c>
       <c r="U7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U7" ca="1">IF(OR(U$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Colombia</v>
       </c>
       <c r="V7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V7" ca="1">IF(OR(V$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Uruguay</v>
+        <v>Colombia</v>
       </c>
       <c r="W7" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">IF(OR(W$5="",$S7=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S7,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
@@ -12615,29 +12615,29 @@
       <c r="C8" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="221" t="str">
+      <c r="D8" s="221">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="E8" s="222" t="str">
+        <v>2</v>
+      </c>
+      <c r="E8" s="222">
         <f ca="1">+IF(D8="","",IF(D8&gt;F8,1,IF(D8=F8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="F8" s="223" t="str">
+        <v>1</v>
+      </c>
+      <c r="F8" s="223">
         <f ca="1">VLOOKUP(D1,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="G8" s="221" t="str">
+        <v>0</v>
+      </c>
+      <c r="G8" s="221">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="H8" s="222" t="str">
+        <v>0</v>
+      </c>
+      <c r="H8" s="222">
         <f ca="1">+IF(G8="","",IF(G8&gt;I8,1,IF(G8=I8,"X",2)))</f>
-        <v/>
-      </c>
-      <c r="I8" s="223" t="str">
+        <v>2</v>
+      </c>
+      <c r="I8" s="223">
         <f ca="1">VLOOKUP(G1,Aux!$F:$O,10,0)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J8" s="221" t="str">
         <f ca="1">VLOOKUP(J1,Aux!$F:$O,9,0)</f>
@@ -12667,11 +12667,11 @@
       <c r="R8" s="214"/>
       <c r="S8" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="T8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">IF(OR(T$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
-        <v>Venezuela</v>
+        <v>Argentina</v>
       </c>
       <c r="U8" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(OR(U$5="",$S8=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S8,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
@@ -12711,7 +12711,7 @@
       <c r="R9" s="214"/>
       <c r="S9" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="T9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">IF(OR(T$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12719,11 +12719,11 @@
       </c>
       <c r="U9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U9" ca="1">IF(OR(U$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="V9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V9" ca="1">IF(OR(V$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="W9" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">IF(OR(W$5="",$S9=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S9,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
@@ -12807,7 +12807,7 @@
       <c r="R10" s="214"/>
       <c r="S10" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="T10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">IF(OR(T$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12815,11 +12815,11 @@
       </c>
       <c r="U10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(OR(U$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Uruguay</v>
       </c>
       <c r="V10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(OR(V$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:V$1)-1),0))</f>
-        <v>Brasil</v>
+        <v>Uruguay</v>
       </c>
       <c r="W10" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(OR(W$5="",$S10=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S10,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:W$1)-1),0))</f>
@@ -12849,11 +12849,11 @@
       <c r="B11" s="214"/>
       <c r="C11" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D6=0,"",ClasificaciónPorra!D6)</f>
-        <v>Moises</v>
+        <v xml:space="preserve">  German Rodriguez</v>
       </c>
       <c r="D11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="231">
         <f t="shared" ref="E11:E29" ca="1" si="6">+IF(D11="","",IF(D11&gt;F11,1,IF(D11=F11,"X",2)))</f>
@@ -12865,19 +12865,19 @@
       </c>
       <c r="G11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="231">
         <f t="shared" ref="H11:H29" ca="1" si="7">+IF(G11="","",IF(G11&gt;I11,1,IF(G11=I11,"X",2)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="233" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J11" s="230">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="231">
         <f t="shared" ref="K11:K29" ca="1" si="8">+IF(J11="","",IF(J11&gt;L11,1,IF(J11=L11,"X",2)))</f>
@@ -12885,11 +12885,11 @@
       </c>
       <c r="L11" s="230" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="232">
         <f ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="231">
         <f t="shared" ref="N11:N29" ca="1" si="9">+IF(M11="","",IF(M11&gt;O11,1,IF(M11=O11,"X",2)))</f>
@@ -12897,13 +12897,13 @@
       </c>
       <c r="O11" s="233" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">IF($C11="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C11,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="123"/>
       <c r="R11" s="214"/>
       <c r="S11" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="T11" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">IF(OR(T$5="",$S11=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S11,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
@@ -12945,23 +12945,23 @@
       <c r="B12" s="214"/>
       <c r="C12" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D7=0,"",ClasificaciónPorra!D7)</f>
-        <v xml:space="preserve">Luis Rondón </v>
+        <v>Moises</v>
       </c>
       <c r="D12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="230" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -12969,19 +12969,19 @@
       </c>
       <c r="I12" s="233" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="230">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="230" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="232">
         <f ca="1">IF($C12="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C12,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -12999,11 +12999,11 @@
       <c r="R12" s="214"/>
       <c r="S12" s="218" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="T12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">IF(OR(T$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:T$1)-1),0))</f>
-        <v>Argentina</v>
+        <v>Venezuela</v>
       </c>
       <c r="U12" s="171" t="str" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">IF(OR(U$5="",$S12=""),"",IFERROR(INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$S12,TotalApuestas!$B$1:$B$50000,0),MATCH("Equipos"&amp;Seguimiento!$S$1,Resultado!$4:$4,0)+COLUMNS($T$1:U$1)-1),0))</f>
@@ -13041,11 +13041,11 @@
       <c r="B13" s="214"/>
       <c r="C13" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D8=0,"",ClasificaciónPorra!D8)</f>
-        <v xml:space="preserve">  German Rodriguez</v>
+        <v>ISAAC BERMUDEZ</v>
       </c>
       <c r="D13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13053,31 +13053,31 @@
       </c>
       <c r="F13" s="230" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
         <v>2</v>
       </c>
-      <c r="H13" s="231">
+      <c r="H13" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="I13" s="233" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" s="230">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="230" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M13" s="232">
         <f ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -13089,7 +13089,7 @@
       </c>
       <c r="O13" s="233" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">IF($C13="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C13,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="123"/>
       <c r="R13" s="214"/>
@@ -13137,11 +13137,11 @@
       <c r="B14" s="214"/>
       <c r="C14" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D9=0,"",ClasificaciónPorra!D9)</f>
-        <v>ISAAC BERMUDEZ</v>
+        <v>Juan Diego De Abreu</v>
       </c>
       <c r="D14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13149,11 +13149,11 @@
       </c>
       <c r="F14" s="230" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="231" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -13161,7 +13161,7 @@
       </c>
       <c r="I14" s="233" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="230">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
@@ -13177,7 +13177,7 @@
       </c>
       <c r="M14" s="232">
         <f ca="1">IF($C14="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C14,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="231">
         <f t="shared" ca="1" si="9"/>
@@ -13233,11 +13233,11 @@
       <c r="B15" s="214"/>
       <c r="C15" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D10=0,"",ClasificaciónPorra!D10)</f>
-        <v>Juan Diego De Abreu</v>
+        <v>YUTA</v>
       </c>
       <c r="D15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="231">
         <f t="shared" ca="1" si="6"/>
@@ -13249,27 +13249,27 @@
       </c>
       <c r="G15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="H15" s="231" t="str">
+        <v>3</v>
+      </c>
+      <c r="H15" s="231">
         <f t="shared" ca="1" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="I15" s="233" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="230">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="230" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="232">
         <f ca="1">IF($C15="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C15,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -13329,23 +13329,23 @@
       <c r="B16" s="214"/>
       <c r="C16" s="229" t="str">
         <f ca="1">IF(ClasificaciónPorra!D11=0,"",ClasificaciónPorra!D11)</f>
-        <v>YUTA</v>
+        <v xml:space="preserve">Luis Rondón </v>
       </c>
       <c r="D16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="231">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="230" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!D$1,Resultado!$2:$2,0)+1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="231">
         <f t="shared" ca="1" si="7"/>
@@ -13353,19 +13353,19 @@
       </c>
       <c r="I16" s="233" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!G$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="230">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="231">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" s="230" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!J$1,Resultado!$2:$2,0)+1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M16" s="232">
         <f ca="1">IF($C16="","",INDEX(TotalApuestas!$A$1:$GL$50000,MATCH(Seguimiento!$C16,TotalApuestas!$B$1:$B$50000,0),MATCH(Seguimiento!M$1,Resultado!$2:$2,0)))</f>
@@ -19295,12 +19295,12 @@
         <v>Colombia</v>
       </c>
       <c r="CO3" s="191" t="str">
-        <f>Final!H15</f>
-        <v/>
+        <f ca="1">Final!H15</f>
+        <v>Argentina</v>
       </c>
       <c r="CP3" s="191" t="str">
-        <f>Final!N15</f>
-        <v/>
+        <f ca="1">Final!N15</f>
+        <v>Colombia</v>
       </c>
       <c r="CQ3" s="191" t="str">
         <f>Final!H22</f>
@@ -19354,29 +19354,29 @@
         <f t="shared" ref="DC3" ca="1" si="26">IF(OR(DA3="",DB3=""),"",IF(DA3&gt;DB3,1,IF(DA3=DB3,"x",2)))</f>
         <v>x</v>
       </c>
-      <c r="DD3" s="191" t="str">
+      <c r="DD3" s="191">
         <f ca="1">VLOOKUP(DD2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="DE3" s="191" t="str">
+        <v>2</v>
+      </c>
+      <c r="DE3" s="191">
         <f ca="1">VLOOKUP(DD2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="DF3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="191">
         <f t="shared" ref="DF3" ca="1" si="27">IF(OR(DD3="",DE3=""),"",IF(DD3&gt;DE3,1,IF(DD3=DE3,"x",2)))</f>
-        <v/>
-      </c>
-      <c r="DG3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="DG3" s="191">
         <f ca="1">VLOOKUP(DG2,Aux!$F:$O,9,0)</f>
-        <v/>
-      </c>
-      <c r="DH3" s="191" t="str">
+        <v>0</v>
+      </c>
+      <c r="DH3" s="191">
         <f ca="1">VLOOKUP(DG2,Aux!$F:$O,10,0)</f>
-        <v/>
-      </c>
-      <c r="DI3" s="191" t="str">
+        <v>1</v>
+      </c>
+      <c r="DI3" s="191">
         <f t="shared" ref="DI3" ca="1" si="28">IF(OR(DG3="",DH3=""),"",IF(DG3&gt;DH3,1,IF(DG3=DH3,"x",2)))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="DJ3" s="191" t="str">
         <f ca="1">VLOOKUP(DJ2,Aux!$F:$O,9,0)</f>
@@ -20587,11 +20587,11 @@
         <v>0</v>
       </c>
       <c r="CO7">
-        <f>IF($B7=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO2)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO2)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP7">
-        <f>IF($B7=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP2)=1,CP$5,0))</f>
+        <f ca="1">IF($B7=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP2)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ7">
@@ -20656,7 +20656,7 @@
       </c>
       <c r="DF7">
         <f ca="1">IF($B7=0,0,IF(AND(DD$3=TotalApuestas!DD2,Resultado!DE$3=TotalApuestas!DE2),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF2,DF$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DG7">
         <f ca="1">IF($B7=0,0,IF(DG$3=TotalApuestas!DG2,DG$5,0))</f>
@@ -21053,11 +21053,11 @@
         <v>0</v>
       </c>
       <c r="CO8">
-        <f>IF($B8=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO3)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO3)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP8">
-        <f>IF($B8=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP3)=1,CP$5,0))</f>
+        <f ca="1">IF($B8=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP3)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ8">
@@ -21122,7 +21122,7 @@
       </c>
       <c r="DF8">
         <f ca="1">IF($B8=0,0,IF(AND(DD$3=TotalApuestas!DD3,Resultado!DE$3=TotalApuestas!DE3),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF3,DF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DG8">
         <f ca="1">IF($B8=0,0,IF(DG$3=TotalApuestas!DG3,DG$5,0))</f>
@@ -21519,12 +21519,12 @@
         <v>25</v>
       </c>
       <c r="CO9">
-        <f>IF($B9=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO4)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO4)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP9">
-        <f>IF($B9=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP4)=1,CP$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B9=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP4)=1,CP$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CQ9">
         <f>IF($B9=0,0,IF(CQ$3=TotalApuestas!CQ4,CQ$5,0))</f>
@@ -21588,7 +21588,7 @@
       </c>
       <c r="DF9">
         <f ca="1">IF($B9=0,0,IF(AND(DD$3=TotalApuestas!DD4,Resultado!DE$3=TotalApuestas!DE4),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF4,DF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DG9">
         <f ca="1">IF($B9=0,0,IF(DG$3=TotalApuestas!DG4,DG$5,0))</f>
@@ -21600,7 +21600,7 @@
       </c>
       <c r="DI9">
         <f ca="1">IF($B9=0,0,IF(AND(DG$3=TotalApuestas!DG4,Resultado!DH$3=TotalApuestas!DH4),Resultado!DI$5+VLOOKUP(DI$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DI$3=TotalApuestas!DI4,DI$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DJ9">
         <f ca="1">IF($B9=0,0,IF(DJ$3=TotalApuestas!DJ4,DJ$5,0))</f>
@@ -21985,11 +21985,11 @@
         <v>0</v>
       </c>
       <c r="CO10">
-        <f>IF($B10=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO5)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO5)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP10">
-        <f>IF($B10=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP5)=1,CP$5,0))</f>
+        <f ca="1">IF($B10=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP5)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ10">
@@ -22054,7 +22054,7 @@
       </c>
       <c r="DF10">
         <f ca="1">IF($B10=0,0,IF(AND(DD$3=TotalApuestas!DD5,Resultado!DE$3=TotalApuestas!DE5),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF5,DF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DG10">
         <f ca="1">IF($B10=0,0,IF(DG$3=TotalApuestas!DG5,DG$5,0))</f>
@@ -22451,11 +22451,11 @@
         <v>0</v>
       </c>
       <c r="CO11">
-        <f>IF($B11=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO6)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO6)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP11">
-        <f>IF($B11=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP6)=1,CP$5,0))</f>
+        <f ca="1">IF($B11=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP6)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ11">
@@ -22520,7 +22520,7 @@
       </c>
       <c r="DF11">
         <f ca="1">IF($B11=0,0,IF(AND(DD$3=TotalApuestas!DD6,Resultado!DE$3=TotalApuestas!DE6),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF6,DF$5,0)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DG11">
         <f ca="1">IF($B11=0,0,IF(DG$3=TotalApuestas!DG6,DG$5,0))</f>
@@ -22917,11 +22917,11 @@
         <v>0</v>
       </c>
       <c r="CO12">
-        <f>IF($B12=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO7)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO7)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP12">
-        <f>IF($B12=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP7)=1,CP$5,0))</f>
+        <f ca="1">IF($B12=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP7)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ12">
@@ -22986,7 +22986,7 @@
       </c>
       <c r="DF12">
         <f ca="1">IF($B12=0,0,IF(AND(DD$3=TotalApuestas!DD7,Resultado!DE$3=TotalApuestas!DE7),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF7,DF$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DG12">
         <f ca="1">IF($B12=0,0,IF(DG$3=TotalApuestas!DG7,DG$5,0))</f>
@@ -23383,11 +23383,11 @@
         <v>25</v>
       </c>
       <c r="CO13">
-        <f>IF($B13=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO8)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO8)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP13">
-        <f>IF($B13=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP8)=1,CP$5,0))</f>
+        <f ca="1">IF($B13=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP8)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ13">
@@ -23452,7 +23452,7 @@
       </c>
       <c r="DF13">
         <f ca="1">IF($B13=0,0,IF(AND(DD$3=TotalApuestas!DD8,Resultado!DE$3=TotalApuestas!DE8),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF8,DF$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DG13">
         <f ca="1">IF($B13=0,0,IF(DG$3=TotalApuestas!DG8,DG$5,0))</f>
@@ -23849,11 +23849,11 @@
         <v>0</v>
       </c>
       <c r="CO14">
-        <f>IF($B14=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO9)=1,CO$5,0))</f>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO9)=1,CO$5,0))</f>
         <v>0</v>
       </c>
       <c r="CP14">
-        <f>IF($B14=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP9)=1,CP$5,0))</f>
+        <f ca="1">IF($B14=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP9)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ14">
@@ -24315,11 +24315,11 @@
         <v>0</v>
       </c>
       <c r="CO15">
-        <f>IF($B15=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO10)=1,CO$5,0))</f>
-        <v>0</v>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CO10)=1,CO$5,0))</f>
+        <v>30</v>
       </c>
       <c r="CP15">
-        <f>IF($B15=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP10)=1,CP$5,0))</f>
+        <f ca="1">IF($B15=0,0,IF(COUNTIF($CO$3:$CP$3,TotalApuestas!CP10)=1,CP$5,0))</f>
         <v>0</v>
       </c>
       <c r="CQ15">
@@ -24384,7 +24384,7 @@
       </c>
       <c r="DF15">
         <f ca="1">IF($B15=0,0,IF(AND(DD$3=TotalApuestas!DD10,Resultado!DE$3=TotalApuestas!DE10),Resultado!DF$5+VLOOKUP(DF$4&amp;"bonus",Aux!$W$1:$X$46,2,0),IF(DF$3=TotalApuestas!DF10,DF$5,0)))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DG15">
         <f ca="1">IF($B15=0,0,IF(DG$3=TotalApuestas!DG10,DG$5,0))</f>
@@ -41584,12 +41584,12 @@
         <v>Colombia</v>
       </c>
       <c r="CO1" s="84" t="str">
-        <f>+Resultado!CO3</f>
-        <v/>
+        <f ca="1">+Resultado!CO3</f>
+        <v>Argentina</v>
       </c>
       <c r="CP1" s="84" t="str">
-        <f>+Resultado!CP3</f>
-        <v/>
+        <f ca="1">+Resultado!CP3</f>
+        <v>Colombia</v>
       </c>
       <c r="CQ1" s="84" t="str">
         <f>+Resultado!CQ3</f>
@@ -41643,29 +41643,29 @@
         <f ca="1">+Resultado!DC3</f>
         <v>x</v>
       </c>
-      <c r="DD1" s="84" t="str">
+      <c r="DD1" s="84">
         <f ca="1">+Resultado!DD3</f>
-        <v/>
-      </c>
-      <c r="DE1" s="84" t="str">
+        <v>2</v>
+      </c>
+      <c r="DE1" s="84">
         <f ca="1">+Resultado!DE3</f>
-        <v/>
-      </c>
-      <c r="DF1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="DF1" s="84">
         <f ca="1">+Resultado!DF3</f>
-        <v/>
-      </c>
-      <c r="DG1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="DG1" s="84">
         <f ca="1">+Resultado!DG3</f>
-        <v/>
-      </c>
-      <c r="DH1" s="84" t="str">
+        <v>0</v>
+      </c>
+      <c r="DH1" s="84">
         <f ca="1">+Resultado!DH3</f>
-        <v/>
-      </c>
-      <c r="DI1" s="84" t="str">
+        <v>1</v>
+      </c>
+      <c r="DI1" s="84">
         <f ca="1">+Resultado!DI3</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="DJ1" s="84" t="str">
         <f ca="1">+Resultado!DJ3</f>
@@ -48812,7 +48812,7 @@
   <dimension ref="A7:S21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48907,11 +48907,15 @@
         <v>Argentina</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="16">
+        <v>2</v>
+      </c>
       <c r="K9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="16"/>
+      <c r="L9" s="16">
+        <v>0</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="17" t="str">
         <f ca="1">+Cuartos!S12</f>
@@ -48927,8 +48931,8 @@
         <v>MetLife Stadium - EAST RUTHERFORD, NJ</v>
       </c>
       <c r="S9" s="18" t="str">
-        <f>IF(OR(J9="",L9=""),"",IF(J9&gt;L9,H9,IF(J9&lt;L9,N9,IF(OR(J10="",L10=""),"",IF(J10&gt;L10,H9,N9)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J9="",L9=""),"",IF(J9&gt;L9,H9,IF(J9&lt;L9,N9,IF(OR(J10="",L10=""),"",IF(J10&gt;L10,H9,N9)))))</f>
+        <v>Argentina</v>
       </c>
     </row>
     <row r="10" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48994,11 +48998,15 @@
         <v>Uruguay</v>
       </c>
       <c r="I12" s="25"/>
-      <c r="J12" s="16"/>
+      <c r="J12" s="16">
+        <v>0</v>
+      </c>
       <c r="K12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="L12" s="16">
+        <v>1</v>
+      </c>
       <c r="M12" s="6"/>
       <c r="N12" s="17" t="str">
         <f ca="1">+Cuartos!S15</f>
@@ -49014,8 +49022,8 @@
         <v>Bank of America Stadium - CHARLOTTE, NC</v>
       </c>
       <c r="S12" s="18" t="str">
-        <f>IF(OR(J12="",L12=""),"",IF(J12&gt;L12,H12,IF(J12&lt;L12,N12,IF(OR(J13="",L13=""),"",IF(J13&gt;L13,H12,N12)))))</f>
-        <v/>
+        <f ca="1">IF(OR(J12="",L12=""),"",IF(J12&gt;L12,H12,IF(J12&lt;L12,N12,IF(OR(J13="",L13=""),"",IF(J13&gt;L13,H12,N12)))))</f>
+        <v>Colombia</v>
       </c>
     </row>
     <row r="13" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -49264,13 +49272,13 @@
         <v>45486.833333333336</v>
       </c>
       <c r="F9" s="180"/>
-      <c r="G9" s="180" t="str">
-        <f>IFERROR(VLOOKUP(H9,Aux!$A:$C,3,0),"")</f>
-        <v/>
+      <c r="G9" s="180" t="e" vm="2">
+        <f ca="1">IFERROR(VLOOKUP(H9,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H9" s="7" t="str">
-        <f>IF(OR(Semis!J9="",Semis!L9=""),"",IF(Semis!J9&gt;Semis!L9,Semis!N9,IF(Semis!J9&lt;Semis!L9,Semis!H9,IF(OR(Semis!J10="",Semis!L10=""),"",IF(Semis!J10&gt;Semis!L10,Semis!N9,Semis!H9)))))</f>
-        <v/>
+        <f ca="1">IF(OR(Semis!J9="",Semis!L9=""),"",IF(Semis!J9&gt;Semis!L9,Semis!N9,IF(Semis!J9&lt;Semis!L9,Semis!H9,IF(OR(Semis!J10="",Semis!L10=""),"",IF(Semis!J10&gt;Semis!L10,Semis!N9,Semis!H9)))))</f>
+        <v>Canadá</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="16"/>
@@ -49280,12 +49288,12 @@
       <c r="L9" s="16"/>
       <c r="M9" s="6"/>
       <c r="N9" s="17" t="str">
-        <f>IF(OR(Semis!J12="",Semis!L12=""),"",IF(Semis!J12&gt;Semis!L12,Semis!N12,IF(Semis!J12&lt;Semis!L12,Semis!H12,IF(OR(Semis!J13="",Semis!L13=""),"",IF(Semis!J13&gt;Semis!L13,Semis!N12,Semis!H12)))))</f>
-        <v/>
-      </c>
-      <c r="O9" s="180" t="str">
-        <f>IFERROR(VLOOKUP(N9,Aux!$A:$C,3,0),"")</f>
-        <v/>
+        <f ca="1">IF(OR(Semis!J12="",Semis!L12=""),"",IF(Semis!J12&gt;Semis!L12,Semis!N12,IF(Semis!J12&lt;Semis!L12,Semis!H12,IF(OR(Semis!J13="",Semis!L13=""),"",IF(Semis!J13&gt;Semis!L13,Semis!N12,Semis!H12)))))</f>
+        <v>Uruguay</v>
+      </c>
+      <c r="O9" s="180" t="e" vm="11">
+        <f ca="1">IFERROR(VLOOKUP(N9,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="175" t="str">
@@ -49388,13 +49396,13 @@
         <v>45487.833333333336</v>
       </c>
       <c r="F15" s="180"/>
-      <c r="G15" s="180" t="str">
-        <f>IFERROR(VLOOKUP(H15,Aux!$A:$C,3,0),"")</f>
-        <v/>
+      <c r="G15" s="180" t="e" vm="1">
+        <f ca="1">IFERROR(VLOOKUP(H15,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H15" s="7" t="str">
-        <f>+Semis!S9</f>
-        <v/>
+        <f ca="1">+Semis!S9</f>
+        <v>Argentina</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="16"/>
@@ -49404,12 +49412,12 @@
       <c r="L15" s="16"/>
       <c r="M15" s="6"/>
       <c r="N15" s="17" t="str">
-        <f>+Semis!S12</f>
-        <v/>
-      </c>
-      <c r="O15" s="180" t="str">
-        <f>IFERROR(VLOOKUP(N15,Aux!$A:$C,3,0),"")</f>
-        <v/>
+        <f ca="1">+Semis!S12</f>
+        <v>Colombia</v>
+      </c>
+      <c r="O15" s="180" t="e" vm="13">
+        <f ca="1">IFERROR(VLOOKUP(N15,Aux!$A:$C,3,0),"")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="P15" s="17"/>
       <c r="Q15" s="175" t="str">
@@ -51257,13 +51265,13 @@
       <c r="M30" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="N30" s="68" t="str">
+      <c r="N30" s="68">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O30" s="68" t="str">
+        <v>2</v>
+      </c>
+      <c r="O30" s="68">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="2"/>
@@ -51294,13 +51302,13 @@
       <c r="M31" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="68" t="str">
+      <c r="N31" s="68">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O31" s="68" t="str">
+        <v>0</v>
+      </c>
+      <c r="O31" s="68">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="2"/>

</xml_diff>